<commit_message>
update testoutput files and objects
</commit_message>
<xml_diff>
--- a/inst/testdata/examples_of_output/testoutput_ejam2excel_10pts_1miles.xlsx
+++ b/inst/testdata/examples_of_output/testoutput_ejam2excel_10pts_1miles.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1215" uniqueCount="1215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1216" uniqueCount="1216">
   <si>
     <t xml:space="preserve">Analysis Title</t>
   </si>
@@ -3164,6 +3164,9 @@
     <t xml:space="preserve">US percentile for Supplemental Summary Index for Particulate Matter</t>
   </si>
   <si>
+    <t xml:space="preserve">46</t>
+  </si>
+  <si>
     <t xml:space="preserve">US percentile for Supplemental Summary Index for Ozone</t>
   </si>
   <si>
@@ -3359,7 +3362,7 @@
     <t xml:space="preserve">US type of raw score for Particulate Matter Summary Index</t>
   </si>
   <si>
-    <t xml:space="preserve">83.142</t>
+    <t xml:space="preserve">66.855</t>
   </si>
   <si>
     <t xml:space="preserve">US type of raw score for Ozone Summary Index</t>
@@ -3389,7 +3392,7 @@
     <t xml:space="preserve">US type of raw score for Traffic Proximity and Volume Summary Index</t>
   </si>
   <si>
-    <t xml:space="preserve">94.692</t>
+    <t xml:space="preserve">94.667</t>
   </si>
   <si>
     <t xml:space="preserve">US type of raw score for Lead Paint Summary Index</t>
@@ -3407,7 +3410,7 @@
     <t xml:space="preserve">US type of raw score for RMP Proximity Summary Index</t>
   </si>
   <si>
-    <t xml:space="preserve">123.057</t>
+    <t xml:space="preserve">122.999</t>
   </si>
   <si>
     <t xml:space="preserve">US type of raw score for Hazardous Waste Proximity Summary Index</t>
@@ -3425,7 +3428,7 @@
     <t xml:space="preserve">US type of raw score for Wastewater Discharge Summary Index</t>
   </si>
   <si>
-    <t xml:space="preserve">80.294</t>
+    <t xml:space="preserve">80.283</t>
   </si>
   <si>
     <t xml:space="preserve">US type of raw score for Drinking Water Non-Compliance Summary Index</t>
@@ -3437,7 +3440,7 @@
     <t xml:space="preserve">State type of raw score for Particulate Matter Summary Index</t>
   </si>
   <si>
-    <t xml:space="preserve">58.857</t>
+    <t xml:space="preserve">48.636</t>
   </si>
   <si>
     <t xml:space="preserve">State type of raw score for Ozone Summary Index</t>
@@ -3485,7 +3488,7 @@
     <t xml:space="preserve">State type of raw score for RMP Proximity Summary Index</t>
   </si>
   <si>
-    <t xml:space="preserve">106.043</t>
+    <t xml:space="preserve">106.014</t>
   </si>
   <si>
     <t xml:space="preserve">State type of raw score for Hazardous Waste Proximity Summary Index</t>
@@ -3503,7 +3506,7 @@
     <t xml:space="preserve">State type of raw score for Wastewater Discharge Summary Index</t>
   </si>
   <si>
-    <t xml:space="preserve">46.56</t>
+    <t xml:space="preserve">46.43</t>
   </si>
   <si>
     <t xml:space="preserve">State type of raw score for Drinking Water Non-Compliance Summary Index</t>
@@ -3515,7 +3518,7 @@
     <t xml:space="preserve">US type of raw score for Particulate Matter Supplemental Summary Index</t>
   </si>
   <si>
-    <t xml:space="preserve">78.034</t>
+    <t xml:space="preserve">62.937</t>
   </si>
   <si>
     <t xml:space="preserve">US type of raw score for Ozone Supplemental Summary Index</t>
@@ -3545,7 +3548,7 @@
     <t xml:space="preserve">US type of raw score for Traffic Proximity and Volume Supplemental Summary Index</t>
   </si>
   <si>
-    <t xml:space="preserve">91.293</t>
+    <t xml:space="preserve">91.252</t>
   </si>
   <si>
     <t xml:space="preserve">US type of raw score for Lead Paint Supplemental Summary Index</t>
@@ -3563,7 +3566,7 @@
     <t xml:space="preserve">US type of raw score for RMP Proximity Supplemental Summary Index</t>
   </si>
   <si>
-    <t xml:space="preserve">114.085</t>
+    <t xml:space="preserve">114.012</t>
   </si>
   <si>
     <t xml:space="preserve">US type of raw score for Hazardous Waste Proximity Supplemental Summary Index</t>
@@ -3581,7 +3584,7 @@
     <t xml:space="preserve">US type of raw score for Wastewater Discharge Supplemental Summary Index</t>
   </si>
   <si>
-    <t xml:space="preserve">78.09</t>
+    <t xml:space="preserve">78.077</t>
   </si>
   <si>
     <t xml:space="preserve">US type of raw score for Drinking Water Non-Compliance Supplemental Summary Index</t>
@@ -3593,7 +3596,7 @@
     <t xml:space="preserve">State type of raw score for Particulate Matter Supplemental Summary Index</t>
   </si>
   <si>
-    <t xml:space="preserve">55.113</t>
+    <t xml:space="preserve">45.359</t>
   </si>
   <si>
     <t xml:space="preserve">State type of raw score for Ozone Supplemental Summary Index</t>
@@ -3641,7 +3644,7 @@
     <t xml:space="preserve">State type of raw score for RMP Proximity Supplemental Summary Index</t>
   </si>
   <si>
-    <t xml:space="preserve">97.693</t>
+    <t xml:space="preserve">97.655</t>
   </si>
   <si>
     <t xml:space="preserve">State type of raw score for Hazardous Waste Proximity Supplemental Summary Index</t>
@@ -3659,7 +3662,7 @@
     <t xml:space="preserve">State type of raw score for Wastewater Discharge Supplemental Summary Index</t>
   </si>
   <si>
-    <t xml:space="preserve">47.318</t>
+    <t xml:space="preserve">47.177</t>
   </si>
   <si>
     <t xml:space="preserve">State type of raw score for Drinking Water Non-Compliance Supplemental Summary Index</t>
@@ -5619,322 +5622,322 @@
         <v>1045</v>
       </c>
       <c r="MZ1" s="19" t="s">
-        <v>1046</v>
+        <v>1047</v>
       </c>
       <c r="NA1" s="19" t="s">
-        <v>1047</v>
+        <v>1048</v>
       </c>
       <c r="NB1" s="19" t="s">
-        <v>1048</v>
+        <v>1049</v>
       </c>
       <c r="NC1" s="19" t="s">
-        <v>1049</v>
+        <v>1050</v>
       </c>
       <c r="ND1" s="19" t="s">
-        <v>1050</v>
+        <v>1051</v>
       </c>
       <c r="NE1" s="19" t="s">
-        <v>1051</v>
+        <v>1052</v>
       </c>
       <c r="NF1" s="19" t="s">
-        <v>1052</v>
+        <v>1053</v>
       </c>
       <c r="NG1" s="19" t="s">
-        <v>1054</v>
+        <v>1055</v>
       </c>
       <c r="NH1" s="19" t="s">
-        <v>1056</v>
+        <v>1057</v>
       </c>
       <c r="NI1" s="19" t="s">
-        <v>1058</v>
+        <v>1059</v>
       </c>
       <c r="NJ1" s="19" t="s">
-        <v>1059</v>
+        <v>1060</v>
       </c>
       <c r="NK1" s="19" t="s">
-        <v>1060</v>
+        <v>1061</v>
       </c>
       <c r="NL1" s="20" t="s">
-        <v>1061</v>
+        <v>1062</v>
       </c>
       <c r="NM1" s="20" t="s">
-        <v>1062</v>
+        <v>1063</v>
       </c>
       <c r="NN1" s="20" t="s">
-        <v>1063</v>
+        <v>1064</v>
       </c>
       <c r="NO1" s="20" t="s">
-        <v>1064</v>
+        <v>1065</v>
       </c>
       <c r="NP1" s="20" t="s">
-        <v>1065</v>
+        <v>1066</v>
       </c>
       <c r="NQ1" s="20" t="s">
-        <v>1066</v>
+        <v>1067</v>
       </c>
       <c r="NR1" s="20" t="s">
-        <v>1067</v>
+        <v>1068</v>
       </c>
       <c r="NS1" s="20" t="s">
-        <v>1068</v>
+        <v>1069</v>
       </c>
       <c r="NT1" s="20" t="s">
-        <v>1069</v>
+        <v>1070</v>
       </c>
       <c r="NU1" s="20" t="s">
-        <v>1070</v>
+        <v>1071</v>
       </c>
       <c r="NV1" s="20" t="s">
-        <v>1071</v>
+        <v>1072</v>
       </c>
       <c r="NW1" s="20" t="s">
-        <v>1072</v>
+        <v>1073</v>
       </c>
       <c r="NX1" s="20" t="s">
-        <v>1073</v>
+        <v>1074</v>
       </c>
       <c r="NY1" s="20" t="s">
-        <v>1074</v>
+        <v>1075</v>
       </c>
       <c r="NZ1" s="20" t="s">
-        <v>1075</v>
+        <v>1076</v>
       </c>
       <c r="OA1" s="20" t="s">
-        <v>1076</v>
+        <v>1077</v>
       </c>
       <c r="OB1" s="20" t="s">
-        <v>1077</v>
+        <v>1078</v>
       </c>
       <c r="OC1" s="20" t="s">
-        <v>1078</v>
+        <v>1079</v>
       </c>
       <c r="OD1" s="20" t="s">
-        <v>1079</v>
+        <v>1080</v>
       </c>
       <c r="OE1" s="20" t="s">
-        <v>1080</v>
+        <v>1081</v>
       </c>
       <c r="OF1" s="20" t="s">
-        <v>1081</v>
+        <v>1082</v>
       </c>
       <c r="OG1" s="20" t="s">
-        <v>1083</v>
+        <v>1084</v>
       </c>
       <c r="OH1" s="20" t="s">
-        <v>1084</v>
+        <v>1085</v>
       </c>
       <c r="OI1" s="20" t="s">
-        <v>1086</v>
+        <v>1087</v>
       </c>
       <c r="OJ1" s="20" t="s">
-        <v>1087</v>
+        <v>1088</v>
       </c>
       <c r="OK1" s="20" t="s">
-        <v>1088</v>
+        <v>1089</v>
       </c>
       <c r="OL1" s="10" t="s">
-        <v>1090</v>
+        <v>1091</v>
       </c>
       <c r="OM1" s="10" t="s">
-        <v>1092</v>
+        <v>1093</v>
       </c>
       <c r="ON1" s="10" t="s">
-        <v>1093</v>
+        <v>1094</v>
       </c>
       <c r="OO1" s="9" t="s">
-        <v>1094</v>
+        <v>1095</v>
       </c>
       <c r="OP1" s="9" t="s">
-        <v>1096</v>
+        <v>1097</v>
       </c>
       <c r="OQ1" s="3" t="s">
-        <v>1098</v>
+        <v>1099</v>
       </c>
       <c r="OR1" s="3" t="s">
-        <v>1100</v>
+        <v>1101</v>
       </c>
       <c r="OS1" s="3" t="s">
-        <v>1101</v>
+        <v>1102</v>
       </c>
       <c r="OT1" s="9" t="s">
-        <v>1102</v>
+        <v>1103</v>
       </c>
       <c r="OU1" s="9" t="s">
-        <v>1103</v>
+        <v>1104</v>
       </c>
       <c r="OV1" s="9" t="s">
-        <v>1104</v>
+        <v>1105</v>
       </c>
       <c r="OW1" s="9" t="s">
-        <v>1105</v>
+        <v>1106</v>
       </c>
       <c r="OX1" s="9" t="s">
-        <v>1106</v>
+        <v>1107</v>
       </c>
       <c r="OY1" s="9" t="s">
-        <v>1107</v>
+        <v>1108</v>
       </c>
       <c r="OZ1" s="9" t="s">
-        <v>1108</v>
+        <v>1109</v>
       </c>
       <c r="PA1" s="21" t="s">
-        <v>1110</v>
+        <v>1111</v>
       </c>
       <c r="PB1" s="21" t="s">
-        <v>1112</v>
+        <v>1113</v>
       </c>
       <c r="PC1" s="21" t="s">
-        <v>1114</v>
+        <v>1115</v>
       </c>
       <c r="PD1" s="21" t="s">
-        <v>1116</v>
+        <v>1117</v>
       </c>
       <c r="PE1" s="21" t="s">
-        <v>1118</v>
+        <v>1119</v>
       </c>
       <c r="PF1" s="21" t="s">
-        <v>1120</v>
+        <v>1121</v>
       </c>
       <c r="PG1" s="21" t="s">
-        <v>1122</v>
+        <v>1123</v>
       </c>
       <c r="PH1" s="21" t="s">
-        <v>1124</v>
+        <v>1125</v>
       </c>
       <c r="PI1" s="21" t="s">
-        <v>1126</v>
+        <v>1127</v>
       </c>
       <c r="PJ1" s="21" t="s">
-        <v>1128</v>
+        <v>1129</v>
       </c>
       <c r="PK1" s="21" t="s">
-        <v>1130</v>
+        <v>1131</v>
       </c>
       <c r="PL1" s="21" t="s">
-        <v>1132</v>
+        <v>1133</v>
       </c>
       <c r="PM1" s="21" t="s">
-        <v>1134</v>
+        <v>1135</v>
       </c>
       <c r="PN1" s="19" t="s">
-        <v>1136</v>
+        <v>1137</v>
       </c>
       <c r="PO1" s="19" t="s">
-        <v>1138</v>
+        <v>1139</v>
       </c>
       <c r="PP1" s="19" t="s">
-        <v>1140</v>
+        <v>1141</v>
       </c>
       <c r="PQ1" s="19" t="s">
-        <v>1142</v>
+        <v>1143</v>
       </c>
       <c r="PR1" s="19" t="s">
-        <v>1144</v>
+        <v>1145</v>
       </c>
       <c r="PS1" s="19" t="s">
-        <v>1146</v>
+        <v>1147</v>
       </c>
       <c r="PT1" s="19" t="s">
-        <v>1148</v>
+        <v>1149</v>
       </c>
       <c r="PU1" s="19" t="s">
-        <v>1150</v>
+        <v>1151</v>
       </c>
       <c r="PV1" s="19" t="s">
-        <v>1152</v>
+        <v>1153</v>
       </c>
       <c r="PW1" s="19" t="s">
-        <v>1154</v>
+        <v>1155</v>
       </c>
       <c r="PX1" s="19" t="s">
-        <v>1156</v>
+        <v>1157</v>
       </c>
       <c r="PY1" s="19" t="s">
-        <v>1158</v>
+        <v>1159</v>
       </c>
       <c r="PZ1" s="19" t="s">
-        <v>1160</v>
+        <v>1161</v>
       </c>
       <c r="QA1" s="21" t="s">
-        <v>1162</v>
+        <v>1163</v>
       </c>
       <c r="QB1" s="21" t="s">
-        <v>1164</v>
+        <v>1165</v>
       </c>
       <c r="QC1" s="21" t="s">
-        <v>1166</v>
+        <v>1167</v>
       </c>
       <c r="QD1" s="21" t="s">
-        <v>1168</v>
+        <v>1169</v>
       </c>
       <c r="QE1" s="21" t="s">
-        <v>1170</v>
+        <v>1171</v>
       </c>
       <c r="QF1" s="21" t="s">
-        <v>1172</v>
+        <v>1173</v>
       </c>
       <c r="QG1" s="21" t="s">
-        <v>1174</v>
+        <v>1175</v>
       </c>
       <c r="QH1" s="21" t="s">
-        <v>1176</v>
+        <v>1177</v>
       </c>
       <c r="QI1" s="21" t="s">
-        <v>1178</v>
+        <v>1179</v>
       </c>
       <c r="QJ1" s="21" t="s">
-        <v>1180</v>
+        <v>1181</v>
       </c>
       <c r="QK1" s="21" t="s">
-        <v>1182</v>
+        <v>1183</v>
       </c>
       <c r="QL1" s="21" t="s">
-        <v>1184</v>
+        <v>1185</v>
       </c>
       <c r="QM1" s="21" t="s">
-        <v>1186</v>
+        <v>1187</v>
       </c>
       <c r="QN1" s="19" t="s">
-        <v>1188</v>
+        <v>1189</v>
       </c>
       <c r="QO1" s="19" t="s">
-        <v>1190</v>
+        <v>1191</v>
       </c>
       <c r="QP1" s="19" t="s">
-        <v>1192</v>
+        <v>1193</v>
       </c>
       <c r="QQ1" s="19" t="s">
-        <v>1194</v>
+        <v>1195</v>
       </c>
       <c r="QR1" s="19" t="s">
-        <v>1196</v>
+        <v>1197</v>
       </c>
       <c r="QS1" s="19" t="s">
-        <v>1198</v>
+        <v>1199</v>
       </c>
       <c r="QT1" s="19" t="s">
-        <v>1200</v>
+        <v>1201</v>
       </c>
       <c r="QU1" s="19" t="s">
-        <v>1202</v>
+        <v>1203</v>
       </c>
       <c r="QV1" s="19" t="s">
-        <v>1204</v>
+        <v>1205</v>
       </c>
       <c r="QW1" s="19" t="s">
-        <v>1206</v>
+        <v>1207</v>
       </c>
       <c r="QX1" s="19" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="QY1" s="19" t="s">
-        <v>1210</v>
+        <v>1211</v>
       </c>
       <c r="QZ1" s="19" t="s">
-        <v>1212</v>
+        <v>1213</v>
       </c>
       <c r="RA1" s="3" t="s">
-        <v>1214</v>
+        <v>1215</v>
       </c>
     </row>
     <row r="2">
@@ -6961,7 +6964,7 @@
         <v>85</v>
       </c>
       <c r="MM2" s="29" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="MN2" s="29" t="n">
         <v>76</v>
@@ -7000,7 +7003,7 @@
         <v>78</v>
       </c>
       <c r="MZ2" s="29" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="NA2" s="29" t="n">
         <v>67</v>
@@ -7162,7 +7165,7 @@
         <v>147.526020073567</v>
       </c>
       <c r="PB2" s="25" t="n">
-        <v>0</v>
+        <v>1.73908625064187</v>
       </c>
       <c r="PC2" s="25" t="n">
         <v>117.411682117158</v>
@@ -7201,7 +7204,7 @@
         <v>30.261877629349</v>
       </c>
       <c r="PO2" s="25" t="n">
-        <v>7.81492351857363</v>
+        <v>7.62900682444057</v>
       </c>
       <c r="PP2" s="25" t="n">
         <v>102.341562793256</v>
@@ -7240,7 +7243,7 @@
         <v>123.623333748108</v>
       </c>
       <c r="QB2" s="25" t="n">
-        <v>0</v>
+        <v>1.45910485025071</v>
       </c>
       <c r="QC2" s="25" t="n">
         <v>97.5633727537407</v>
@@ -7279,7 +7282,7 @@
         <v>20.1659993085997</v>
       </c>
       <c r="QO2" s="25" t="n">
-        <v>5.25275661180307</v>
+        <v>5.13716694653457</v>
       </c>
       <c r="QP2" s="25" t="n">
         <v>67.4866656619721</v>
@@ -8334,7 +8337,7 @@
         <v>2</v>
       </c>
       <c r="MM3" s="29" t="n">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="MN3" s="29" t="n">
         <v>20</v>
@@ -8373,7 +8376,7 @@
         <v>2</v>
       </c>
       <c r="MZ3" s="29" t="n">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="NA3" s="29" t="n">
         <v>25</v>
@@ -8412,7 +8415,7 @@
         <v>31</v>
       </c>
       <c r="NM3" s="29" t="n">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="NN3" s="29" t="n">
         <v>52</v>
@@ -8451,7 +8454,7 @@
         <v>34</v>
       </c>
       <c r="NZ3" s="29" t="n">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="OA3" s="29" t="n">
         <v>58</v>
@@ -8535,10 +8538,10 @@
         <v>1.02026861584964</v>
       </c>
       <c r="PB3" s="25" t="n">
-        <v>1.53040292377445</v>
+        <v>8.67228323472191</v>
       </c>
       <c r="PC3" s="25" t="n">
-        <v>13.1908713550649</v>
+        <v>13.1908713550648</v>
       </c>
       <c r="PD3" s="25" t="n">
         <v>1.53040292377445</v>
@@ -8559,7 +8562,7 @@
         <v>0</v>
       </c>
       <c r="PJ3" s="25" t="n">
-        <v>0.387310138562228</v>
+        <v>0.387310138562227</v>
       </c>
       <c r="PK3" s="25" t="n">
         <v>33.69486095776</v>
@@ -8568,13 +8571,13 @@
         <v>4.66382942230378</v>
       </c>
       <c r="PM3" s="25" t="n">
-        <v>39.9115104364365</v>
+        <v>39.7904760181358</v>
       </c>
       <c r="PN3" s="25" t="n">
         <v>29.3478476488843</v>
       </c>
       <c r="PO3" s="25" t="n">
-        <v>9.46704762867236</v>
+        <v>20.8275047830792</v>
       </c>
       <c r="PP3" s="25" t="n">
         <v>55.7276054566087</v>
@@ -8613,7 +8616,7 @@
         <v>2.56516565088795</v>
       </c>
       <c r="QB3" s="25" t="n">
-        <v>3.84774847633193</v>
+        <v>21.8039080325476</v>
       </c>
       <c r="QC3" s="25" t="n">
         <v>33.1607334747035</v>
@@ -8646,13 +8649,13 @@
         <v>11.7296654158357</v>
       </c>
       <c r="QM3" s="25" t="n">
-        <v>100.352160362697</v>
+        <v>100.04146038463</v>
       </c>
       <c r="QN3" s="25" t="n">
         <v>40.9150689864568</v>
       </c>
       <c r="QO3" s="25" t="n">
-        <v>13.1984093504699</v>
+        <v>29.0365005710339</v>
       </c>
       <c r="QP3" s="25" t="n">
         <v>77.6720353423386</v>
@@ -9715,7 +9718,7 @@
         <v>58</v>
       </c>
       <c r="MM4" s="29" t="n">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="MN4" s="29" t="n">
         <v>79</v>
@@ -9754,7 +9757,7 @@
         <v>43</v>
       </c>
       <c r="MZ4" s="29" t="n">
-        <v>64</v>
+        <v>52</v>
       </c>
       <c r="NA4" s="29" t="n">
         <v>78</v>
@@ -9793,7 +9796,7 @@
         <v>72</v>
       </c>
       <c r="NM4" s="29" t="n">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="NN4" s="29" t="n">
         <v>74</v>
@@ -9832,7 +9835,7 @@
         <v>72</v>
       </c>
       <c r="NZ4" s="29" t="n">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="OA4" s="29" t="n">
         <v>76</v>
@@ -9865,7 +9868,7 @@
         <v>71</v>
       </c>
       <c r="OK4" s="29" t="n">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="OL4" s="22" t="n">
         <v>121</v>
@@ -9916,7 +9919,7 @@
         <v>61.9334383542575</v>
       </c>
       <c r="PB4" s="25" t="n">
-        <v>92.0170480357706</v>
+        <v>73.5831486297469</v>
       </c>
       <c r="PC4" s="25" t="n">
         <v>130.362913541297</v>
@@ -9949,13 +9952,13 @@
         <v>116.507485254061</v>
       </c>
       <c r="PM4" s="25" t="n">
-        <v>122.681265493211</v>
+        <v>122.665964781077</v>
       </c>
       <c r="PN4" s="25" t="n">
         <v>99.5955004053087</v>
       </c>
       <c r="PO4" s="25" t="n">
-        <v>64.9079205832168</v>
+        <v>52.2258272098887</v>
       </c>
       <c r="PP4" s="25" t="n">
         <v>116.992026021754</v>
@@ -9988,13 +9991,13 @@
         <v>99.498695445133</v>
       </c>
       <c r="PZ4" s="25" t="n">
-        <v>70.3255780609697</v>
+        <v>70.1255436840799</v>
       </c>
       <c r="QA4" s="25" t="n">
         <v>59.8066990248148</v>
       </c>
       <c r="QB4" s="25" t="n">
-        <v>88.7164059904571</v>
+        <v>70.9223064278375</v>
       </c>
       <c r="QC4" s="25" t="n">
         <v>125.729072309413</v>
@@ -10027,13 +10030,13 @@
         <v>112.464386000112</v>
       </c>
       <c r="QM4" s="25" t="n">
-        <v>118.342435978211</v>
+        <v>118.326861908482</v>
       </c>
       <c r="QN4" s="25" t="n">
         <v>100.535119459682</v>
       </c>
       <c r="QO4" s="25" t="n">
-        <v>65.3126791318764</v>
+        <v>52.5458095107339</v>
       </c>
       <c r="QP4" s="25" t="n">
         <v>118.02557250542</v>
@@ -10066,7 +10069,7 @@
         <v>100.504794101966</v>
       </c>
       <c r="QZ4" s="25" t="n">
-        <v>70.9656682960832</v>
+        <v>70.7484835206945</v>
       </c>
       <c r="RA4" s="23" t="n">
         <v>3.14159265358979</v>
@@ -11096,7 +11099,7 @@
         <v>10</v>
       </c>
       <c r="MM5" s="29" t="n">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="MN5" s="29" t="n">
         <v>29</v>
@@ -11135,7 +11138,7 @@
         <v>12</v>
       </c>
       <c r="MZ5" s="29" t="n">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="NA5" s="29" t="n">
         <v>41</v>
@@ -11174,7 +11177,7 @@
         <v>40</v>
       </c>
       <c r="NM5" s="29" t="n">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="NN5" s="29" t="n">
         <v>34</v>
@@ -11213,7 +11216,7 @@
         <v>55</v>
       </c>
       <c r="NZ5" s="29" t="n">
-        <v>74</v>
+        <v>63</v>
       </c>
       <c r="OA5" s="29" t="n">
         <v>42</v>
@@ -11297,7 +11300,7 @@
         <v>6.18106233110586</v>
       </c>
       <c r="PB5" s="25" t="n">
-        <v>15.2311958777375</v>
+        <v>13.670686056997</v>
       </c>
       <c r="PC5" s="25" t="n">
         <v>20.7134557649812</v>
@@ -11312,7 +11315,7 @@
         <v>17.5273118887225</v>
       </c>
       <c r="PG5" s="25" t="n">
-        <v>23.4354008386389</v>
+        <v>23.4354008386388</v>
       </c>
       <c r="PH5" s="25" t="n">
         <v>0</v>
@@ -11336,7 +11339,7 @@
         <v>26.4793069071469</v>
       </c>
       <c r="PO5" s="25" t="n">
-        <v>43.2873588710858</v>
+        <v>34.7549654650404</v>
       </c>
       <c r="PP5" s="25" t="n">
         <v>20.9065803078131</v>
@@ -11375,7 +11378,7 @@
         <v>15.5800649015706</v>
       </c>
       <c r="QB5" s="25" t="n">
-        <v>38.7170574772691</v>
+        <v>34.7504070270963</v>
       </c>
       <c r="QC5" s="25" t="n">
         <v>53.4826080364208</v>
@@ -11414,7 +11417,7 @@
         <v>53.6364288591919</v>
       </c>
       <c r="QO5" s="25" t="n">
-        <v>88.2582589647063</v>
+        <v>71.2110570067934</v>
       </c>
       <c r="QP5" s="25" t="n">
         <v>43.7864105760659</v>
@@ -12469,7 +12472,7 @@
         <v>30</v>
       </c>
       <c r="MM6" s="29" t="n">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="MN6" s="29" t="n">
         <v>14</v>
@@ -12493,7 +12496,7 @@
         <v>0</v>
       </c>
       <c r="MU6" s="29" t="n">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="MV6" s="29" t="n">
         <v>59</v>
@@ -12508,7 +12511,7 @@
         <v>24</v>
       </c>
       <c r="MZ6" s="29" t="n">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="NA6" s="29" t="n">
         <v>8</v>
@@ -12532,7 +12535,7 @@
         <v>0</v>
       </c>
       <c r="NH6" s="29" t="n">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="NI6" s="29" t="n">
         <v>57</v>
@@ -12547,7 +12550,7 @@
         <v>30</v>
       </c>
       <c r="NM6" s="29" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="NN6" s="29" t="n">
         <v>5</v>
@@ -12571,7 +12574,7 @@
         <v>0</v>
       </c>
       <c r="NU6" s="29" t="n">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="NV6" s="29" t="n">
         <v>42</v>
@@ -12586,7 +12589,7 @@
         <v>28</v>
       </c>
       <c r="NZ6" s="29" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="OA6" s="29" t="n">
         <v>2</v>
@@ -12610,7 +12613,7 @@
         <v>0</v>
       </c>
       <c r="OH6" s="29" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="OI6" s="29" t="n">
         <v>40</v>
@@ -12670,7 +12673,7 @@
         <v>23.0409848173639</v>
       </c>
       <c r="PB6" s="25" t="n">
-        <v>38.3412972176782</v>
+        <v>39.6968154045372</v>
       </c>
       <c r="PC6" s="25" t="n">
         <v>8.60817609314943</v>
@@ -12679,7 +12682,7 @@
         <v>23.7860525053971</v>
       </c>
       <c r="PE6" s="25" t="n">
-        <v>10.048249479784</v>
+        <v>10.0482494797839</v>
       </c>
       <c r="PF6" s="25" t="n">
         <v>29.2050913014527</v>
@@ -12694,7 +12697,7 @@
         <v>0</v>
       </c>
       <c r="PJ6" s="25" t="n">
-        <v>14.4085372098873</v>
+        <v>6.19607543280081</v>
       </c>
       <c r="PK6" s="25" t="n">
         <v>58.2397351865338</v>
@@ -12709,7 +12712,7 @@
         <v>19.9775292553547</v>
       </c>
       <c r="PO6" s="25" t="n">
-        <v>3.51759786028714</v>
+        <v>0.592906303592776</v>
       </c>
       <c r="PP6" s="25" t="n">
         <v>1.78813830308018</v>
@@ -12733,7 +12736,7 @@
         <v>0</v>
       </c>
       <c r="PW6" s="25" t="n">
-        <v>3.9915237843948</v>
+        <v>0</v>
       </c>
       <c r="PX6" s="25" t="n">
         <v>30.4151655251991</v>
@@ -12742,13 +12745,13 @@
         <v>14.2500183574574</v>
       </c>
       <c r="PZ6" s="25" t="n">
-        <v>38.4739015817123</v>
+        <v>38.4699021294061</v>
       </c>
       <c r="QA6" s="25" t="n">
         <v>31.3458835047324</v>
       </c>
       <c r="QB6" s="25" t="n">
-        <v>52.279349558934</v>
+        <v>54.0675406722285</v>
       </c>
       <c r="QC6" s="25" t="n">
         <v>11.9004922248481</v>
@@ -12772,7 +12775,7 @@
         <v>0</v>
       </c>
       <c r="QJ6" s="25" t="n">
-        <v>20.6658053899061</v>
+        <v>10.3630513735587</v>
       </c>
       <c r="QK6" s="25" t="n">
         <v>79.2183890714953</v>
@@ -12787,7 +12790,7 @@
         <v>24.9374188259632</v>
       </c>
       <c r="QO6" s="25" t="n">
-        <v>4.37388171593421</v>
+        <v>0.692512809959195</v>
       </c>
       <c r="QP6" s="25" t="n">
         <v>2.28970040109511</v>
@@ -12811,7 +12814,7 @@
         <v>0</v>
       </c>
       <c r="QW6" s="25" t="n">
-        <v>5.26382328212159</v>
+        <v>0</v>
       </c>
       <c r="QX6" s="25" t="n">
         <v>37.4967271481087</v>
@@ -12820,7 +12823,7 @@
         <v>17.6579693326827</v>
       </c>
       <c r="QZ6" s="25" t="n">
-        <v>51.6122746427208</v>
+        <v>51.6031654117135</v>
       </c>
       <c r="RA6" s="23" t="n">
         <v>3.14159265358979</v>
@@ -13928,7 +13931,7 @@
         <v>30</v>
       </c>
       <c r="NM7" s="29" t="n">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="NN7" s="29" t="n">
         <v>52</v>
@@ -13967,7 +13970,7 @@
         <v>17</v>
       </c>
       <c r="NZ7" s="29" t="n">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="OA7" s="29" t="n">
         <v>40</v>
@@ -14051,7 +14054,7 @@
         <v>2.57799526706975</v>
       </c>
       <c r="PB7" s="25" t="n">
-        <v>21.4832938922479</v>
+        <v>21.5561089571271</v>
       </c>
       <c r="PC7" s="25" t="n">
         <v>37.6638998618618</v>
@@ -14090,7 +14093,7 @@
         <v>18.5456956459861</v>
       </c>
       <c r="PO7" s="25" t="n">
-        <v>51.7381606363633</v>
+        <v>45.0342108257509</v>
       </c>
       <c r="PP7" s="25" t="n">
         <v>42.0493123414748</v>
@@ -14129,7 +14132,7 @@
         <v>3.44053764346531</v>
       </c>
       <c r="QB7" s="25" t="n">
-        <v>28.6711470288776</v>
+        <v>28.7381910170622</v>
       </c>
       <c r="QC7" s="25" t="n">
         <v>45.0936442405563</v>
@@ -14168,7 +14171,7 @@
         <v>20.2600396385842</v>
       </c>
       <c r="QO7" s="25" t="n">
-        <v>56.6697766152045</v>
+        <v>49.2575284291922</v>
       </c>
       <c r="QP7" s="25" t="n">
         <v>41.0611492852566</v>
@@ -15231,7 +15234,7 @@
         <v>91</v>
       </c>
       <c r="MM8" s="29" t="n">
-        <v>88</v>
+        <v>78</v>
       </c>
       <c r="MN8" s="29" t="n">
         <v>70</v>
@@ -15270,7 +15273,7 @@
         <v>86</v>
       </c>
       <c r="MZ8" s="29" t="n">
-        <v>82</v>
+        <v>63</v>
       </c>
       <c r="NA8" s="29" t="n">
         <v>57</v>
@@ -15309,7 +15312,7 @@
         <v>67</v>
       </c>
       <c r="NM8" s="29" t="n">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="NN8" s="29" t="n">
         <v>39</v>
@@ -15348,7 +15351,7 @@
         <v>60</v>
       </c>
       <c r="NZ8" s="29" t="n">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="OA8" s="29" t="n">
         <v>33</v>
@@ -15432,7 +15435,7 @@
         <v>183.713982493363</v>
       </c>
       <c r="PB8" s="25" t="n">
-        <v>160.11928862861</v>
+        <v>107.969029034477</v>
       </c>
       <c r="PC8" s="25" t="n">
         <v>96.1876930283443</v>
@@ -15471,7 +15474,7 @@
         <v>121.916671389955</v>
       </c>
       <c r="PO8" s="25" t="n">
-        <v>71.6344433323325</v>
+        <v>69.164659040453</v>
       </c>
       <c r="PP8" s="25" t="n">
         <v>58.4536247063949</v>
@@ -15510,7 +15513,7 @@
         <v>149.792008783348</v>
       </c>
       <c r="QB8" s="25" t="n">
-        <v>130.53747044082</v>
+        <v>88.0883946524944</v>
       </c>
       <c r="QC8" s="25" t="n">
         <v>78.042392169296</v>
@@ -15549,7 +15552,7 @@
         <v>80.0075160437923</v>
       </c>
       <c r="QO8" s="25" t="n">
-        <v>47.0387666280044</v>
+        <v>45.3850939945673</v>
       </c>
       <c r="QP8" s="25" t="n">
         <v>37.9858914292202</v>
@@ -16612,7 +16615,7 @@
         <v>28</v>
       </c>
       <c r="MM9" s="29" t="n">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="MN9" s="29" t="n">
         <v>34</v>
@@ -16651,7 +16654,7 @@
         <v>21</v>
       </c>
       <c r="MZ9" s="29" t="n">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="NA9" s="29" t="n">
         <v>28</v>
@@ -16690,7 +16693,7 @@
         <v>33</v>
       </c>
       <c r="NM9" s="29" t="n">
-        <v>16</v>
+        <v>35</v>
       </c>
       <c r="NN9" s="29" t="n">
         <v>50</v>
@@ -16729,7 +16732,7 @@
         <v>18</v>
       </c>
       <c r="NZ9" s="29" t="n">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="OA9" s="29" t="n">
         <v>29</v>
@@ -16813,16 +16816,16 @@
         <v>21.0934471762864</v>
       </c>
       <c r="PB9" s="25" t="n">
-        <v>3.87543581374187</v>
+        <v>8.27365312211825</v>
       </c>
       <c r="PC9" s="25" t="n">
         <v>25.9808235385794</v>
       </c>
       <c r="PD9" s="25" t="n">
-        <v>27.577735351445</v>
+        <v>27.5777353514449</v>
       </c>
       <c r="PE9" s="25" t="n">
-        <v>36.0995966939889</v>
+        <v>36.0995966939888</v>
       </c>
       <c r="PF9" s="25" t="n">
         <v>31.6729652349235</v>
@@ -16852,7 +16855,7 @@
         <v>37.5073196608144</v>
       </c>
       <c r="PO9" s="25" t="n">
-        <v>17.5255175520074</v>
+        <v>38.6350906668497</v>
       </c>
       <c r="PP9" s="25" t="n">
         <v>56.4852300203805</v>
@@ -16891,7 +16894,7 @@
         <v>27.8119851657603</v>
       </c>
       <c r="QB9" s="25" t="n">
-        <v>5.13898531536718</v>
+        <v>10.8947662597267</v>
       </c>
       <c r="QC9" s="25" t="n">
         <v>36.2860097736636</v>
@@ -16930,7 +16933,7 @@
         <v>24.7792011444907</v>
       </c>
       <c r="QO9" s="25" t="n">
-        <v>11.4833476487372</v>
+        <v>25.1104498138086</v>
       </c>
       <c r="QP9" s="25" t="n">
         <v>37.7679634019357</v>
@@ -17993,7 +17996,7 @@
         <v>49</v>
       </c>
       <c r="MM10" s="29" t="n">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="MN10" s="29" t="n">
         <v>53</v>
@@ -18008,7 +18011,7 @@
         <v>58</v>
       </c>
       <c r="MR10" s="29" t="n">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="MS10" s="29" t="n">
         <v>66</v>
@@ -18032,7 +18035,7 @@
         <v>46</v>
       </c>
       <c r="MZ10" s="29" t="n">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="NA10" s="29" t="n">
         <v>51</v>
@@ -18071,7 +18074,7 @@
         <v>71</v>
       </c>
       <c r="NM10" s="29" t="n">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="NN10" s="29" t="n">
         <v>67</v>
@@ -18110,7 +18113,7 @@
         <v>61</v>
       </c>
       <c r="NZ10" s="29" t="n">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="OA10" s="29" t="n">
         <v>54</v>
@@ -18191,10 +18194,10 @@
         <v>0.843764143081404</v>
       </c>
       <c r="PA10" s="25" t="n">
-        <v>47.1479182343853</v>
+        <v>47.1479182343852</v>
       </c>
       <c r="PB10" s="25" t="n">
-        <v>53.6611490887787</v>
+        <v>39.4522146565577</v>
       </c>
       <c r="PC10" s="25" t="n">
         <v>55.0335196211626</v>
@@ -18206,13 +18209,13 @@
         <v>25.2133589307869</v>
       </c>
       <c r="PF10" s="25" t="n">
-        <v>64.7822363720813</v>
+        <v>64.7822363720812</v>
       </c>
       <c r="PG10" s="25" t="n">
-        <v>17.7422557329089</v>
+        <v>16.4827165782504</v>
       </c>
       <c r="PH10" s="25" t="n">
-        <v>50.613991257526</v>
+        <v>50.6139912575259</v>
       </c>
       <c r="PI10" s="25" t="n">
         <v>21.2077916366126</v>
@@ -18233,7 +18236,7 @@
         <v>69.0723068317792</v>
       </c>
       <c r="PO10" s="25" t="n">
-        <v>44.8413229406556</v>
+        <v>48.6275430037101</v>
       </c>
       <c r="PP10" s="25" t="n">
         <v>66.9741704985442</v>
@@ -18272,7 +18275,7 @@
         <v>64.926617169684</v>
       </c>
       <c r="QB10" s="25" t="n">
-        <v>73.9210013386079</v>
+        <v>54.7405821338403</v>
       </c>
       <c r="QC10" s="25" t="n">
         <v>68.8855863379048</v>
@@ -18287,7 +18290,7 @@
         <v>86.7990563292608</v>
       </c>
       <c r="QG10" s="25" t="n">
-        <v>12.9397720475342</v>
+        <v>10.8284537243925</v>
       </c>
       <c r="QH10" s="25" t="n">
         <v>70.9644761564981</v>
@@ -18311,7 +18314,7 @@
         <v>67.6349438776366</v>
       </c>
       <c r="QO10" s="25" t="n">
-        <v>42.889994072906</v>
+        <v>47.097680605551</v>
       </c>
       <c r="QP10" s="25" t="n">
         <v>59.0302599490193</v>
@@ -19374,7 +19377,7 @@
         <v>57</v>
       </c>
       <c r="MM11" s="29" t="n">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="MN11" s="29" t="n">
         <v>76</v>
@@ -19413,7 +19416,7 @@
         <v>37</v>
       </c>
       <c r="MZ11" s="29" t="n">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="NA11" s="29" t="n">
         <v>67</v>
@@ -19452,7 +19455,7 @@
         <v>71</v>
       </c>
       <c r="NM11" s="29" t="n">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="NN11" s="29" t="n">
         <v>71</v>
@@ -19491,7 +19494,7 @@
         <v>64</v>
       </c>
       <c r="NZ11" s="29" t="n">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="OA11" s="29" t="n">
         <v>65</v>
@@ -19575,7 +19578,7 @@
         <v>61.0020809233515</v>
       </c>
       <c r="PB11" s="25" t="n">
-        <v>75.8067266377541</v>
+        <v>71.0396690997364</v>
       </c>
       <c r="PC11" s="25" t="n">
         <v>117.483965121849</v>
@@ -19614,7 +19617,7 @@
         <v>101.543406542951</v>
       </c>
       <c r="PO11" s="25" t="n">
-        <v>63.417268256965</v>
+        <v>47.6740729628828</v>
       </c>
       <c r="PP11" s="25" t="n">
         <v>104.662130239603</v>
@@ -19653,7 +19656,7 @@
         <v>50.5022609094815</v>
       </c>
       <c r="QB11" s="25" t="n">
-        <v>62.7649371293407</v>
+        <v>58.9329405461773</v>
       </c>
       <c r="QC11" s="25" t="n">
         <v>97.2135957776166</v>
@@ -19692,7 +19695,7 @@
         <v>72.4675006882293</v>
       </c>
       <c r="QO11" s="25" t="n">
-        <v>45.0975937644931</v>
+        <v>34.145699505396</v>
       </c>
       <c r="QP11" s="25" t="n">
         <v>74.9016792834264</v>
@@ -21103,322 +21106,322 @@
         <v>1045</v>
       </c>
       <c r="MZ1" s="19" t="s">
-        <v>1046</v>
+        <v>1047</v>
       </c>
       <c r="NA1" s="19" t="s">
-        <v>1047</v>
+        <v>1048</v>
       </c>
       <c r="NB1" s="19" t="s">
-        <v>1048</v>
+        <v>1049</v>
       </c>
       <c r="NC1" s="19" t="s">
-        <v>1049</v>
+        <v>1050</v>
       </c>
       <c r="ND1" s="19" t="s">
-        <v>1050</v>
+        <v>1051</v>
       </c>
       <c r="NE1" s="19" t="s">
-        <v>1051</v>
+        <v>1052</v>
       </c>
       <c r="NF1" s="19" t="s">
-        <v>1052</v>
+        <v>1053</v>
       </c>
       <c r="NG1" s="19" t="s">
-        <v>1054</v>
+        <v>1055</v>
       </c>
       <c r="NH1" s="19" t="s">
-        <v>1056</v>
+        <v>1057</v>
       </c>
       <c r="NI1" s="19" t="s">
-        <v>1058</v>
+        <v>1059</v>
       </c>
       <c r="NJ1" s="19" t="s">
-        <v>1059</v>
+        <v>1060</v>
       </c>
       <c r="NK1" s="19" t="s">
-        <v>1060</v>
+        <v>1061</v>
       </c>
       <c r="NL1" s="20" t="s">
-        <v>1061</v>
+        <v>1062</v>
       </c>
       <c r="NM1" s="20" t="s">
-        <v>1062</v>
+        <v>1063</v>
       </c>
       <c r="NN1" s="20" t="s">
-        <v>1063</v>
+        <v>1064</v>
       </c>
       <c r="NO1" s="20" t="s">
-        <v>1064</v>
+        <v>1065</v>
       </c>
       <c r="NP1" s="20" t="s">
-        <v>1065</v>
+        <v>1066</v>
       </c>
       <c r="NQ1" s="20" t="s">
-        <v>1066</v>
+        <v>1067</v>
       </c>
       <c r="NR1" s="20" t="s">
-        <v>1067</v>
+        <v>1068</v>
       </c>
       <c r="NS1" s="20" t="s">
-        <v>1068</v>
+        <v>1069</v>
       </c>
       <c r="NT1" s="20" t="s">
-        <v>1069</v>
+        <v>1070</v>
       </c>
       <c r="NU1" s="20" t="s">
-        <v>1070</v>
+        <v>1071</v>
       </c>
       <c r="NV1" s="20" t="s">
-        <v>1071</v>
+        <v>1072</v>
       </c>
       <c r="NW1" s="20" t="s">
-        <v>1072</v>
+        <v>1073</v>
       </c>
       <c r="NX1" s="20" t="s">
-        <v>1073</v>
+        <v>1074</v>
       </c>
       <c r="NY1" s="20" t="s">
-        <v>1074</v>
+        <v>1075</v>
       </c>
       <c r="NZ1" s="20" t="s">
-        <v>1075</v>
+        <v>1076</v>
       </c>
       <c r="OA1" s="20" t="s">
-        <v>1076</v>
+        <v>1077</v>
       </c>
       <c r="OB1" s="20" t="s">
-        <v>1077</v>
+        <v>1078</v>
       </c>
       <c r="OC1" s="20" t="s">
-        <v>1078</v>
+        <v>1079</v>
       </c>
       <c r="OD1" s="20" t="s">
-        <v>1079</v>
+        <v>1080</v>
       </c>
       <c r="OE1" s="20" t="s">
-        <v>1080</v>
+        <v>1081</v>
       </c>
       <c r="OF1" s="20" t="s">
-        <v>1081</v>
+        <v>1082</v>
       </c>
       <c r="OG1" s="20" t="s">
-        <v>1083</v>
+        <v>1084</v>
       </c>
       <c r="OH1" s="20" t="s">
-        <v>1084</v>
+        <v>1085</v>
       </c>
       <c r="OI1" s="20" t="s">
-        <v>1086</v>
+        <v>1087</v>
       </c>
       <c r="OJ1" s="20" t="s">
-        <v>1087</v>
+        <v>1088</v>
       </c>
       <c r="OK1" s="20" t="s">
-        <v>1088</v>
+        <v>1089</v>
       </c>
       <c r="OL1" s="10" t="s">
-        <v>1090</v>
+        <v>1091</v>
       </c>
       <c r="OM1" s="10" t="s">
-        <v>1092</v>
+        <v>1093</v>
       </c>
       <c r="ON1" s="10" t="s">
-        <v>1093</v>
+        <v>1094</v>
       </c>
       <c r="OO1" s="9" t="s">
-        <v>1094</v>
+        <v>1095</v>
       </c>
       <c r="OP1" s="9" t="s">
-        <v>1096</v>
+        <v>1097</v>
       </c>
       <c r="OQ1" s="3" t="s">
-        <v>1098</v>
+        <v>1099</v>
       </c>
       <c r="OR1" s="3" t="s">
-        <v>1100</v>
+        <v>1101</v>
       </c>
       <c r="OS1" s="3" t="s">
-        <v>1101</v>
+        <v>1102</v>
       </c>
       <c r="OT1" s="9" t="s">
-        <v>1102</v>
+        <v>1103</v>
       </c>
       <c r="OU1" s="9" t="s">
-        <v>1103</v>
+        <v>1104</v>
       </c>
       <c r="OV1" s="9" t="s">
-        <v>1104</v>
+        <v>1105</v>
       </c>
       <c r="OW1" s="9" t="s">
-        <v>1105</v>
+        <v>1106</v>
       </c>
       <c r="OX1" s="9" t="s">
-        <v>1106</v>
+        <v>1107</v>
       </c>
       <c r="OY1" s="9" t="s">
-        <v>1107</v>
+        <v>1108</v>
       </c>
       <c r="OZ1" s="9" t="s">
-        <v>1108</v>
+        <v>1109</v>
       </c>
       <c r="PA1" s="21" t="s">
-        <v>1110</v>
+        <v>1111</v>
       </c>
       <c r="PB1" s="21" t="s">
-        <v>1112</v>
+        <v>1113</v>
       </c>
       <c r="PC1" s="21" t="s">
-        <v>1114</v>
+        <v>1115</v>
       </c>
       <c r="PD1" s="21" t="s">
-        <v>1116</v>
+        <v>1117</v>
       </c>
       <c r="PE1" s="21" t="s">
-        <v>1118</v>
+        <v>1119</v>
       </c>
       <c r="PF1" s="21" t="s">
-        <v>1120</v>
+        <v>1121</v>
       </c>
       <c r="PG1" s="21" t="s">
-        <v>1122</v>
+        <v>1123</v>
       </c>
       <c r="PH1" s="21" t="s">
-        <v>1124</v>
+        <v>1125</v>
       </c>
       <c r="PI1" s="21" t="s">
-        <v>1126</v>
+        <v>1127</v>
       </c>
       <c r="PJ1" s="21" t="s">
-        <v>1128</v>
+        <v>1129</v>
       </c>
       <c r="PK1" s="21" t="s">
-        <v>1130</v>
+        <v>1131</v>
       </c>
       <c r="PL1" s="21" t="s">
-        <v>1132</v>
+        <v>1133</v>
       </c>
       <c r="PM1" s="21" t="s">
-        <v>1134</v>
+        <v>1135</v>
       </c>
       <c r="PN1" s="19" t="s">
-        <v>1136</v>
+        <v>1137</v>
       </c>
       <c r="PO1" s="19" t="s">
-        <v>1138</v>
+        <v>1139</v>
       </c>
       <c r="PP1" s="19" t="s">
-        <v>1140</v>
+        <v>1141</v>
       </c>
       <c r="PQ1" s="19" t="s">
-        <v>1142</v>
+        <v>1143</v>
       </c>
       <c r="PR1" s="19" t="s">
-        <v>1144</v>
+        <v>1145</v>
       </c>
       <c r="PS1" s="19" t="s">
-        <v>1146</v>
+        <v>1147</v>
       </c>
       <c r="PT1" s="19" t="s">
-        <v>1148</v>
+        <v>1149</v>
       </c>
       <c r="PU1" s="19" t="s">
-        <v>1150</v>
+        <v>1151</v>
       </c>
       <c r="PV1" s="19" t="s">
-        <v>1152</v>
+        <v>1153</v>
       </c>
       <c r="PW1" s="19" t="s">
-        <v>1154</v>
+        <v>1155</v>
       </c>
       <c r="PX1" s="19" t="s">
-        <v>1156</v>
+        <v>1157</v>
       </c>
       <c r="PY1" s="19" t="s">
-        <v>1158</v>
+        <v>1159</v>
       </c>
       <c r="PZ1" s="19" t="s">
-        <v>1160</v>
+        <v>1161</v>
       </c>
       <c r="QA1" s="21" t="s">
-        <v>1162</v>
+        <v>1163</v>
       </c>
       <c r="QB1" s="21" t="s">
-        <v>1164</v>
+        <v>1165</v>
       </c>
       <c r="QC1" s="21" t="s">
-        <v>1166</v>
+        <v>1167</v>
       </c>
       <c r="QD1" s="21" t="s">
-        <v>1168</v>
+        <v>1169</v>
       </c>
       <c r="QE1" s="21" t="s">
-        <v>1170</v>
+        <v>1171</v>
       </c>
       <c r="QF1" s="21" t="s">
-        <v>1172</v>
+        <v>1173</v>
       </c>
       <c r="QG1" s="21" t="s">
-        <v>1174</v>
+        <v>1175</v>
       </c>
       <c r="QH1" s="21" t="s">
-        <v>1176</v>
+        <v>1177</v>
       </c>
       <c r="QI1" s="21" t="s">
-        <v>1178</v>
+        <v>1179</v>
       </c>
       <c r="QJ1" s="21" t="s">
-        <v>1180</v>
+        <v>1181</v>
       </c>
       <c r="QK1" s="21" t="s">
-        <v>1182</v>
+        <v>1183</v>
       </c>
       <c r="QL1" s="21" t="s">
-        <v>1184</v>
+        <v>1185</v>
       </c>
       <c r="QM1" s="21" t="s">
-        <v>1186</v>
+        <v>1187</v>
       </c>
       <c r="QN1" s="19" t="s">
-        <v>1188</v>
+        <v>1189</v>
       </c>
       <c r="QO1" s="19" t="s">
-        <v>1190</v>
+        <v>1191</v>
       </c>
       <c r="QP1" s="19" t="s">
-        <v>1192</v>
+        <v>1193</v>
       </c>
       <c r="QQ1" s="19" t="s">
-        <v>1194</v>
+        <v>1195</v>
       </c>
       <c r="QR1" s="19" t="s">
-        <v>1196</v>
+        <v>1197</v>
       </c>
       <c r="QS1" s="19" t="s">
-        <v>1198</v>
+        <v>1199</v>
       </c>
       <c r="QT1" s="19" t="s">
-        <v>1200</v>
+        <v>1201</v>
       </c>
       <c r="QU1" s="19" t="s">
-        <v>1202</v>
+        <v>1203</v>
       </c>
       <c r="QV1" s="19" t="s">
-        <v>1204</v>
+        <v>1205</v>
       </c>
       <c r="QW1" s="19" t="s">
-        <v>1206</v>
+        <v>1207</v>
       </c>
       <c r="QX1" s="19" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="QY1" s="19" t="s">
-        <v>1210</v>
+        <v>1211</v>
       </c>
       <c r="QZ1" s="19" t="s">
-        <v>1212</v>
+        <v>1213</v>
       </c>
       <c r="RA1" s="3" t="s">
-        <v>1214</v>
+        <v>1215</v>
       </c>
     </row>
     <row r="2">
@@ -22433,7 +22436,7 @@
         <v>63</v>
       </c>
       <c r="MM2" s="29" t="n">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="MN2" s="29" t="n">
         <v>76</v>
@@ -22472,7 +22475,7 @@
         <v>47</v>
       </c>
       <c r="MZ2" s="29" t="n">
-        <v>57</v>
+        <v>46</v>
       </c>
       <c r="NA2" s="29" t="n">
         <v>72</v>
@@ -22511,7 +22514,7 @@
         <v>65.9916718868485</v>
       </c>
       <c r="NM2" s="29" t="n">
-        <v>52.9351361407706</v>
+        <v>48.1651798960988</v>
       </c>
       <c r="NN2" s="29" t="n">
         <v>68.1843319187818</v>
@@ -22535,7 +22538,7 @@
         <v>58.4935831798678</v>
       </c>
       <c r="NU2" s="29" t="n">
-        <v>68.1637358289727</v>
+        <v>68.0993250658214</v>
       </c>
       <c r="NV2" s="29" t="n">
         <v>58.9182420625763</v>
@@ -22550,7 +22553,7 @@
         <v>63.6663550257398</v>
       </c>
       <c r="NZ2" s="29" t="n">
-        <v>44.9597728867684</v>
+        <v>38.4349863647282</v>
       </c>
       <c r="OA2" s="29" t="n">
         <v>67.030258528521</v>
@@ -22574,7 +22577,7 @@
         <v>50.8433719391288</v>
       </c>
       <c r="OH2" s="29" t="n">
-        <v>67.0468007743139</v>
+        <v>67.0110170170076</v>
       </c>
       <c r="OI2" s="29" t="n">
         <v>56.1140017049977</v>
@@ -22583,7 +22586,7 @@
         <v>63.0163547902429</v>
       </c>
       <c r="OK2" s="29" t="n">
-        <v>43.2909107607964</v>
+        <v>42.6417173377544</v>
       </c>
       <c r="OL2" s="22" t="n">
         <v>211</v>
@@ -22634,7 +22637,7 @@
         <v>72.6619597700568</v>
       </c>
       <c r="PB2" s="25" t="n">
-        <v>83.1416945170066</v>
+        <v>66.8545766278586</v>
       </c>
       <c r="PC2" s="25" t="n">
         <v>117.640621006597</v>
@@ -22649,7 +22652,7 @@
         <v>118.693098519419</v>
       </c>
       <c r="PG2" s="25" t="n">
-        <v>94.6922782888973</v>
+        <v>94.6674584422416</v>
       </c>
       <c r="PH2" s="25" t="n">
         <v>108.064546401517</v>
@@ -22658,7 +22661,7 @@
         <v>36.5023495513042</v>
       </c>
       <c r="PJ2" s="25" t="n">
-        <v>123.057468677466</v>
+        <v>122.998695800964</v>
       </c>
       <c r="PK2" s="25" t="n">
         <v>99.9937829973154</v>
@@ -22667,13 +22670,13 @@
         <v>105.869093064804</v>
       </c>
       <c r="PM2" s="25" t="n">
-        <v>80.2935890241642</v>
+        <v>80.2827525589517</v>
       </c>
       <c r="PN2" s="25" t="n">
         <v>91.9527509182466</v>
       </c>
       <c r="PO2" s="25" t="n">
-        <v>58.8572690001761</v>
+        <v>48.6357262376477</v>
       </c>
       <c r="PP2" s="25" t="n">
         <v>104.733423555764</v>
@@ -22697,7 +22700,7 @@
         <v>54.6269558563915</v>
       </c>
       <c r="PW2" s="25" t="n">
-        <v>106.042794848972</v>
+        <v>106.014229317612</v>
       </c>
       <c r="PX2" s="25" t="n">
         <v>83.8538521918065</v>
@@ -22706,13 +22709,13 @@
         <v>91.4786217624796</v>
       </c>
       <c r="PZ2" s="25" t="n">
-        <v>46.5603671912465</v>
+        <v>46.4304775726821</v>
       </c>
       <c r="QA2" s="25" t="n">
         <v>66.5518972827937</v>
       </c>
       <c r="QB2" s="25" t="n">
-        <v>78.033507483792</v>
+        <v>62.9365352710808</v>
       </c>
       <c r="QC2" s="25" t="n">
         <v>110.354042859017</v>
@@ -22727,7 +22730,7 @@
         <v>110.814812977949</v>
       </c>
       <c r="QG2" s="25" t="n">
-        <v>91.2933667180923</v>
+        <v>91.2517621384903</v>
       </c>
       <c r="QH2" s="25" t="n">
         <v>101.69882674781</v>
@@ -22736,7 +22739,7 @@
         <v>35.5090691453336</v>
       </c>
       <c r="QJ2" s="25" t="n">
-        <v>114.085497135402</v>
+        <v>114.011764982258</v>
       </c>
       <c r="QK2" s="25" t="n">
         <v>94.9010404844178</v>
@@ -22745,13 +22748,13 @@
         <v>99.4132247539213</v>
       </c>
       <c r="QM2" s="25" t="n">
-        <v>78.0895169147354</v>
+        <v>78.0770874130736</v>
       </c>
       <c r="QN2" s="25" t="n">
         <v>85.1457224445399</v>
       </c>
       <c r="QO2" s="25" t="n">
-        <v>55.1130700140601</v>
+        <v>45.3592755597441</v>
       </c>
       <c r="QP2" s="25" t="n">
         <v>97.4761401450092</v>
@@ -22775,7 +22778,7 @@
         <v>53.506016172586</v>
       </c>
       <c r="QW2" s="25" t="n">
-        <v>97.6928554913635</v>
+        <v>97.6551846876399</v>
       </c>
       <c r="QX2" s="25" t="n">
         <v>80.1989678532379</v>
@@ -22784,7 +22787,7 @@
         <v>84.6056979431081</v>
       </c>
       <c r="QZ2" s="25" t="n">
-        <v>47.3184947927219</v>
+        <v>47.1774346803506</v>
       </c>
       <c r="RA2" s="23" t="n">
         <v>31.4159265358979</v>
@@ -25686,7 +25689,7 @@
     </row>
     <row r="352">
       <c r="A352" t="s">
-        <v>714</v>
+        <v>812</v>
       </c>
       <c r="B352" t="s">
         <v>1030</v>
@@ -25790,10 +25793,10 @@
     </row>
     <row r="365">
       <c r="A365" t="s">
-        <v>797</v>
+        <v>1046</v>
       </c>
       <c r="B365" t="s">
-        <v>1046</v>
+        <v>1047</v>
       </c>
     </row>
     <row r="366">
@@ -25801,7 +25804,7 @@
         <v>717</v>
       </c>
       <c r="B366" t="s">
-        <v>1047</v>
+        <v>1048</v>
       </c>
     </row>
     <row r="367">
@@ -25809,7 +25812,7 @@
         <v>1035</v>
       </c>
       <c r="B367" t="s">
-        <v>1048</v>
+        <v>1049</v>
       </c>
     </row>
     <row r="368">
@@ -25817,7 +25820,7 @@
         <v>799</v>
       </c>
       <c r="B368" t="s">
-        <v>1049</v>
+        <v>1050</v>
       </c>
     </row>
     <row r="369">
@@ -25825,7 +25828,7 @@
         <v>816</v>
       </c>
       <c r="B369" t="s">
-        <v>1050</v>
+        <v>1051</v>
       </c>
     </row>
     <row r="370">
@@ -25833,7 +25836,7 @@
         <v>871</v>
       </c>
       <c r="B370" t="s">
-        <v>1051</v>
+        <v>1052</v>
       </c>
     </row>
     <row r="371">
@@ -25841,31 +25844,31 @@
         <v>816</v>
       </c>
       <c r="B371" t="s">
-        <v>1052</v>
+        <v>1053</v>
       </c>
     </row>
     <row r="372">
       <c r="A372" t="s">
-        <v>1053</v>
+        <v>1054</v>
       </c>
       <c r="B372" t="s">
-        <v>1054</v>
+        <v>1055</v>
       </c>
     </row>
     <row r="373">
       <c r="A373" t="s">
-        <v>1055</v>
+        <v>1056</v>
       </c>
       <c r="B373" t="s">
-        <v>1056</v>
+        <v>1057</v>
       </c>
     </row>
     <row r="374">
       <c r="A374" t="s">
-        <v>1057</v>
+        <v>1058</v>
       </c>
       <c r="B374" t="s">
-        <v>1058</v>
+        <v>1059</v>
       </c>
     </row>
     <row r="375">
@@ -25873,7 +25876,7 @@
         <v>754</v>
       </c>
       <c r="B375" t="s">
-        <v>1059</v>
+        <v>1060</v>
       </c>
     </row>
     <row r="376">
@@ -25881,7 +25884,7 @@
         <v>835</v>
       </c>
       <c r="B376" t="s">
-        <v>1060</v>
+        <v>1061</v>
       </c>
     </row>
     <row r="377">
@@ -25889,15 +25892,15 @@
         <v>808</v>
       </c>
       <c r="B377" t="s">
-        <v>1061</v>
+        <v>1062</v>
       </c>
     </row>
     <row r="378">
       <c r="A378" t="s">
-        <v>621</v>
+        <v>641</v>
       </c>
       <c r="B378" t="s">
-        <v>1062</v>
+        <v>1063</v>
       </c>
     </row>
     <row r="379">
@@ -25905,7 +25908,7 @@
         <v>746</v>
       </c>
       <c r="B379" t="s">
-        <v>1063</v>
+        <v>1064</v>
       </c>
     </row>
     <row r="380">
@@ -25913,7 +25916,7 @@
         <v>750</v>
       </c>
       <c r="B380" t="s">
-        <v>1064</v>
+        <v>1065</v>
       </c>
     </row>
     <row r="381">
@@ -25921,7 +25924,7 @@
         <v>808</v>
       </c>
       <c r="B381" t="s">
-        <v>1065</v>
+        <v>1066</v>
       </c>
     </row>
     <row r="382">
@@ -25929,7 +25932,7 @@
         <v>746</v>
       </c>
       <c r="B382" t="s">
-        <v>1066</v>
+        <v>1067</v>
       </c>
     </row>
     <row r="383">
@@ -25937,15 +25940,15 @@
         <v>871</v>
       </c>
       <c r="B383" t="s">
-        <v>1067</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="384">
       <c r="A384" t="s">
-        <v>1057</v>
+        <v>1058</v>
       </c>
       <c r="B384" t="s">
-        <v>1068</v>
+        <v>1069</v>
       </c>
     </row>
     <row r="385">
@@ -25953,7 +25956,7 @@
         <v>738</v>
       </c>
       <c r="B385" t="s">
-        <v>1069</v>
+        <v>1070</v>
       </c>
     </row>
     <row r="386">
@@ -25961,7 +25964,7 @@
         <v>746</v>
       </c>
       <c r="B386" t="s">
-        <v>1070</v>
+        <v>1071</v>
       </c>
     </row>
     <row r="387">
@@ -25969,7 +25972,7 @@
         <v>777</v>
       </c>
       <c r="B387" t="s">
-        <v>1071</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="388">
@@ -25977,7 +25980,7 @@
         <v>808</v>
       </c>
       <c r="B388" t="s">
-        <v>1072</v>
+        <v>1073</v>
       </c>
     </row>
     <row r="389">
@@ -25985,23 +25988,23 @@
         <v>1038</v>
       </c>
       <c r="B389" t="s">
-        <v>1073</v>
+        <v>1074</v>
       </c>
     </row>
     <row r="390">
       <c r="A390" t="s">
-        <v>1057</v>
+        <v>1058</v>
       </c>
       <c r="B390" t="s">
-        <v>1074</v>
+        <v>1075</v>
       </c>
     </row>
     <row r="391">
       <c r="A391" t="s">
-        <v>1038</v>
+        <v>649</v>
       </c>
       <c r="B391" t="s">
-        <v>1075</v>
+        <v>1076</v>
       </c>
     </row>
     <row r="392">
@@ -26009,7 +26012,7 @@
         <v>754</v>
       </c>
       <c r="B392" t="s">
-        <v>1076</v>
+        <v>1077</v>
       </c>
     </row>
     <row r="393">
@@ -26017,7 +26020,7 @@
         <v>750</v>
       </c>
       <c r="B393" t="s">
-        <v>1077</v>
+        <v>1078</v>
       </c>
     </row>
     <row r="394">
@@ -26025,7 +26028,7 @@
         <v>779</v>
       </c>
       <c r="B394" t="s">
-        <v>1078</v>
+        <v>1079</v>
       </c>
     </row>
     <row r="395">
@@ -26033,7 +26036,7 @@
         <v>754</v>
       </c>
       <c r="B395" t="s">
-        <v>1079</v>
+        <v>1080</v>
       </c>
     </row>
     <row r="396">
@@ -26041,23 +26044,23 @@
         <v>748</v>
       </c>
       <c r="B396" t="s">
-        <v>1080</v>
+        <v>1081</v>
       </c>
     </row>
     <row r="397">
       <c r="A397" t="s">
-        <v>1057</v>
+        <v>1058</v>
       </c>
       <c r="B397" t="s">
-        <v>1081</v>
+        <v>1082</v>
       </c>
     </row>
     <row r="398">
       <c r="A398" t="s">
-        <v>1082</v>
+        <v>1083</v>
       </c>
       <c r="B398" t="s">
-        <v>1083</v>
+        <v>1084</v>
       </c>
     </row>
     <row r="399">
@@ -26065,15 +26068,15 @@
         <v>754</v>
       </c>
       <c r="B399" t="s">
-        <v>1084</v>
+        <v>1085</v>
       </c>
     </row>
     <row r="400">
       <c r="A400" t="s">
-        <v>1085</v>
+        <v>1086</v>
       </c>
       <c r="B400" t="s">
-        <v>1086</v>
+        <v>1087</v>
       </c>
     </row>
     <row r="401">
@@ -26081,7 +26084,7 @@
         <v>804</v>
       </c>
       <c r="B401" t="s">
-        <v>1087</v>
+        <v>1088</v>
       </c>
     </row>
     <row r="402">
@@ -26089,23 +26092,23 @@
         <v>742</v>
       </c>
       <c r="B402" t="s">
-        <v>1088</v>
+        <v>1089</v>
       </c>
     </row>
     <row r="403">
       <c r="A403" t="s">
-        <v>1089</v>
+        <v>1090</v>
       </c>
       <c r="B403" t="s">
-        <v>1090</v>
+        <v>1091</v>
       </c>
     </row>
     <row r="404">
       <c r="A404" t="s">
-        <v>1091</v>
+        <v>1092</v>
       </c>
       <c r="B404" t="s">
-        <v>1092</v>
+        <v>1093</v>
       </c>
     </row>
     <row r="405">
@@ -26113,7 +26116,7 @@
         <v>7</v>
       </c>
       <c r="B405" t="s">
-        <v>1093</v>
+        <v>1094</v>
       </c>
     </row>
     <row r="406">
@@ -26121,31 +26124,31 @@
         <v>982</v>
       </c>
       <c r="B406" t="s">
-        <v>1094</v>
+        <v>1095</v>
       </c>
     </row>
     <row r="407">
       <c r="A407" t="s">
-        <v>1095</v>
+        <v>1096</v>
       </c>
       <c r="B407" t="s">
-        <v>1096</v>
+        <v>1097</v>
       </c>
     </row>
     <row r="408">
       <c r="A408" t="s">
-        <v>1097</v>
+        <v>1098</v>
       </c>
       <c r="B408" t="s">
-        <v>1098</v>
+        <v>1099</v>
       </c>
     </row>
     <row r="409">
       <c r="A409" t="s">
-        <v>1099</v>
+        <v>1100</v>
       </c>
       <c r="B409" t="s">
-        <v>1100</v>
+        <v>1101</v>
       </c>
     </row>
     <row r="410">
@@ -26153,7 +26156,7 @@
         <v>562</v>
       </c>
       <c r="B410" t="s">
-        <v>1101</v>
+        <v>1102</v>
       </c>
     </row>
     <row r="411">
@@ -26161,7 +26164,7 @@
         <v>674</v>
       </c>
       <c r="B411" t="s">
-        <v>1102</v>
+        <v>1103</v>
       </c>
     </row>
     <row r="412">
@@ -26169,7 +26172,7 @@
         <v>627</v>
       </c>
       <c r="B412" t="s">
-        <v>1103</v>
+        <v>1104</v>
       </c>
     </row>
     <row r="413">
@@ -26177,7 +26180,7 @@
         <v>562</v>
       </c>
       <c r="B413" t="s">
-        <v>1104</v>
+        <v>1105</v>
       </c>
     </row>
     <row r="414">
@@ -26185,7 +26188,7 @@
         <v>562</v>
       </c>
       <c r="B414" t="s">
-        <v>1105</v>
+        <v>1106</v>
       </c>
     </row>
     <row r="415">
@@ -26193,7 +26196,7 @@
         <v>514</v>
       </c>
       <c r="B415" t="s">
-        <v>1106</v>
+        <v>1107</v>
       </c>
     </row>
     <row r="416">
@@ -26201,7 +26204,7 @@
         <v>857</v>
       </c>
       <c r="B416" t="s">
-        <v>1107</v>
+        <v>1108</v>
       </c>
     </row>
     <row r="417">
@@ -26209,431 +26212,431 @@
         <v>621</v>
       </c>
       <c r="B417" t="s">
-        <v>1108</v>
+        <v>1109</v>
       </c>
     </row>
     <row r="418">
       <c r="A418" t="s">
-        <v>1109</v>
+        <v>1110</v>
       </c>
       <c r="B418" t="s">
-        <v>1110</v>
+        <v>1111</v>
       </c>
     </row>
     <row r="419">
       <c r="A419" t="s">
-        <v>1111</v>
+        <v>1112</v>
       </c>
       <c r="B419" t="s">
-        <v>1112</v>
+        <v>1113</v>
       </c>
     </row>
     <row r="420">
       <c r="A420" t="s">
-        <v>1113</v>
+        <v>1114</v>
       </c>
       <c r="B420" t="s">
-        <v>1114</v>
+        <v>1115</v>
       </c>
     </row>
     <row r="421">
       <c r="A421" t="s">
-        <v>1115</v>
+        <v>1116</v>
       </c>
       <c r="B421" t="s">
-        <v>1116</v>
+        <v>1117</v>
       </c>
     </row>
     <row r="422">
       <c r="A422" t="s">
-        <v>1117</v>
+        <v>1118</v>
       </c>
       <c r="B422" t="s">
-        <v>1118</v>
+        <v>1119</v>
       </c>
     </row>
     <row r="423">
       <c r="A423" t="s">
-        <v>1119</v>
+        <v>1120</v>
       </c>
       <c r="B423" t="s">
-        <v>1120</v>
+        <v>1121</v>
       </c>
     </row>
     <row r="424">
       <c r="A424" t="s">
-        <v>1121</v>
+        <v>1122</v>
       </c>
       <c r="B424" t="s">
-        <v>1122</v>
+        <v>1123</v>
       </c>
     </row>
     <row r="425">
       <c r="A425" t="s">
-        <v>1123</v>
+        <v>1124</v>
       </c>
       <c r="B425" t="s">
-        <v>1124</v>
+        <v>1125</v>
       </c>
     </row>
     <row r="426">
       <c r="A426" t="s">
-        <v>1125</v>
+        <v>1126</v>
       </c>
       <c r="B426" t="s">
-        <v>1126</v>
+        <v>1127</v>
       </c>
     </row>
     <row r="427">
       <c r="A427" t="s">
-        <v>1127</v>
+        <v>1128</v>
       </c>
       <c r="B427" t="s">
-        <v>1128</v>
+        <v>1129</v>
       </c>
     </row>
     <row r="428">
       <c r="A428" t="s">
-        <v>1129</v>
+        <v>1130</v>
       </c>
       <c r="B428" t="s">
-        <v>1130</v>
+        <v>1131</v>
       </c>
     </row>
     <row r="429">
       <c r="A429" t="s">
-        <v>1131</v>
+        <v>1132</v>
       </c>
       <c r="B429" t="s">
-        <v>1132</v>
+        <v>1133</v>
       </c>
     </row>
     <row r="430">
       <c r="A430" t="s">
-        <v>1133</v>
+        <v>1134</v>
       </c>
       <c r="B430" t="s">
-        <v>1134</v>
+        <v>1135</v>
       </c>
     </row>
     <row r="431">
       <c r="A431" t="s">
-        <v>1135</v>
+        <v>1136</v>
       </c>
       <c r="B431" t="s">
-        <v>1136</v>
+        <v>1137</v>
       </c>
     </row>
     <row r="432">
       <c r="A432" t="s">
-        <v>1137</v>
+        <v>1138</v>
       </c>
       <c r="B432" t="s">
-        <v>1138</v>
+        <v>1139</v>
       </c>
     </row>
     <row r="433">
       <c r="A433" t="s">
-        <v>1139</v>
+        <v>1140</v>
       </c>
       <c r="B433" t="s">
-        <v>1140</v>
+        <v>1141</v>
       </c>
     </row>
     <row r="434">
       <c r="A434" t="s">
-        <v>1141</v>
+        <v>1142</v>
       </c>
       <c r="B434" t="s">
-        <v>1142</v>
+        <v>1143</v>
       </c>
     </row>
     <row r="435">
       <c r="A435" t="s">
-        <v>1143</v>
+        <v>1144</v>
       </c>
       <c r="B435" t="s">
-        <v>1144</v>
+        <v>1145</v>
       </c>
     </row>
     <row r="436">
       <c r="A436" t="s">
-        <v>1145</v>
+        <v>1146</v>
       </c>
       <c r="B436" t="s">
-        <v>1146</v>
+        <v>1147</v>
       </c>
     </row>
     <row r="437">
       <c r="A437" t="s">
-        <v>1147</v>
+        <v>1148</v>
       </c>
       <c r="B437" t="s">
-        <v>1148</v>
+        <v>1149</v>
       </c>
     </row>
     <row r="438">
       <c r="A438" t="s">
-        <v>1149</v>
+        <v>1150</v>
       </c>
       <c r="B438" t="s">
-        <v>1150</v>
+        <v>1151</v>
       </c>
     </row>
     <row r="439">
       <c r="A439" t="s">
-        <v>1151</v>
+        <v>1152</v>
       </c>
       <c r="B439" t="s">
-        <v>1152</v>
+        <v>1153</v>
       </c>
     </row>
     <row r="440">
       <c r="A440" t="s">
-        <v>1153</v>
+        <v>1154</v>
       </c>
       <c r="B440" t="s">
-        <v>1154</v>
+        <v>1155</v>
       </c>
     </row>
     <row r="441">
       <c r="A441" t="s">
-        <v>1155</v>
+        <v>1156</v>
       </c>
       <c r="B441" t="s">
-        <v>1156</v>
+        <v>1157</v>
       </c>
     </row>
     <row r="442">
       <c r="A442" t="s">
-        <v>1157</v>
+        <v>1158</v>
       </c>
       <c r="B442" t="s">
-        <v>1158</v>
+        <v>1159</v>
       </c>
     </row>
     <row r="443">
       <c r="A443" t="s">
-        <v>1159</v>
+        <v>1160</v>
       </c>
       <c r="B443" t="s">
-        <v>1160</v>
+        <v>1161</v>
       </c>
     </row>
     <row r="444">
       <c r="A444" t="s">
-        <v>1161</v>
+        <v>1162</v>
       </c>
       <c r="B444" t="s">
-        <v>1162</v>
+        <v>1163</v>
       </c>
     </row>
     <row r="445">
       <c r="A445" t="s">
-        <v>1163</v>
+        <v>1164</v>
       </c>
       <c r="B445" t="s">
-        <v>1164</v>
+        <v>1165</v>
       </c>
     </row>
     <row r="446">
       <c r="A446" t="s">
-        <v>1165</v>
+        <v>1166</v>
       </c>
       <c r="B446" t="s">
-        <v>1166</v>
+        <v>1167</v>
       </c>
     </row>
     <row r="447">
       <c r="A447" t="s">
-        <v>1167</v>
+        <v>1168</v>
       </c>
       <c r="B447" t="s">
-        <v>1168</v>
+        <v>1169</v>
       </c>
     </row>
     <row r="448">
       <c r="A448" t="s">
-        <v>1169</v>
+        <v>1170</v>
       </c>
       <c r="B448" t="s">
-        <v>1170</v>
+        <v>1171</v>
       </c>
     </row>
     <row r="449">
       <c r="A449" t="s">
-        <v>1171</v>
+        <v>1172</v>
       </c>
       <c r="B449" t="s">
-        <v>1172</v>
+        <v>1173</v>
       </c>
     </row>
     <row r="450">
       <c r="A450" t="s">
-        <v>1173</v>
+        <v>1174</v>
       </c>
       <c r="B450" t="s">
-        <v>1174</v>
+        <v>1175</v>
       </c>
     </row>
     <row r="451">
       <c r="A451" t="s">
-        <v>1175</v>
+        <v>1176</v>
       </c>
       <c r="B451" t="s">
-        <v>1176</v>
+        <v>1177</v>
       </c>
     </row>
     <row r="452">
       <c r="A452" t="s">
-        <v>1177</v>
+        <v>1178</v>
       </c>
       <c r="B452" t="s">
-        <v>1178</v>
+        <v>1179</v>
       </c>
     </row>
     <row r="453">
       <c r="A453" t="s">
-        <v>1179</v>
+        <v>1180</v>
       </c>
       <c r="B453" t="s">
-        <v>1180</v>
+        <v>1181</v>
       </c>
     </row>
     <row r="454">
       <c r="A454" t="s">
-        <v>1181</v>
+        <v>1182</v>
       </c>
       <c r="B454" t="s">
-        <v>1182</v>
+        <v>1183</v>
       </c>
     </row>
     <row r="455">
       <c r="A455" t="s">
-        <v>1183</v>
+        <v>1184</v>
       </c>
       <c r="B455" t="s">
-        <v>1184</v>
+        <v>1185</v>
       </c>
     </row>
     <row r="456">
       <c r="A456" t="s">
-        <v>1185</v>
+        <v>1186</v>
       </c>
       <c r="B456" t="s">
-        <v>1186</v>
+        <v>1187</v>
       </c>
     </row>
     <row r="457">
       <c r="A457" t="s">
-        <v>1187</v>
+        <v>1188</v>
       </c>
       <c r="B457" t="s">
-        <v>1188</v>
+        <v>1189</v>
       </c>
     </row>
     <row r="458">
       <c r="A458" t="s">
-        <v>1189</v>
+        <v>1190</v>
       </c>
       <c r="B458" t="s">
-        <v>1190</v>
+        <v>1191</v>
       </c>
     </row>
     <row r="459">
       <c r="A459" t="s">
-        <v>1191</v>
+        <v>1192</v>
       </c>
       <c r="B459" t="s">
-        <v>1192</v>
+        <v>1193</v>
       </c>
     </row>
     <row r="460">
       <c r="A460" t="s">
-        <v>1193</v>
+        <v>1194</v>
       </c>
       <c r="B460" t="s">
-        <v>1194</v>
+        <v>1195</v>
       </c>
     </row>
     <row r="461">
       <c r="A461" t="s">
-        <v>1195</v>
+        <v>1196</v>
       </c>
       <c r="B461" t="s">
-        <v>1196</v>
+        <v>1197</v>
       </c>
     </row>
     <row r="462">
       <c r="A462" t="s">
-        <v>1197</v>
+        <v>1198</v>
       </c>
       <c r="B462" t="s">
-        <v>1198</v>
+        <v>1199</v>
       </c>
     </row>
     <row r="463">
       <c r="A463" t="s">
-        <v>1199</v>
+        <v>1200</v>
       </c>
       <c r="B463" t="s">
-        <v>1200</v>
+        <v>1201</v>
       </c>
     </row>
     <row r="464">
       <c r="A464" t="s">
-        <v>1201</v>
+        <v>1202</v>
       </c>
       <c r="B464" t="s">
-        <v>1202</v>
+        <v>1203</v>
       </c>
     </row>
     <row r="465">
       <c r="A465" t="s">
-        <v>1203</v>
+        <v>1204</v>
       </c>
       <c r="B465" t="s">
-        <v>1204</v>
+        <v>1205</v>
       </c>
     </row>
     <row r="466">
       <c r="A466" t="s">
-        <v>1205</v>
+        <v>1206</v>
       </c>
       <c r="B466" t="s">
-        <v>1206</v>
+        <v>1207</v>
       </c>
     </row>
     <row r="467">
       <c r="A467" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="B467" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
     </row>
     <row r="468">
       <c r="A468" t="s">
-        <v>1209</v>
+        <v>1210</v>
       </c>
       <c r="B468" t="s">
-        <v>1210</v>
+        <v>1211</v>
       </c>
     </row>
     <row r="469">
       <c r="A469" t="s">
-        <v>1211</v>
+        <v>1212</v>
       </c>
       <c r="B469" t="s">
-        <v>1212</v>
+        <v>1213</v>
       </c>
     </row>
     <row r="470">
       <c r="A470" t="s">
-        <v>1213</v>
+        <v>1214</v>
       </c>
       <c r="B470" t="s">
-        <v>1214</v>
+        <v>1215</v>
       </c>
     </row>
   </sheetData>
@@ -26842,13 +26845,13 @@
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B5" t="n">
         <v>0</v>
       </c>
       <c r="C5" t="n">
-        <v>74</v>
+        <v>63</v>
       </c>
       <c r="D5" t="n">
         <v>0</v>
@@ -26887,13 +26890,13 @@
         <v>91</v>
       </c>
       <c r="B8" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C8" t="n">
         <v>86</v>
       </c>
       <c r="D8" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9">

</xml_diff>

<commit_message>
Redo testoutput objects and files, and pkgdown
</commit_message>
<xml_diff>
--- a/inst/testdata/examples_of_output/testoutput_ejam2excel_10pts_1miles.xlsx
+++ b/inst/testdata/examples_of_output/testoutput_ejam2excel_10pts_1miles.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1216" uniqueCount="1216">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1215" uniqueCount="1215">
   <si>
     <t xml:space="preserve">Analysis Title</t>
   </si>
@@ -3164,9 +3164,6 @@
     <t xml:space="preserve">US percentile for Supplemental Summary Index for Particulate Matter</t>
   </si>
   <si>
-    <t xml:space="preserve">46</t>
-  </si>
-  <si>
     <t xml:space="preserve">US percentile for Supplemental Summary Index for Ozone</t>
   </si>
   <si>
@@ -3362,7 +3359,7 @@
     <t xml:space="preserve">US type of raw score for Particulate Matter Summary Index</t>
   </si>
   <si>
-    <t xml:space="preserve">66.855</t>
+    <t xml:space="preserve">83.142</t>
   </si>
   <si>
     <t xml:space="preserve">US type of raw score for Ozone Summary Index</t>
@@ -3392,7 +3389,7 @@
     <t xml:space="preserve">US type of raw score for Traffic Proximity and Volume Summary Index</t>
   </si>
   <si>
-    <t xml:space="preserve">94.667</t>
+    <t xml:space="preserve">94.692</t>
   </si>
   <si>
     <t xml:space="preserve">US type of raw score for Lead Paint Summary Index</t>
@@ -3410,7 +3407,7 @@
     <t xml:space="preserve">US type of raw score for RMP Proximity Summary Index</t>
   </si>
   <si>
-    <t xml:space="preserve">122.999</t>
+    <t xml:space="preserve">123.057</t>
   </si>
   <si>
     <t xml:space="preserve">US type of raw score for Hazardous Waste Proximity Summary Index</t>
@@ -3428,7 +3425,7 @@
     <t xml:space="preserve">US type of raw score for Wastewater Discharge Summary Index</t>
   </si>
   <si>
-    <t xml:space="preserve">80.283</t>
+    <t xml:space="preserve">80.294</t>
   </si>
   <si>
     <t xml:space="preserve">US type of raw score for Drinking Water Non-Compliance Summary Index</t>
@@ -3440,7 +3437,7 @@
     <t xml:space="preserve">State type of raw score for Particulate Matter Summary Index</t>
   </si>
   <si>
-    <t xml:space="preserve">48.636</t>
+    <t xml:space="preserve">58.857</t>
   </si>
   <si>
     <t xml:space="preserve">State type of raw score for Ozone Summary Index</t>
@@ -3488,7 +3485,7 @@
     <t xml:space="preserve">State type of raw score for RMP Proximity Summary Index</t>
   </si>
   <si>
-    <t xml:space="preserve">106.014</t>
+    <t xml:space="preserve">106.043</t>
   </si>
   <si>
     <t xml:space="preserve">State type of raw score for Hazardous Waste Proximity Summary Index</t>
@@ -3506,7 +3503,7 @@
     <t xml:space="preserve">State type of raw score for Wastewater Discharge Summary Index</t>
   </si>
   <si>
-    <t xml:space="preserve">46.43</t>
+    <t xml:space="preserve">46.56</t>
   </si>
   <si>
     <t xml:space="preserve">State type of raw score for Drinking Water Non-Compliance Summary Index</t>
@@ -3518,7 +3515,7 @@
     <t xml:space="preserve">US type of raw score for Particulate Matter Supplemental Summary Index</t>
   </si>
   <si>
-    <t xml:space="preserve">62.937</t>
+    <t xml:space="preserve">78.034</t>
   </si>
   <si>
     <t xml:space="preserve">US type of raw score for Ozone Supplemental Summary Index</t>
@@ -3548,7 +3545,7 @@
     <t xml:space="preserve">US type of raw score for Traffic Proximity and Volume Supplemental Summary Index</t>
   </si>
   <si>
-    <t xml:space="preserve">91.252</t>
+    <t xml:space="preserve">91.293</t>
   </si>
   <si>
     <t xml:space="preserve">US type of raw score for Lead Paint Supplemental Summary Index</t>
@@ -3566,7 +3563,7 @@
     <t xml:space="preserve">US type of raw score for RMP Proximity Supplemental Summary Index</t>
   </si>
   <si>
-    <t xml:space="preserve">114.012</t>
+    <t xml:space="preserve">114.085</t>
   </si>
   <si>
     <t xml:space="preserve">US type of raw score for Hazardous Waste Proximity Supplemental Summary Index</t>
@@ -3584,7 +3581,7 @@
     <t xml:space="preserve">US type of raw score for Wastewater Discharge Supplemental Summary Index</t>
   </si>
   <si>
-    <t xml:space="preserve">78.077</t>
+    <t xml:space="preserve">78.09</t>
   </si>
   <si>
     <t xml:space="preserve">US type of raw score for Drinking Water Non-Compliance Supplemental Summary Index</t>
@@ -3596,7 +3593,7 @@
     <t xml:space="preserve">State type of raw score for Particulate Matter Supplemental Summary Index</t>
   </si>
   <si>
-    <t xml:space="preserve">45.359</t>
+    <t xml:space="preserve">55.113</t>
   </si>
   <si>
     <t xml:space="preserve">State type of raw score for Ozone Supplemental Summary Index</t>
@@ -3644,7 +3641,7 @@
     <t xml:space="preserve">State type of raw score for RMP Proximity Supplemental Summary Index</t>
   </si>
   <si>
-    <t xml:space="preserve">97.655</t>
+    <t xml:space="preserve">97.693</t>
   </si>
   <si>
     <t xml:space="preserve">State type of raw score for Hazardous Waste Proximity Supplemental Summary Index</t>
@@ -3662,7 +3659,7 @@
     <t xml:space="preserve">State type of raw score for Wastewater Discharge Supplemental Summary Index</t>
   </si>
   <si>
-    <t xml:space="preserve">47.177</t>
+    <t xml:space="preserve">47.318</t>
   </si>
   <si>
     <t xml:space="preserve">State type of raw score for Drinking Water Non-Compliance Supplemental Summary Index</t>
@@ -5622,322 +5619,322 @@
         <v>1045</v>
       </c>
       <c r="MZ1" s="19" t="s">
+        <v>1046</v>
+      </c>
+      <c r="NA1" s="19" t="s">
         <v>1047</v>
       </c>
-      <c r="NA1" s="19" t="s">
+      <c r="NB1" s="19" t="s">
         <v>1048</v>
       </c>
-      <c r="NB1" s="19" t="s">
+      <c r="NC1" s="19" t="s">
         <v>1049</v>
       </c>
-      <c r="NC1" s="19" t="s">
+      <c r="ND1" s="19" t="s">
         <v>1050</v>
       </c>
-      <c r="ND1" s="19" t="s">
+      <c r="NE1" s="19" t="s">
         <v>1051</v>
       </c>
-      <c r="NE1" s="19" t="s">
+      <c r="NF1" s="19" t="s">
         <v>1052</v>
       </c>
-      <c r="NF1" s="19" t="s">
-        <v>1053</v>
-      </c>
       <c r="NG1" s="19" t="s">
-        <v>1055</v>
+        <v>1054</v>
       </c>
       <c r="NH1" s="19" t="s">
-        <v>1057</v>
+        <v>1056</v>
       </c>
       <c r="NI1" s="19" t="s">
+        <v>1058</v>
+      </c>
+      <c r="NJ1" s="19" t="s">
         <v>1059</v>
       </c>
-      <c r="NJ1" s="19" t="s">
+      <c r="NK1" s="19" t="s">
         <v>1060</v>
       </c>
-      <c r="NK1" s="19" t="s">
+      <c r="NL1" s="20" t="s">
         <v>1061</v>
       </c>
-      <c r="NL1" s="20" t="s">
+      <c r="NM1" s="20" t="s">
         <v>1062</v>
       </c>
-      <c r="NM1" s="20" t="s">
+      <c r="NN1" s="20" t="s">
         <v>1063</v>
       </c>
-      <c r="NN1" s="20" t="s">
+      <c r="NO1" s="20" t="s">
         <v>1064</v>
       </c>
-      <c r="NO1" s="20" t="s">
+      <c r="NP1" s="20" t="s">
         <v>1065</v>
       </c>
-      <c r="NP1" s="20" t="s">
+      <c r="NQ1" s="20" t="s">
         <v>1066</v>
       </c>
-      <c r="NQ1" s="20" t="s">
+      <c r="NR1" s="20" t="s">
         <v>1067</v>
       </c>
-      <c r="NR1" s="20" t="s">
+      <c r="NS1" s="20" t="s">
         <v>1068</v>
       </c>
-      <c r="NS1" s="20" t="s">
+      <c r="NT1" s="20" t="s">
         <v>1069</v>
       </c>
-      <c r="NT1" s="20" t="s">
+      <c r="NU1" s="20" t="s">
         <v>1070</v>
       </c>
-      <c r="NU1" s="20" t="s">
+      <c r="NV1" s="20" t="s">
         <v>1071</v>
       </c>
-      <c r="NV1" s="20" t="s">
+      <c r="NW1" s="20" t="s">
         <v>1072</v>
       </c>
-      <c r="NW1" s="20" t="s">
+      <c r="NX1" s="20" t="s">
         <v>1073</v>
       </c>
-      <c r="NX1" s="20" t="s">
+      <c r="NY1" s="20" t="s">
         <v>1074</v>
       </c>
-      <c r="NY1" s="20" t="s">
+      <c r="NZ1" s="20" t="s">
         <v>1075</v>
       </c>
-      <c r="NZ1" s="20" t="s">
+      <c r="OA1" s="20" t="s">
         <v>1076</v>
       </c>
-      <c r="OA1" s="20" t="s">
+      <c r="OB1" s="20" t="s">
         <v>1077</v>
       </c>
-      <c r="OB1" s="20" t="s">
+      <c r="OC1" s="20" t="s">
         <v>1078</v>
       </c>
-      <c r="OC1" s="20" t="s">
+      <c r="OD1" s="20" t="s">
         <v>1079</v>
       </c>
-      <c r="OD1" s="20" t="s">
+      <c r="OE1" s="20" t="s">
         <v>1080</v>
       </c>
-      <c r="OE1" s="20" t="s">
+      <c r="OF1" s="20" t="s">
         <v>1081</v>
       </c>
-      <c r="OF1" s="20" t="s">
-        <v>1082</v>
-      </c>
       <c r="OG1" s="20" t="s">
+        <v>1083</v>
+      </c>
+      <c r="OH1" s="20" t="s">
         <v>1084</v>
       </c>
-      <c r="OH1" s="20" t="s">
-        <v>1085</v>
-      </c>
       <c r="OI1" s="20" t="s">
+        <v>1086</v>
+      </c>
+      <c r="OJ1" s="20" t="s">
         <v>1087</v>
       </c>
-      <c r="OJ1" s="20" t="s">
+      <c r="OK1" s="20" t="s">
         <v>1088</v>
       </c>
-      <c r="OK1" s="20" t="s">
-        <v>1089</v>
-      </c>
       <c r="OL1" s="10" t="s">
-        <v>1091</v>
+        <v>1090</v>
       </c>
       <c r="OM1" s="10" t="s">
+        <v>1092</v>
+      </c>
+      <c r="ON1" s="10" t="s">
         <v>1093</v>
       </c>
-      <c r="ON1" s="10" t="s">
+      <c r="OO1" s="9" t="s">
         <v>1094</v>
       </c>
-      <c r="OO1" s="9" t="s">
-        <v>1095</v>
-      </c>
       <c r="OP1" s="9" t="s">
-        <v>1097</v>
+        <v>1096</v>
       </c>
       <c r="OQ1" s="3" t="s">
-        <v>1099</v>
+        <v>1098</v>
       </c>
       <c r="OR1" s="3" t="s">
+        <v>1100</v>
+      </c>
+      <c r="OS1" s="3" t="s">
         <v>1101</v>
       </c>
-      <c r="OS1" s="3" t="s">
+      <c r="OT1" s="9" t="s">
         <v>1102</v>
       </c>
-      <c r="OT1" s="9" t="s">
+      <c r="OU1" s="9" t="s">
         <v>1103</v>
       </c>
-      <c r="OU1" s="9" t="s">
+      <c r="OV1" s="9" t="s">
         <v>1104</v>
       </c>
-      <c r="OV1" s="9" t="s">
+      <c r="OW1" s="9" t="s">
         <v>1105</v>
       </c>
-      <c r="OW1" s="9" t="s">
+      <c r="OX1" s="9" t="s">
         <v>1106</v>
       </c>
-      <c r="OX1" s="9" t="s">
+      <c r="OY1" s="9" t="s">
         <v>1107</v>
       </c>
-      <c r="OY1" s="9" t="s">
+      <c r="OZ1" s="9" t="s">
         <v>1108</v>
       </c>
-      <c r="OZ1" s="9" t="s">
-        <v>1109</v>
-      </c>
       <c r="PA1" s="21" t="s">
-        <v>1111</v>
+        <v>1110</v>
       </c>
       <c r="PB1" s="21" t="s">
-        <v>1113</v>
+        <v>1112</v>
       </c>
       <c r="PC1" s="21" t="s">
-        <v>1115</v>
+        <v>1114</v>
       </c>
       <c r="PD1" s="21" t="s">
-        <v>1117</v>
+        <v>1116</v>
       </c>
       <c r="PE1" s="21" t="s">
-        <v>1119</v>
+        <v>1118</v>
       </c>
       <c r="PF1" s="21" t="s">
-        <v>1121</v>
+        <v>1120</v>
       </c>
       <c r="PG1" s="21" t="s">
-        <v>1123</v>
+        <v>1122</v>
       </c>
       <c r="PH1" s="21" t="s">
-        <v>1125</v>
+        <v>1124</v>
       </c>
       <c r="PI1" s="21" t="s">
-        <v>1127</v>
+        <v>1126</v>
       </c>
       <c r="PJ1" s="21" t="s">
-        <v>1129</v>
+        <v>1128</v>
       </c>
       <c r="PK1" s="21" t="s">
-        <v>1131</v>
+        <v>1130</v>
       </c>
       <c r="PL1" s="21" t="s">
-        <v>1133</v>
+        <v>1132</v>
       </c>
       <c r="PM1" s="21" t="s">
-        <v>1135</v>
+        <v>1134</v>
       </c>
       <c r="PN1" s="19" t="s">
-        <v>1137</v>
+        <v>1136</v>
       </c>
       <c r="PO1" s="19" t="s">
-        <v>1139</v>
+        <v>1138</v>
       </c>
       <c r="PP1" s="19" t="s">
-        <v>1141</v>
+        <v>1140</v>
       </c>
       <c r="PQ1" s="19" t="s">
-        <v>1143</v>
+        <v>1142</v>
       </c>
       <c r="PR1" s="19" t="s">
-        <v>1145</v>
+        <v>1144</v>
       </c>
       <c r="PS1" s="19" t="s">
-        <v>1147</v>
+        <v>1146</v>
       </c>
       <c r="PT1" s="19" t="s">
-        <v>1149</v>
+        <v>1148</v>
       </c>
       <c r="PU1" s="19" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="PV1" s="19" t="s">
-        <v>1153</v>
+        <v>1152</v>
       </c>
       <c r="PW1" s="19" t="s">
-        <v>1155</v>
+        <v>1154</v>
       </c>
       <c r="PX1" s="19" t="s">
-        <v>1157</v>
+        <v>1156</v>
       </c>
       <c r="PY1" s="19" t="s">
-        <v>1159</v>
+        <v>1158</v>
       </c>
       <c r="PZ1" s="19" t="s">
-        <v>1161</v>
+        <v>1160</v>
       </c>
       <c r="QA1" s="21" t="s">
-        <v>1163</v>
+        <v>1162</v>
       </c>
       <c r="QB1" s="21" t="s">
-        <v>1165</v>
+        <v>1164</v>
       </c>
       <c r="QC1" s="21" t="s">
-        <v>1167</v>
+        <v>1166</v>
       </c>
       <c r="QD1" s="21" t="s">
-        <v>1169</v>
+        <v>1168</v>
       </c>
       <c r="QE1" s="21" t="s">
-        <v>1171</v>
+        <v>1170</v>
       </c>
       <c r="QF1" s="21" t="s">
-        <v>1173</v>
+        <v>1172</v>
       </c>
       <c r="QG1" s="21" t="s">
-        <v>1175</v>
+        <v>1174</v>
       </c>
       <c r="QH1" s="21" t="s">
-        <v>1177</v>
+        <v>1176</v>
       </c>
       <c r="QI1" s="21" t="s">
-        <v>1179</v>
+        <v>1178</v>
       </c>
       <c r="QJ1" s="21" t="s">
-        <v>1181</v>
+        <v>1180</v>
       </c>
       <c r="QK1" s="21" t="s">
-        <v>1183</v>
+        <v>1182</v>
       </c>
       <c r="QL1" s="21" t="s">
-        <v>1185</v>
+        <v>1184</v>
       </c>
       <c r="QM1" s="21" t="s">
-        <v>1187</v>
+        <v>1186</v>
       </c>
       <c r="QN1" s="19" t="s">
-        <v>1189</v>
+        <v>1188</v>
       </c>
       <c r="QO1" s="19" t="s">
-        <v>1191</v>
+        <v>1190</v>
       </c>
       <c r="QP1" s="19" t="s">
-        <v>1193</v>
+        <v>1192</v>
       </c>
       <c r="QQ1" s="19" t="s">
-        <v>1195</v>
+        <v>1194</v>
       </c>
       <c r="QR1" s="19" t="s">
-        <v>1197</v>
+        <v>1196</v>
       </c>
       <c r="QS1" s="19" t="s">
-        <v>1199</v>
+        <v>1198</v>
       </c>
       <c r="QT1" s="19" t="s">
-        <v>1201</v>
+        <v>1200</v>
       </c>
       <c r="QU1" s="19" t="s">
-        <v>1203</v>
+        <v>1202</v>
       </c>
       <c r="QV1" s="19" t="s">
-        <v>1205</v>
+        <v>1204</v>
       </c>
       <c r="QW1" s="19" t="s">
-        <v>1207</v>
+        <v>1206</v>
       </c>
       <c r="QX1" s="19" t="s">
-        <v>1209</v>
+        <v>1208</v>
       </c>
       <c r="QY1" s="19" t="s">
-        <v>1211</v>
+        <v>1210</v>
       </c>
       <c r="QZ1" s="19" t="s">
-        <v>1213</v>
+        <v>1212</v>
       </c>
       <c r="RA1" s="3" t="s">
-        <v>1215</v>
+        <v>1214</v>
       </c>
     </row>
     <row r="2">
@@ -6964,7 +6961,7 @@
         <v>85</v>
       </c>
       <c r="MM2" s="29" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="MN2" s="29" t="n">
         <v>76</v>
@@ -7003,7 +7000,7 @@
         <v>78</v>
       </c>
       <c r="MZ2" s="29" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="NA2" s="29" t="n">
         <v>67</v>
@@ -7165,7 +7162,7 @@
         <v>147.526020073567</v>
       </c>
       <c r="PB2" s="25" t="n">
-        <v>1.73908625064187</v>
+        <v>0</v>
       </c>
       <c r="PC2" s="25" t="n">
         <v>117.411682117158</v>
@@ -7204,7 +7201,7 @@
         <v>30.261877629349</v>
       </c>
       <c r="PO2" s="25" t="n">
-        <v>7.62900682444057</v>
+        <v>7.81492351857363</v>
       </c>
       <c r="PP2" s="25" t="n">
         <v>102.341562793256</v>
@@ -7243,7 +7240,7 @@
         <v>123.623333748108</v>
       </c>
       <c r="QB2" s="25" t="n">
-        <v>1.45910485025071</v>
+        <v>0</v>
       </c>
       <c r="QC2" s="25" t="n">
         <v>97.5633727537407</v>
@@ -7282,7 +7279,7 @@
         <v>20.1659993085997</v>
       </c>
       <c r="QO2" s="25" t="n">
-        <v>5.13716694653457</v>
+        <v>5.25275661180307</v>
       </c>
       <c r="QP2" s="25" t="n">
         <v>67.4866656619721</v>
@@ -8337,7 +8334,7 @@
         <v>2</v>
       </c>
       <c r="MM3" s="29" t="n">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="MN3" s="29" t="n">
         <v>20</v>
@@ -8376,7 +8373,7 @@
         <v>2</v>
       </c>
       <c r="MZ3" s="29" t="n">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="NA3" s="29" t="n">
         <v>25</v>
@@ -8415,7 +8412,7 @@
         <v>31</v>
       </c>
       <c r="NM3" s="29" t="n">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="NN3" s="29" t="n">
         <v>52</v>
@@ -8454,7 +8451,7 @@
         <v>34</v>
       </c>
       <c r="NZ3" s="29" t="n">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="OA3" s="29" t="n">
         <v>58</v>
@@ -8538,10 +8535,10 @@
         <v>1.02026861584964</v>
       </c>
       <c r="PB3" s="25" t="n">
-        <v>8.67228323472191</v>
+        <v>1.53040292377445</v>
       </c>
       <c r="PC3" s="25" t="n">
-        <v>13.1908713550648</v>
+        <v>13.1908713550649</v>
       </c>
       <c r="PD3" s="25" t="n">
         <v>1.53040292377445</v>
@@ -8562,7 +8559,7 @@
         <v>0</v>
       </c>
       <c r="PJ3" s="25" t="n">
-        <v>0.387310138562227</v>
+        <v>0.387310138562228</v>
       </c>
       <c r="PK3" s="25" t="n">
         <v>33.69486095776</v>
@@ -8571,13 +8568,13 @@
         <v>4.66382942230378</v>
       </c>
       <c r="PM3" s="25" t="n">
-        <v>39.7904760181358</v>
+        <v>39.9115104364365</v>
       </c>
       <c r="PN3" s="25" t="n">
         <v>29.3478476488843</v>
       </c>
       <c r="PO3" s="25" t="n">
-        <v>20.8275047830792</v>
+        <v>9.46704762867236</v>
       </c>
       <c r="PP3" s="25" t="n">
         <v>55.7276054566087</v>
@@ -8616,7 +8613,7 @@
         <v>2.56516565088795</v>
       </c>
       <c r="QB3" s="25" t="n">
-        <v>21.8039080325476</v>
+        <v>3.84774847633193</v>
       </c>
       <c r="QC3" s="25" t="n">
         <v>33.1607334747035</v>
@@ -8649,13 +8646,13 @@
         <v>11.7296654158357</v>
       </c>
       <c r="QM3" s="25" t="n">
-        <v>100.04146038463</v>
+        <v>100.352160362697</v>
       </c>
       <c r="QN3" s="25" t="n">
         <v>40.9150689864568</v>
       </c>
       <c r="QO3" s="25" t="n">
-        <v>29.0365005710339</v>
+        <v>13.1984093504699</v>
       </c>
       <c r="QP3" s="25" t="n">
         <v>77.6720353423386</v>
@@ -9718,7 +9715,7 @@
         <v>58</v>
       </c>
       <c r="MM4" s="29" t="n">
-        <v>66</v>
+        <v>73</v>
       </c>
       <c r="MN4" s="29" t="n">
         <v>79</v>
@@ -9757,7 +9754,7 @@
         <v>43</v>
       </c>
       <c r="MZ4" s="29" t="n">
-        <v>52</v>
+        <v>64</v>
       </c>
       <c r="NA4" s="29" t="n">
         <v>78</v>
@@ -9796,7 +9793,7 @@
         <v>72</v>
       </c>
       <c r="NM4" s="29" t="n">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="NN4" s="29" t="n">
         <v>74</v>
@@ -9835,7 +9832,7 @@
         <v>72</v>
       </c>
       <c r="NZ4" s="29" t="n">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="OA4" s="29" t="n">
         <v>76</v>
@@ -9868,7 +9865,7 @@
         <v>71</v>
       </c>
       <c r="OK4" s="29" t="n">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="OL4" s="22" t="n">
         <v>121</v>
@@ -9919,7 +9916,7 @@
         <v>61.9334383542575</v>
       </c>
       <c r="PB4" s="25" t="n">
-        <v>73.5831486297469</v>
+        <v>92.0170480357706</v>
       </c>
       <c r="PC4" s="25" t="n">
         <v>130.362913541297</v>
@@ -9952,13 +9949,13 @@
         <v>116.507485254061</v>
       </c>
       <c r="PM4" s="25" t="n">
-        <v>122.665964781077</v>
+        <v>122.681265493211</v>
       </c>
       <c r="PN4" s="25" t="n">
         <v>99.5955004053087</v>
       </c>
       <c r="PO4" s="25" t="n">
-        <v>52.2258272098887</v>
+        <v>64.9079205832168</v>
       </c>
       <c r="PP4" s="25" t="n">
         <v>116.992026021754</v>
@@ -9991,13 +9988,13 @@
         <v>99.498695445133</v>
       </c>
       <c r="PZ4" s="25" t="n">
-        <v>70.1255436840799</v>
+        <v>70.3255780609697</v>
       </c>
       <c r="QA4" s="25" t="n">
         <v>59.8066990248148</v>
       </c>
       <c r="QB4" s="25" t="n">
-        <v>70.9223064278375</v>
+        <v>88.7164059904571</v>
       </c>
       <c r="QC4" s="25" t="n">
         <v>125.729072309413</v>
@@ -10030,13 +10027,13 @@
         <v>112.464386000112</v>
       </c>
       <c r="QM4" s="25" t="n">
-        <v>118.326861908482</v>
+        <v>118.342435978211</v>
       </c>
       <c r="QN4" s="25" t="n">
         <v>100.535119459682</v>
       </c>
       <c r="QO4" s="25" t="n">
-        <v>52.5458095107339</v>
+        <v>65.3126791318764</v>
       </c>
       <c r="QP4" s="25" t="n">
         <v>118.02557250542</v>
@@ -10069,7 +10066,7 @@
         <v>100.504794101966</v>
       </c>
       <c r="QZ4" s="25" t="n">
-        <v>70.7484835206945</v>
+        <v>70.9656682960832</v>
       </c>
       <c r="RA4" s="23" t="n">
         <v>3.14159265358979</v>
@@ -11099,7 +11096,7 @@
         <v>10</v>
       </c>
       <c r="MM5" s="29" t="n">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="MN5" s="29" t="n">
         <v>29</v>
@@ -11138,7 +11135,7 @@
         <v>12</v>
       </c>
       <c r="MZ5" s="29" t="n">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="NA5" s="29" t="n">
         <v>41</v>
@@ -11177,7 +11174,7 @@
         <v>40</v>
       </c>
       <c r="NM5" s="29" t="n">
-        <v>43</v>
+        <v>52</v>
       </c>
       <c r="NN5" s="29" t="n">
         <v>34</v>
@@ -11216,7 +11213,7 @@
         <v>55</v>
       </c>
       <c r="NZ5" s="29" t="n">
-        <v>63</v>
+        <v>74</v>
       </c>
       <c r="OA5" s="29" t="n">
         <v>42</v>
@@ -11300,7 +11297,7 @@
         <v>6.18106233110586</v>
       </c>
       <c r="PB5" s="25" t="n">
-        <v>13.670686056997</v>
+        <v>15.2311958777375</v>
       </c>
       <c r="PC5" s="25" t="n">
         <v>20.7134557649812</v>
@@ -11315,7 +11312,7 @@
         <v>17.5273118887225</v>
       </c>
       <c r="PG5" s="25" t="n">
-        <v>23.4354008386388</v>
+        <v>23.4354008386389</v>
       </c>
       <c r="PH5" s="25" t="n">
         <v>0</v>
@@ -11339,7 +11336,7 @@
         <v>26.4793069071469</v>
       </c>
       <c r="PO5" s="25" t="n">
-        <v>34.7549654650404</v>
+        <v>43.2873588710858</v>
       </c>
       <c r="PP5" s="25" t="n">
         <v>20.9065803078131</v>
@@ -11378,7 +11375,7 @@
         <v>15.5800649015706</v>
       </c>
       <c r="QB5" s="25" t="n">
-        <v>34.7504070270963</v>
+        <v>38.7170574772691</v>
       </c>
       <c r="QC5" s="25" t="n">
         <v>53.4826080364208</v>
@@ -11417,7 +11414,7 @@
         <v>53.6364288591919</v>
       </c>
       <c r="QO5" s="25" t="n">
-        <v>71.2110570067934</v>
+        <v>88.2582589647063</v>
       </c>
       <c r="QP5" s="25" t="n">
         <v>43.7864105760659</v>
@@ -12472,7 +12469,7 @@
         <v>30</v>
       </c>
       <c r="MM6" s="29" t="n">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="MN6" s="29" t="n">
         <v>14</v>
@@ -12496,7 +12493,7 @@
         <v>0</v>
       </c>
       <c r="MU6" s="29" t="n">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="MV6" s="29" t="n">
         <v>59</v>
@@ -12511,7 +12508,7 @@
         <v>24</v>
       </c>
       <c r="MZ6" s="29" t="n">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="NA6" s="29" t="n">
         <v>8</v>
@@ -12535,7 +12532,7 @@
         <v>0</v>
       </c>
       <c r="NH6" s="29" t="n">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="NI6" s="29" t="n">
         <v>57</v>
@@ -12550,7 +12547,7 @@
         <v>30</v>
       </c>
       <c r="NM6" s="29" t="n">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="NN6" s="29" t="n">
         <v>5</v>
@@ -12574,7 +12571,7 @@
         <v>0</v>
       </c>
       <c r="NU6" s="29" t="n">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="NV6" s="29" t="n">
         <v>42</v>
@@ -12589,7 +12586,7 @@
         <v>28</v>
       </c>
       <c r="NZ6" s="29" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="OA6" s="29" t="n">
         <v>2</v>
@@ -12613,7 +12610,7 @@
         <v>0</v>
       </c>
       <c r="OH6" s="29" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="OI6" s="29" t="n">
         <v>40</v>
@@ -12673,7 +12670,7 @@
         <v>23.0409848173639</v>
       </c>
       <c r="PB6" s="25" t="n">
-        <v>39.6968154045372</v>
+        <v>38.3412972176782</v>
       </c>
       <c r="PC6" s="25" t="n">
         <v>8.60817609314943</v>
@@ -12682,7 +12679,7 @@
         <v>23.7860525053971</v>
       </c>
       <c r="PE6" s="25" t="n">
-        <v>10.0482494797839</v>
+        <v>10.048249479784</v>
       </c>
       <c r="PF6" s="25" t="n">
         <v>29.2050913014527</v>
@@ -12697,7 +12694,7 @@
         <v>0</v>
       </c>
       <c r="PJ6" s="25" t="n">
-        <v>6.19607543280081</v>
+        <v>14.4085372098873</v>
       </c>
       <c r="PK6" s="25" t="n">
         <v>58.2397351865338</v>
@@ -12712,7 +12709,7 @@
         <v>19.9775292553547</v>
       </c>
       <c r="PO6" s="25" t="n">
-        <v>0.592906303592776</v>
+        <v>3.51759786028714</v>
       </c>
       <c r="PP6" s="25" t="n">
         <v>1.78813830308018</v>
@@ -12736,7 +12733,7 @@
         <v>0</v>
       </c>
       <c r="PW6" s="25" t="n">
-        <v>0</v>
+        <v>3.9915237843948</v>
       </c>
       <c r="PX6" s="25" t="n">
         <v>30.4151655251991</v>
@@ -12745,13 +12742,13 @@
         <v>14.2500183574574</v>
       </c>
       <c r="PZ6" s="25" t="n">
-        <v>38.4699021294061</v>
+        <v>38.4739015817123</v>
       </c>
       <c r="QA6" s="25" t="n">
         <v>31.3458835047324</v>
       </c>
       <c r="QB6" s="25" t="n">
-        <v>54.0675406722285</v>
+        <v>52.279349558934</v>
       </c>
       <c r="QC6" s="25" t="n">
         <v>11.9004922248481</v>
@@ -12775,7 +12772,7 @@
         <v>0</v>
       </c>
       <c r="QJ6" s="25" t="n">
-        <v>10.3630513735587</v>
+        <v>20.6658053899061</v>
       </c>
       <c r="QK6" s="25" t="n">
         <v>79.2183890714953</v>
@@ -12790,7 +12787,7 @@
         <v>24.9374188259632</v>
       </c>
       <c r="QO6" s="25" t="n">
-        <v>0.692512809959195</v>
+        <v>4.37388171593421</v>
       </c>
       <c r="QP6" s="25" t="n">
         <v>2.28970040109511</v>
@@ -12814,7 +12811,7 @@
         <v>0</v>
       </c>
       <c r="QW6" s="25" t="n">
-        <v>0</v>
+        <v>5.26382328212159</v>
       </c>
       <c r="QX6" s="25" t="n">
         <v>37.4967271481087</v>
@@ -12823,7 +12820,7 @@
         <v>17.6579693326827</v>
       </c>
       <c r="QZ6" s="25" t="n">
-        <v>51.6031654117135</v>
+        <v>51.6122746427208</v>
       </c>
       <c r="RA6" s="23" t="n">
         <v>3.14159265358979</v>
@@ -13931,7 +13928,7 @@
         <v>30</v>
       </c>
       <c r="NM7" s="29" t="n">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="NN7" s="29" t="n">
         <v>52</v>
@@ -13970,7 +13967,7 @@
         <v>17</v>
       </c>
       <c r="NZ7" s="29" t="n">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="OA7" s="29" t="n">
         <v>40</v>
@@ -14054,7 +14051,7 @@
         <v>2.57799526706975</v>
       </c>
       <c r="PB7" s="25" t="n">
-        <v>21.5561089571271</v>
+        <v>21.4832938922479</v>
       </c>
       <c r="PC7" s="25" t="n">
         <v>37.6638998618618</v>
@@ -14093,7 +14090,7 @@
         <v>18.5456956459861</v>
       </c>
       <c r="PO7" s="25" t="n">
-        <v>45.0342108257509</v>
+        <v>51.7381606363633</v>
       </c>
       <c r="PP7" s="25" t="n">
         <v>42.0493123414748</v>
@@ -14132,7 +14129,7 @@
         <v>3.44053764346531</v>
       </c>
       <c r="QB7" s="25" t="n">
-        <v>28.7381910170622</v>
+        <v>28.6711470288776</v>
       </c>
       <c r="QC7" s="25" t="n">
         <v>45.0936442405563</v>
@@ -14171,7 +14168,7 @@
         <v>20.2600396385842</v>
       </c>
       <c r="QO7" s="25" t="n">
-        <v>49.2575284291922</v>
+        <v>56.6697766152045</v>
       </c>
       <c r="QP7" s="25" t="n">
         <v>41.0611492852566</v>
@@ -15234,7 +15231,7 @@
         <v>91</v>
       </c>
       <c r="MM8" s="29" t="n">
-        <v>78</v>
+        <v>88</v>
       </c>
       <c r="MN8" s="29" t="n">
         <v>70</v>
@@ -15273,7 +15270,7 @@
         <v>86</v>
       </c>
       <c r="MZ8" s="29" t="n">
-        <v>63</v>
+        <v>82</v>
       </c>
       <c r="NA8" s="29" t="n">
         <v>57</v>
@@ -15312,7 +15309,7 @@
         <v>67</v>
       </c>
       <c r="NM8" s="29" t="n">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="NN8" s="29" t="n">
         <v>39</v>
@@ -15351,7 +15348,7 @@
         <v>60</v>
       </c>
       <c r="NZ8" s="29" t="n">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="OA8" s="29" t="n">
         <v>33</v>
@@ -15435,7 +15432,7 @@
         <v>183.713982493363</v>
       </c>
       <c r="PB8" s="25" t="n">
-        <v>107.969029034477</v>
+        <v>160.11928862861</v>
       </c>
       <c r="PC8" s="25" t="n">
         <v>96.1876930283443</v>
@@ -15474,7 +15471,7 @@
         <v>121.916671389955</v>
       </c>
       <c r="PO8" s="25" t="n">
-        <v>69.164659040453</v>
+        <v>71.6344433323325</v>
       </c>
       <c r="PP8" s="25" t="n">
         <v>58.4536247063949</v>
@@ -15513,7 +15510,7 @@
         <v>149.792008783348</v>
       </c>
       <c r="QB8" s="25" t="n">
-        <v>88.0883946524944</v>
+        <v>130.53747044082</v>
       </c>
       <c r="QC8" s="25" t="n">
         <v>78.042392169296</v>
@@ -15552,7 +15549,7 @@
         <v>80.0075160437923</v>
       </c>
       <c r="QO8" s="25" t="n">
-        <v>45.3850939945673</v>
+        <v>47.0387666280044</v>
       </c>
       <c r="QP8" s="25" t="n">
         <v>37.9858914292202</v>
@@ -16615,7 +16612,7 @@
         <v>28</v>
       </c>
       <c r="MM9" s="29" t="n">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="MN9" s="29" t="n">
         <v>34</v>
@@ -16654,7 +16651,7 @@
         <v>21</v>
       </c>
       <c r="MZ9" s="29" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="NA9" s="29" t="n">
         <v>28</v>
@@ -16693,7 +16690,7 @@
         <v>33</v>
       </c>
       <c r="NM9" s="29" t="n">
-        <v>35</v>
+        <v>16</v>
       </c>
       <c r="NN9" s="29" t="n">
         <v>50</v>
@@ -16732,7 +16729,7 @@
         <v>18</v>
       </c>
       <c r="NZ9" s="29" t="n">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="OA9" s="29" t="n">
         <v>29</v>
@@ -16816,16 +16813,16 @@
         <v>21.0934471762864</v>
       </c>
       <c r="PB9" s="25" t="n">
-        <v>8.27365312211825</v>
+        <v>3.87543581374187</v>
       </c>
       <c r="PC9" s="25" t="n">
         <v>25.9808235385794</v>
       </c>
       <c r="PD9" s="25" t="n">
-        <v>27.5777353514449</v>
+        <v>27.577735351445</v>
       </c>
       <c r="PE9" s="25" t="n">
-        <v>36.0995966939888</v>
+        <v>36.0995966939889</v>
       </c>
       <c r="PF9" s="25" t="n">
         <v>31.6729652349235</v>
@@ -16855,7 +16852,7 @@
         <v>37.5073196608144</v>
       </c>
       <c r="PO9" s="25" t="n">
-        <v>38.6350906668497</v>
+        <v>17.5255175520074</v>
       </c>
       <c r="PP9" s="25" t="n">
         <v>56.4852300203805</v>
@@ -16894,7 +16891,7 @@
         <v>27.8119851657603</v>
       </c>
       <c r="QB9" s="25" t="n">
-        <v>10.8947662597267</v>
+        <v>5.13898531536718</v>
       </c>
       <c r="QC9" s="25" t="n">
         <v>36.2860097736636</v>
@@ -16933,7 +16930,7 @@
         <v>24.7792011444907</v>
       </c>
       <c r="QO9" s="25" t="n">
-        <v>25.1104498138086</v>
+        <v>11.4833476487372</v>
       </c>
       <c r="QP9" s="25" t="n">
         <v>37.7679634019357</v>
@@ -17996,7 +17993,7 @@
         <v>49</v>
       </c>
       <c r="MM10" s="29" t="n">
-        <v>45</v>
+        <v>55</v>
       </c>
       <c r="MN10" s="29" t="n">
         <v>53</v>
@@ -18011,7 +18008,7 @@
         <v>58</v>
       </c>
       <c r="MR10" s="29" t="n">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="MS10" s="29" t="n">
         <v>66</v>
@@ -18035,7 +18032,7 @@
         <v>46</v>
       </c>
       <c r="MZ10" s="29" t="n">
-        <v>40</v>
+        <v>54</v>
       </c>
       <c r="NA10" s="29" t="n">
         <v>51</v>
@@ -18074,7 +18071,7 @@
         <v>71</v>
       </c>
       <c r="NM10" s="29" t="n">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="NN10" s="29" t="n">
         <v>67</v>
@@ -18113,7 +18110,7 @@
         <v>61</v>
       </c>
       <c r="NZ10" s="29" t="n">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="OA10" s="29" t="n">
         <v>54</v>
@@ -18194,10 +18191,10 @@
         <v>0.843764143081404</v>
       </c>
       <c r="PA10" s="25" t="n">
-        <v>47.1479182343852</v>
+        <v>47.1479182343853</v>
       </c>
       <c r="PB10" s="25" t="n">
-        <v>39.4522146565577</v>
+        <v>53.6611490887787</v>
       </c>
       <c r="PC10" s="25" t="n">
         <v>55.0335196211626</v>
@@ -18209,13 +18206,13 @@
         <v>25.2133589307869</v>
       </c>
       <c r="PF10" s="25" t="n">
-        <v>64.7822363720812</v>
+        <v>64.7822363720813</v>
       </c>
       <c r="PG10" s="25" t="n">
-        <v>16.4827165782504</v>
+        <v>17.7422557329089</v>
       </c>
       <c r="PH10" s="25" t="n">
-        <v>50.6139912575259</v>
+        <v>50.613991257526</v>
       </c>
       <c r="PI10" s="25" t="n">
         <v>21.2077916366126</v>
@@ -18236,7 +18233,7 @@
         <v>69.0723068317792</v>
       </c>
       <c r="PO10" s="25" t="n">
-        <v>48.6275430037101</v>
+        <v>44.8413229406556</v>
       </c>
       <c r="PP10" s="25" t="n">
         <v>66.9741704985442</v>
@@ -18275,7 +18272,7 @@
         <v>64.926617169684</v>
       </c>
       <c r="QB10" s="25" t="n">
-        <v>54.7405821338403</v>
+        <v>73.9210013386079</v>
       </c>
       <c r="QC10" s="25" t="n">
         <v>68.8855863379048</v>
@@ -18290,7 +18287,7 @@
         <v>86.7990563292608</v>
       </c>
       <c r="QG10" s="25" t="n">
-        <v>10.8284537243925</v>
+        <v>12.9397720475342</v>
       </c>
       <c r="QH10" s="25" t="n">
         <v>70.9644761564981</v>
@@ -18314,7 +18311,7 @@
         <v>67.6349438776366</v>
       </c>
       <c r="QO10" s="25" t="n">
-        <v>47.097680605551</v>
+        <v>42.889994072906</v>
       </c>
       <c r="QP10" s="25" t="n">
         <v>59.0302599490193</v>
@@ -19377,7 +19374,7 @@
         <v>57</v>
       </c>
       <c r="MM11" s="29" t="n">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="MN11" s="29" t="n">
         <v>76</v>
@@ -19416,7 +19413,7 @@
         <v>37</v>
       </c>
       <c r="MZ11" s="29" t="n">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="NA11" s="29" t="n">
         <v>67</v>
@@ -19455,7 +19452,7 @@
         <v>71</v>
       </c>
       <c r="NM11" s="29" t="n">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="NN11" s="29" t="n">
         <v>71</v>
@@ -19494,7 +19491,7 @@
         <v>64</v>
       </c>
       <c r="NZ11" s="29" t="n">
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="OA11" s="29" t="n">
         <v>65</v>
@@ -19578,7 +19575,7 @@
         <v>61.0020809233515</v>
       </c>
       <c r="PB11" s="25" t="n">
-        <v>71.0396690997364</v>
+        <v>75.8067266377541</v>
       </c>
       <c r="PC11" s="25" t="n">
         <v>117.483965121849</v>
@@ -19617,7 +19614,7 @@
         <v>101.543406542951</v>
       </c>
       <c r="PO11" s="25" t="n">
-        <v>47.6740729628828</v>
+        <v>63.417268256965</v>
       </c>
       <c r="PP11" s="25" t="n">
         <v>104.662130239603</v>
@@ -19656,7 +19653,7 @@
         <v>50.5022609094815</v>
       </c>
       <c r="QB11" s="25" t="n">
-        <v>58.9329405461773</v>
+        <v>62.7649371293407</v>
       </c>
       <c r="QC11" s="25" t="n">
         <v>97.2135957776166</v>
@@ -19695,7 +19692,7 @@
         <v>72.4675006882293</v>
       </c>
       <c r="QO11" s="25" t="n">
-        <v>34.145699505396</v>
+        <v>45.0975937644931</v>
       </c>
       <c r="QP11" s="25" t="n">
         <v>74.9016792834264</v>
@@ -21106,322 +21103,322 @@
         <v>1045</v>
       </c>
       <c r="MZ1" s="19" t="s">
+        <v>1046</v>
+      </c>
+      <c r="NA1" s="19" t="s">
         <v>1047</v>
       </c>
-      <c r="NA1" s="19" t="s">
+      <c r="NB1" s="19" t="s">
         <v>1048</v>
       </c>
-      <c r="NB1" s="19" t="s">
+      <c r="NC1" s="19" t="s">
         <v>1049</v>
       </c>
-      <c r="NC1" s="19" t="s">
+      <c r="ND1" s="19" t="s">
         <v>1050</v>
       </c>
-      <c r="ND1" s="19" t="s">
+      <c r="NE1" s="19" t="s">
         <v>1051</v>
       </c>
-      <c r="NE1" s="19" t="s">
+      <c r="NF1" s="19" t="s">
         <v>1052</v>
       </c>
-      <c r="NF1" s="19" t="s">
-        <v>1053</v>
-      </c>
       <c r="NG1" s="19" t="s">
-        <v>1055</v>
+        <v>1054</v>
       </c>
       <c r="NH1" s="19" t="s">
-        <v>1057</v>
+        <v>1056</v>
       </c>
       <c r="NI1" s="19" t="s">
+        <v>1058</v>
+      </c>
+      <c r="NJ1" s="19" t="s">
         <v>1059</v>
       </c>
-      <c r="NJ1" s="19" t="s">
+      <c r="NK1" s="19" t="s">
         <v>1060</v>
       </c>
-      <c r="NK1" s="19" t="s">
+      <c r="NL1" s="20" t="s">
         <v>1061</v>
       </c>
-      <c r="NL1" s="20" t="s">
+      <c r="NM1" s="20" t="s">
         <v>1062</v>
       </c>
-      <c r="NM1" s="20" t="s">
+      <c r="NN1" s="20" t="s">
         <v>1063</v>
       </c>
-      <c r="NN1" s="20" t="s">
+      <c r="NO1" s="20" t="s">
         <v>1064</v>
       </c>
-      <c r="NO1" s="20" t="s">
+      <c r="NP1" s="20" t="s">
         <v>1065</v>
       </c>
-      <c r="NP1" s="20" t="s">
+      <c r="NQ1" s="20" t="s">
         <v>1066</v>
       </c>
-      <c r="NQ1" s="20" t="s">
+      <c r="NR1" s="20" t="s">
         <v>1067</v>
       </c>
-      <c r="NR1" s="20" t="s">
+      <c r="NS1" s="20" t="s">
         <v>1068</v>
       </c>
-      <c r="NS1" s="20" t="s">
+      <c r="NT1" s="20" t="s">
         <v>1069</v>
       </c>
-      <c r="NT1" s="20" t="s">
+      <c r="NU1" s="20" t="s">
         <v>1070</v>
       </c>
-      <c r="NU1" s="20" t="s">
+      <c r="NV1" s="20" t="s">
         <v>1071</v>
       </c>
-      <c r="NV1" s="20" t="s">
+      <c r="NW1" s="20" t="s">
         <v>1072</v>
       </c>
-      <c r="NW1" s="20" t="s">
+      <c r="NX1" s="20" t="s">
         <v>1073</v>
       </c>
-      <c r="NX1" s="20" t="s">
+      <c r="NY1" s="20" t="s">
         <v>1074</v>
       </c>
-      <c r="NY1" s="20" t="s">
+      <c r="NZ1" s="20" t="s">
         <v>1075</v>
       </c>
-      <c r="NZ1" s="20" t="s">
+      <c r="OA1" s="20" t="s">
         <v>1076</v>
       </c>
-      <c r="OA1" s="20" t="s">
+      <c r="OB1" s="20" t="s">
         <v>1077</v>
       </c>
-      <c r="OB1" s="20" t="s">
+      <c r="OC1" s="20" t="s">
         <v>1078</v>
       </c>
-      <c r="OC1" s="20" t="s">
+      <c r="OD1" s="20" t="s">
         <v>1079</v>
       </c>
-      <c r="OD1" s="20" t="s">
+      <c r="OE1" s="20" t="s">
         <v>1080</v>
       </c>
-      <c r="OE1" s="20" t="s">
+      <c r="OF1" s="20" t="s">
         <v>1081</v>
       </c>
-      <c r="OF1" s="20" t="s">
-        <v>1082</v>
-      </c>
       <c r="OG1" s="20" t="s">
+        <v>1083</v>
+      </c>
+      <c r="OH1" s="20" t="s">
         <v>1084</v>
       </c>
-      <c r="OH1" s="20" t="s">
-        <v>1085</v>
-      </c>
       <c r="OI1" s="20" t="s">
+        <v>1086</v>
+      </c>
+      <c r="OJ1" s="20" t="s">
         <v>1087</v>
       </c>
-      <c r="OJ1" s="20" t="s">
+      <c r="OK1" s="20" t="s">
         <v>1088</v>
       </c>
-      <c r="OK1" s="20" t="s">
-        <v>1089</v>
-      </c>
       <c r="OL1" s="10" t="s">
-        <v>1091</v>
+        <v>1090</v>
       </c>
       <c r="OM1" s="10" t="s">
+        <v>1092</v>
+      </c>
+      <c r="ON1" s="10" t="s">
         <v>1093</v>
       </c>
-      <c r="ON1" s="10" t="s">
+      <c r="OO1" s="9" t="s">
         <v>1094</v>
       </c>
-      <c r="OO1" s="9" t="s">
-        <v>1095</v>
-      </c>
       <c r="OP1" s="9" t="s">
-        <v>1097</v>
+        <v>1096</v>
       </c>
       <c r="OQ1" s="3" t="s">
-        <v>1099</v>
+        <v>1098</v>
       </c>
       <c r="OR1" s="3" t="s">
+        <v>1100</v>
+      </c>
+      <c r="OS1" s="3" t="s">
         <v>1101</v>
       </c>
-      <c r="OS1" s="3" t="s">
+      <c r="OT1" s="9" t="s">
         <v>1102</v>
       </c>
-      <c r="OT1" s="9" t="s">
+      <c r="OU1" s="9" t="s">
         <v>1103</v>
       </c>
-      <c r="OU1" s="9" t="s">
+      <c r="OV1" s="9" t="s">
         <v>1104</v>
       </c>
-      <c r="OV1" s="9" t="s">
+      <c r="OW1" s="9" t="s">
         <v>1105</v>
       </c>
-      <c r="OW1" s="9" t="s">
+      <c r="OX1" s="9" t="s">
         <v>1106</v>
       </c>
-      <c r="OX1" s="9" t="s">
+      <c r="OY1" s="9" t="s">
         <v>1107</v>
       </c>
-      <c r="OY1" s="9" t="s">
+      <c r="OZ1" s="9" t="s">
         <v>1108</v>
       </c>
-      <c r="OZ1" s="9" t="s">
-        <v>1109</v>
-      </c>
       <c r="PA1" s="21" t="s">
-        <v>1111</v>
+        <v>1110</v>
       </c>
       <c r="PB1" s="21" t="s">
-        <v>1113</v>
+        <v>1112</v>
       </c>
       <c r="PC1" s="21" t="s">
-        <v>1115</v>
+        <v>1114</v>
       </c>
       <c r="PD1" s="21" t="s">
-        <v>1117</v>
+        <v>1116</v>
       </c>
       <c r="PE1" s="21" t="s">
-        <v>1119</v>
+        <v>1118</v>
       </c>
       <c r="PF1" s="21" t="s">
-        <v>1121</v>
+        <v>1120</v>
       </c>
       <c r="PG1" s="21" t="s">
-        <v>1123</v>
+        <v>1122</v>
       </c>
       <c r="PH1" s="21" t="s">
-        <v>1125</v>
+        <v>1124</v>
       </c>
       <c r="PI1" s="21" t="s">
-        <v>1127</v>
+        <v>1126</v>
       </c>
       <c r="PJ1" s="21" t="s">
-        <v>1129</v>
+        <v>1128</v>
       </c>
       <c r="PK1" s="21" t="s">
-        <v>1131</v>
+        <v>1130</v>
       </c>
       <c r="PL1" s="21" t="s">
-        <v>1133</v>
+        <v>1132</v>
       </c>
       <c r="PM1" s="21" t="s">
-        <v>1135</v>
+        <v>1134</v>
       </c>
       <c r="PN1" s="19" t="s">
-        <v>1137</v>
+        <v>1136</v>
       </c>
       <c r="PO1" s="19" t="s">
-        <v>1139</v>
+        <v>1138</v>
       </c>
       <c r="PP1" s="19" t="s">
-        <v>1141</v>
+        <v>1140</v>
       </c>
       <c r="PQ1" s="19" t="s">
-        <v>1143</v>
+        <v>1142</v>
       </c>
       <c r="PR1" s="19" t="s">
-        <v>1145</v>
+        <v>1144</v>
       </c>
       <c r="PS1" s="19" t="s">
-        <v>1147</v>
+        <v>1146</v>
       </c>
       <c r="PT1" s="19" t="s">
-        <v>1149</v>
+        <v>1148</v>
       </c>
       <c r="PU1" s="19" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="PV1" s="19" t="s">
-        <v>1153</v>
+        <v>1152</v>
       </c>
       <c r="PW1" s="19" t="s">
-        <v>1155</v>
+        <v>1154</v>
       </c>
       <c r="PX1" s="19" t="s">
-        <v>1157</v>
+        <v>1156</v>
       </c>
       <c r="PY1" s="19" t="s">
-        <v>1159</v>
+        <v>1158</v>
       </c>
       <c r="PZ1" s="19" t="s">
-        <v>1161</v>
+        <v>1160</v>
       </c>
       <c r="QA1" s="21" t="s">
-        <v>1163</v>
+        <v>1162</v>
       </c>
       <c r="QB1" s="21" t="s">
-        <v>1165</v>
+        <v>1164</v>
       </c>
       <c r="QC1" s="21" t="s">
-        <v>1167</v>
+        <v>1166</v>
       </c>
       <c r="QD1" s="21" t="s">
-        <v>1169</v>
+        <v>1168</v>
       </c>
       <c r="QE1" s="21" t="s">
-        <v>1171</v>
+        <v>1170</v>
       </c>
       <c r="QF1" s="21" t="s">
-        <v>1173</v>
+        <v>1172</v>
       </c>
       <c r="QG1" s="21" t="s">
-        <v>1175</v>
+        <v>1174</v>
       </c>
       <c r="QH1" s="21" t="s">
-        <v>1177</v>
+        <v>1176</v>
       </c>
       <c r="QI1" s="21" t="s">
-        <v>1179</v>
+        <v>1178</v>
       </c>
       <c r="QJ1" s="21" t="s">
-        <v>1181</v>
+        <v>1180</v>
       </c>
       <c r="QK1" s="21" t="s">
-        <v>1183</v>
+        <v>1182</v>
       </c>
       <c r="QL1" s="21" t="s">
-        <v>1185</v>
+        <v>1184</v>
       </c>
       <c r="QM1" s="21" t="s">
-        <v>1187</v>
+        <v>1186</v>
       </c>
       <c r="QN1" s="19" t="s">
-        <v>1189</v>
+        <v>1188</v>
       </c>
       <c r="QO1" s="19" t="s">
-        <v>1191</v>
+        <v>1190</v>
       </c>
       <c r="QP1" s="19" t="s">
-        <v>1193</v>
+        <v>1192</v>
       </c>
       <c r="QQ1" s="19" t="s">
-        <v>1195</v>
+        <v>1194</v>
       </c>
       <c r="QR1" s="19" t="s">
-        <v>1197</v>
+        <v>1196</v>
       </c>
       <c r="QS1" s="19" t="s">
-        <v>1199</v>
+        <v>1198</v>
       </c>
       <c r="QT1" s="19" t="s">
-        <v>1201</v>
+        <v>1200</v>
       </c>
       <c r="QU1" s="19" t="s">
-        <v>1203</v>
+        <v>1202</v>
       </c>
       <c r="QV1" s="19" t="s">
-        <v>1205</v>
+        <v>1204</v>
       </c>
       <c r="QW1" s="19" t="s">
-        <v>1207</v>
+        <v>1206</v>
       </c>
       <c r="QX1" s="19" t="s">
-        <v>1209</v>
+        <v>1208</v>
       </c>
       <c r="QY1" s="19" t="s">
-        <v>1211</v>
+        <v>1210</v>
       </c>
       <c r="QZ1" s="19" t="s">
-        <v>1213</v>
+        <v>1212</v>
       </c>
       <c r="RA1" s="3" t="s">
-        <v>1215</v>
+        <v>1214</v>
       </c>
     </row>
     <row r="2">
@@ -22436,7 +22433,7 @@
         <v>63</v>
       </c>
       <c r="MM2" s="29" t="n">
-        <v>62</v>
+        <v>69</v>
       </c>
       <c r="MN2" s="29" t="n">
         <v>76</v>
@@ -22475,7 +22472,7 @@
         <v>47</v>
       </c>
       <c r="MZ2" s="29" t="n">
-        <v>46</v>
+        <v>57</v>
       </c>
       <c r="NA2" s="29" t="n">
         <v>72</v>
@@ -22514,7 +22511,7 @@
         <v>65.9916718868485</v>
       </c>
       <c r="NM2" s="29" t="n">
-        <v>48.1651798960988</v>
+        <v>52.9351361407706</v>
       </c>
       <c r="NN2" s="29" t="n">
         <v>68.1843319187818</v>
@@ -22538,7 +22535,7 @@
         <v>58.4935831798678</v>
       </c>
       <c r="NU2" s="29" t="n">
-        <v>68.0993250658214</v>
+        <v>68.1637358289727</v>
       </c>
       <c r="NV2" s="29" t="n">
         <v>58.9182420625763</v>
@@ -22553,7 +22550,7 @@
         <v>63.6663550257398</v>
       </c>
       <c r="NZ2" s="29" t="n">
-        <v>38.4349863647282</v>
+        <v>44.9597728867684</v>
       </c>
       <c r="OA2" s="29" t="n">
         <v>67.030258528521</v>
@@ -22577,7 +22574,7 @@
         <v>50.8433719391288</v>
       </c>
       <c r="OH2" s="29" t="n">
-        <v>67.0110170170076</v>
+        <v>67.0468007743139</v>
       </c>
       <c r="OI2" s="29" t="n">
         <v>56.1140017049977</v>
@@ -22586,7 +22583,7 @@
         <v>63.0163547902429</v>
       </c>
       <c r="OK2" s="29" t="n">
-        <v>42.6417173377544</v>
+        <v>43.2909107607964</v>
       </c>
       <c r="OL2" s="22" t="n">
         <v>211</v>
@@ -22637,7 +22634,7 @@
         <v>72.6619597700568</v>
       </c>
       <c r="PB2" s="25" t="n">
-        <v>66.8545766278586</v>
+        <v>83.1416945170066</v>
       </c>
       <c r="PC2" s="25" t="n">
         <v>117.640621006597</v>
@@ -22652,7 +22649,7 @@
         <v>118.693098519419</v>
       </c>
       <c r="PG2" s="25" t="n">
-        <v>94.6674584422416</v>
+        <v>94.6922782888973</v>
       </c>
       <c r="PH2" s="25" t="n">
         <v>108.064546401517</v>
@@ -22661,7 +22658,7 @@
         <v>36.5023495513042</v>
       </c>
       <c r="PJ2" s="25" t="n">
-        <v>122.998695800964</v>
+        <v>123.057468677466</v>
       </c>
       <c r="PK2" s="25" t="n">
         <v>99.9937829973154</v>
@@ -22670,13 +22667,13 @@
         <v>105.869093064804</v>
       </c>
       <c r="PM2" s="25" t="n">
-        <v>80.2827525589517</v>
+        <v>80.2935890241642</v>
       </c>
       <c r="PN2" s="25" t="n">
         <v>91.9527509182466</v>
       </c>
       <c r="PO2" s="25" t="n">
-        <v>48.6357262376477</v>
+        <v>58.8572690001761</v>
       </c>
       <c r="PP2" s="25" t="n">
         <v>104.733423555764</v>
@@ -22700,7 +22697,7 @@
         <v>54.6269558563915</v>
       </c>
       <c r="PW2" s="25" t="n">
-        <v>106.014229317612</v>
+        <v>106.042794848972</v>
       </c>
       <c r="PX2" s="25" t="n">
         <v>83.8538521918065</v>
@@ -22709,13 +22706,13 @@
         <v>91.4786217624796</v>
       </c>
       <c r="PZ2" s="25" t="n">
-        <v>46.4304775726821</v>
+        <v>46.5603671912465</v>
       </c>
       <c r="QA2" s="25" t="n">
         <v>66.5518972827937</v>
       </c>
       <c r="QB2" s="25" t="n">
-        <v>62.9365352710808</v>
+        <v>78.033507483792</v>
       </c>
       <c r="QC2" s="25" t="n">
         <v>110.354042859017</v>
@@ -22730,7 +22727,7 @@
         <v>110.814812977949</v>
       </c>
       <c r="QG2" s="25" t="n">
-        <v>91.2517621384903</v>
+        <v>91.2933667180923</v>
       </c>
       <c r="QH2" s="25" t="n">
         <v>101.69882674781</v>
@@ -22739,7 +22736,7 @@
         <v>35.5090691453336</v>
       </c>
       <c r="QJ2" s="25" t="n">
-        <v>114.011764982258</v>
+        <v>114.085497135402</v>
       </c>
       <c r="QK2" s="25" t="n">
         <v>94.9010404844178</v>
@@ -22748,13 +22745,13 @@
         <v>99.4132247539213</v>
       </c>
       <c r="QM2" s="25" t="n">
-        <v>78.0770874130736</v>
+        <v>78.0895169147354</v>
       </c>
       <c r="QN2" s="25" t="n">
         <v>85.1457224445399</v>
       </c>
       <c r="QO2" s="25" t="n">
-        <v>45.3592755597441</v>
+        <v>55.1130700140601</v>
       </c>
       <c r="QP2" s="25" t="n">
         <v>97.4761401450092</v>
@@ -22778,7 +22775,7 @@
         <v>53.506016172586</v>
       </c>
       <c r="QW2" s="25" t="n">
-        <v>97.6551846876399</v>
+        <v>97.6928554913635</v>
       </c>
       <c r="QX2" s="25" t="n">
         <v>80.1989678532379</v>
@@ -22787,7 +22784,7 @@
         <v>84.6056979431081</v>
       </c>
       <c r="QZ2" s="25" t="n">
-        <v>47.1774346803506</v>
+        <v>47.3184947927219</v>
       </c>
       <c r="RA2" s="23" t="n">
         <v>31.4159265358979</v>
@@ -25689,7 +25686,7 @@
     </row>
     <row r="352">
       <c r="A352" t="s">
-        <v>812</v>
+        <v>714</v>
       </c>
       <c r="B352" t="s">
         <v>1030</v>
@@ -25793,10 +25790,10 @@
     </row>
     <row r="365">
       <c r="A365" t="s">
+        <v>797</v>
+      </c>
+      <c r="B365" t="s">
         <v>1046</v>
-      </c>
-      <c r="B365" t="s">
-        <v>1047</v>
       </c>
     </row>
     <row r="366">
@@ -25804,7 +25801,7 @@
         <v>717</v>
       </c>
       <c r="B366" t="s">
-        <v>1048</v>
+        <v>1047</v>
       </c>
     </row>
     <row r="367">
@@ -25812,7 +25809,7 @@
         <v>1035</v>
       </c>
       <c r="B367" t="s">
-        <v>1049</v>
+        <v>1048</v>
       </c>
     </row>
     <row r="368">
@@ -25820,7 +25817,7 @@
         <v>799</v>
       </c>
       <c r="B368" t="s">
-        <v>1050</v>
+        <v>1049</v>
       </c>
     </row>
     <row r="369">
@@ -25828,7 +25825,7 @@
         <v>816</v>
       </c>
       <c r="B369" t="s">
-        <v>1051</v>
+        <v>1050</v>
       </c>
     </row>
     <row r="370">
@@ -25836,7 +25833,7 @@
         <v>871</v>
       </c>
       <c r="B370" t="s">
-        <v>1052</v>
+        <v>1051</v>
       </c>
     </row>
     <row r="371">
@@ -25844,31 +25841,31 @@
         <v>816</v>
       </c>
       <c r="B371" t="s">
-        <v>1053</v>
+        <v>1052</v>
       </c>
     </row>
     <row r="372">
       <c r="A372" t="s">
+        <v>1053</v>
+      </c>
+      <c r="B372" t="s">
         <v>1054</v>
-      </c>
-      <c r="B372" t="s">
-        <v>1055</v>
       </c>
     </row>
     <row r="373">
       <c r="A373" t="s">
+        <v>1055</v>
+      </c>
+      <c r="B373" t="s">
         <v>1056</v>
-      </c>
-      <c r="B373" t="s">
-        <v>1057</v>
       </c>
     </row>
     <row r="374">
       <c r="A374" t="s">
+        <v>1057</v>
+      </c>
+      <c r="B374" t="s">
         <v>1058</v>
-      </c>
-      <c r="B374" t="s">
-        <v>1059</v>
       </c>
     </row>
     <row r="375">
@@ -25876,7 +25873,7 @@
         <v>754</v>
       </c>
       <c r="B375" t="s">
-        <v>1060</v>
+        <v>1059</v>
       </c>
     </row>
     <row r="376">
@@ -25884,7 +25881,7 @@
         <v>835</v>
       </c>
       <c r="B376" t="s">
-        <v>1061</v>
+        <v>1060</v>
       </c>
     </row>
     <row r="377">
@@ -25892,15 +25889,15 @@
         <v>808</v>
       </c>
       <c r="B377" t="s">
-        <v>1062</v>
+        <v>1061</v>
       </c>
     </row>
     <row r="378">
       <c r="A378" t="s">
-        <v>641</v>
+        <v>621</v>
       </c>
       <c r="B378" t="s">
-        <v>1063</v>
+        <v>1062</v>
       </c>
     </row>
     <row r="379">
@@ -25908,7 +25905,7 @@
         <v>746</v>
       </c>
       <c r="B379" t="s">
-        <v>1064</v>
+        <v>1063</v>
       </c>
     </row>
     <row r="380">
@@ -25916,7 +25913,7 @@
         <v>750</v>
       </c>
       <c r="B380" t="s">
-        <v>1065</v>
+        <v>1064</v>
       </c>
     </row>
     <row r="381">
@@ -25924,7 +25921,7 @@
         <v>808</v>
       </c>
       <c r="B381" t="s">
-        <v>1066</v>
+        <v>1065</v>
       </c>
     </row>
     <row r="382">
@@ -25932,7 +25929,7 @@
         <v>746</v>
       </c>
       <c r="B382" t="s">
-        <v>1067</v>
+        <v>1066</v>
       </c>
     </row>
     <row r="383">
@@ -25940,15 +25937,15 @@
         <v>871</v>
       </c>
       <c r="B383" t="s">
-        <v>1068</v>
+        <v>1067</v>
       </c>
     </row>
     <row r="384">
       <c r="A384" t="s">
-        <v>1058</v>
+        <v>1057</v>
       </c>
       <c r="B384" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="385">
@@ -25956,7 +25953,7 @@
         <v>738</v>
       </c>
       <c r="B385" t="s">
-        <v>1070</v>
+        <v>1069</v>
       </c>
     </row>
     <row r="386">
@@ -25964,7 +25961,7 @@
         <v>746</v>
       </c>
       <c r="B386" t="s">
-        <v>1071</v>
+        <v>1070</v>
       </c>
     </row>
     <row r="387">
@@ -25972,7 +25969,7 @@
         <v>777</v>
       </c>
       <c r="B387" t="s">
-        <v>1072</v>
+        <v>1071</v>
       </c>
     </row>
     <row r="388">
@@ -25980,7 +25977,7 @@
         <v>808</v>
       </c>
       <c r="B388" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="389">
@@ -25988,23 +25985,23 @@
         <v>1038</v>
       </c>
       <c r="B389" t="s">
-        <v>1074</v>
+        <v>1073</v>
       </c>
     </row>
     <row r="390">
       <c r="A390" t="s">
-        <v>1058</v>
+        <v>1057</v>
       </c>
       <c r="B390" t="s">
-        <v>1075</v>
+        <v>1074</v>
       </c>
     </row>
     <row r="391">
       <c r="A391" t="s">
-        <v>649</v>
+        <v>1038</v>
       </c>
       <c r="B391" t="s">
-        <v>1076</v>
+        <v>1075</v>
       </c>
     </row>
     <row r="392">
@@ -26012,7 +26009,7 @@
         <v>754</v>
       </c>
       <c r="B392" t="s">
-        <v>1077</v>
+        <v>1076</v>
       </c>
     </row>
     <row r="393">
@@ -26020,7 +26017,7 @@
         <v>750</v>
       </c>
       <c r="B393" t="s">
-        <v>1078</v>
+        <v>1077</v>
       </c>
     </row>
     <row r="394">
@@ -26028,7 +26025,7 @@
         <v>779</v>
       </c>
       <c r="B394" t="s">
-        <v>1079</v>
+        <v>1078</v>
       </c>
     </row>
     <row r="395">
@@ -26036,7 +26033,7 @@
         <v>754</v>
       </c>
       <c r="B395" t="s">
-        <v>1080</v>
+        <v>1079</v>
       </c>
     </row>
     <row r="396">
@@ -26044,23 +26041,23 @@
         <v>748</v>
       </c>
       <c r="B396" t="s">
-        <v>1081</v>
+        <v>1080</v>
       </c>
     </row>
     <row r="397">
       <c r="A397" t="s">
-        <v>1058</v>
+        <v>1057</v>
       </c>
       <c r="B397" t="s">
-        <v>1082</v>
+        <v>1081</v>
       </c>
     </row>
     <row r="398">
       <c r="A398" t="s">
+        <v>1082</v>
+      </c>
+      <c r="B398" t="s">
         <v>1083</v>
-      </c>
-      <c r="B398" t="s">
-        <v>1084</v>
       </c>
     </row>
     <row r="399">
@@ -26068,15 +26065,15 @@
         <v>754</v>
       </c>
       <c r="B399" t="s">
-        <v>1085</v>
+        <v>1084</v>
       </c>
     </row>
     <row r="400">
       <c r="A400" t="s">
+        <v>1085</v>
+      </c>
+      <c r="B400" t="s">
         <v>1086</v>
-      </c>
-      <c r="B400" t="s">
-        <v>1087</v>
       </c>
     </row>
     <row r="401">
@@ -26084,7 +26081,7 @@
         <v>804</v>
       </c>
       <c r="B401" t="s">
-        <v>1088</v>
+        <v>1087</v>
       </c>
     </row>
     <row r="402">
@@ -26092,23 +26089,23 @@
         <v>742</v>
       </c>
       <c r="B402" t="s">
-        <v>1089</v>
+        <v>1088</v>
       </c>
     </row>
     <row r="403">
       <c r="A403" t="s">
+        <v>1089</v>
+      </c>
+      <c r="B403" t="s">
         <v>1090</v>
-      </c>
-      <c r="B403" t="s">
-        <v>1091</v>
       </c>
     </row>
     <row r="404">
       <c r="A404" t="s">
+        <v>1091</v>
+      </c>
+      <c r="B404" t="s">
         <v>1092</v>
-      </c>
-      <c r="B404" t="s">
-        <v>1093</v>
       </c>
     </row>
     <row r="405">
@@ -26116,7 +26113,7 @@
         <v>7</v>
       </c>
       <c r="B405" t="s">
-        <v>1094</v>
+        <v>1093</v>
       </c>
     </row>
     <row r="406">
@@ -26124,31 +26121,31 @@
         <v>982</v>
       </c>
       <c r="B406" t="s">
-        <v>1095</v>
+        <v>1094</v>
       </c>
     </row>
     <row r="407">
       <c r="A407" t="s">
+        <v>1095</v>
+      </c>
+      <c r="B407" t="s">
         <v>1096</v>
-      </c>
-      <c r="B407" t="s">
-        <v>1097</v>
       </c>
     </row>
     <row r="408">
       <c r="A408" t="s">
+        <v>1097</v>
+      </c>
+      <c r="B408" t="s">
         <v>1098</v>
-      </c>
-      <c r="B408" t="s">
-        <v>1099</v>
       </c>
     </row>
     <row r="409">
       <c r="A409" t="s">
+        <v>1099</v>
+      </c>
+      <c r="B409" t="s">
         <v>1100</v>
-      </c>
-      <c r="B409" t="s">
-        <v>1101</v>
       </c>
     </row>
     <row r="410">
@@ -26156,7 +26153,7 @@
         <v>562</v>
       </c>
       <c r="B410" t="s">
-        <v>1102</v>
+        <v>1101</v>
       </c>
     </row>
     <row r="411">
@@ -26164,7 +26161,7 @@
         <v>674</v>
       </c>
       <c r="B411" t="s">
-        <v>1103</v>
+        <v>1102</v>
       </c>
     </row>
     <row r="412">
@@ -26172,7 +26169,7 @@
         <v>627</v>
       </c>
       <c r="B412" t="s">
-        <v>1104</v>
+        <v>1103</v>
       </c>
     </row>
     <row r="413">
@@ -26180,7 +26177,7 @@
         <v>562</v>
       </c>
       <c r="B413" t="s">
-        <v>1105</v>
+        <v>1104</v>
       </c>
     </row>
     <row r="414">
@@ -26188,7 +26185,7 @@
         <v>562</v>
       </c>
       <c r="B414" t="s">
-        <v>1106</v>
+        <v>1105</v>
       </c>
     </row>
     <row r="415">
@@ -26196,7 +26193,7 @@
         <v>514</v>
       </c>
       <c r="B415" t="s">
-        <v>1107</v>
+        <v>1106</v>
       </c>
     </row>
     <row r="416">
@@ -26204,7 +26201,7 @@
         <v>857</v>
       </c>
       <c r="B416" t="s">
-        <v>1108</v>
+        <v>1107</v>
       </c>
     </row>
     <row r="417">
@@ -26212,431 +26209,431 @@
         <v>621</v>
       </c>
       <c r="B417" t="s">
-        <v>1109</v>
+        <v>1108</v>
       </c>
     </row>
     <row r="418">
       <c r="A418" t="s">
+        <v>1109</v>
+      </c>
+      <c r="B418" t="s">
         <v>1110</v>
-      </c>
-      <c r="B418" t="s">
-        <v>1111</v>
       </c>
     </row>
     <row r="419">
       <c r="A419" t="s">
+        <v>1111</v>
+      </c>
+      <c r="B419" t="s">
         <v>1112</v>
-      </c>
-      <c r="B419" t="s">
-        <v>1113</v>
       </c>
     </row>
     <row r="420">
       <c r="A420" t="s">
+        <v>1113</v>
+      </c>
+      <c r="B420" t="s">
         <v>1114</v>
-      </c>
-      <c r="B420" t="s">
-        <v>1115</v>
       </c>
     </row>
     <row r="421">
       <c r="A421" t="s">
+        <v>1115</v>
+      </c>
+      <c r="B421" t="s">
         <v>1116</v>
-      </c>
-      <c r="B421" t="s">
-        <v>1117</v>
       </c>
     </row>
     <row r="422">
       <c r="A422" t="s">
+        <v>1117</v>
+      </c>
+      <c r="B422" t="s">
         <v>1118</v>
-      </c>
-      <c r="B422" t="s">
-        <v>1119</v>
       </c>
     </row>
     <row r="423">
       <c r="A423" t="s">
+        <v>1119</v>
+      </c>
+      <c r="B423" t="s">
         <v>1120</v>
-      </c>
-      <c r="B423" t="s">
-        <v>1121</v>
       </c>
     </row>
     <row r="424">
       <c r="A424" t="s">
+        <v>1121</v>
+      </c>
+      <c r="B424" t="s">
         <v>1122</v>
-      </c>
-      <c r="B424" t="s">
-        <v>1123</v>
       </c>
     </row>
     <row r="425">
       <c r="A425" t="s">
+        <v>1123</v>
+      </c>
+      <c r="B425" t="s">
         <v>1124</v>
-      </c>
-      <c r="B425" t="s">
-        <v>1125</v>
       </c>
     </row>
     <row r="426">
       <c r="A426" t="s">
+        <v>1125</v>
+      </c>
+      <c r="B426" t="s">
         <v>1126</v>
-      </c>
-      <c r="B426" t="s">
-        <v>1127</v>
       </c>
     </row>
     <row r="427">
       <c r="A427" t="s">
+        <v>1127</v>
+      </c>
+      <c r="B427" t="s">
         <v>1128</v>
-      </c>
-      <c r="B427" t="s">
-        <v>1129</v>
       </c>
     </row>
     <row r="428">
       <c r="A428" t="s">
+        <v>1129</v>
+      </c>
+      <c r="B428" t="s">
         <v>1130</v>
-      </c>
-      <c r="B428" t="s">
-        <v>1131</v>
       </c>
     </row>
     <row r="429">
       <c r="A429" t="s">
+        <v>1131</v>
+      </c>
+      <c r="B429" t="s">
         <v>1132</v>
-      </c>
-      <c r="B429" t="s">
-        <v>1133</v>
       </c>
     </row>
     <row r="430">
       <c r="A430" t="s">
+        <v>1133</v>
+      </c>
+      <c r="B430" t="s">
         <v>1134</v>
-      </c>
-      <c r="B430" t="s">
-        <v>1135</v>
       </c>
     </row>
     <row r="431">
       <c r="A431" t="s">
+        <v>1135</v>
+      </c>
+      <c r="B431" t="s">
         <v>1136</v>
-      </c>
-      <c r="B431" t="s">
-        <v>1137</v>
       </c>
     </row>
     <row r="432">
       <c r="A432" t="s">
+        <v>1137</v>
+      </c>
+      <c r="B432" t="s">
         <v>1138</v>
-      </c>
-      <c r="B432" t="s">
-        <v>1139</v>
       </c>
     </row>
     <row r="433">
       <c r="A433" t="s">
+        <v>1139</v>
+      </c>
+      <c r="B433" t="s">
         <v>1140</v>
-      </c>
-      <c r="B433" t="s">
-        <v>1141</v>
       </c>
     </row>
     <row r="434">
       <c r="A434" t="s">
+        <v>1141</v>
+      </c>
+      <c r="B434" t="s">
         <v>1142</v>
-      </c>
-      <c r="B434" t="s">
-        <v>1143</v>
       </c>
     </row>
     <row r="435">
       <c r="A435" t="s">
+        <v>1143</v>
+      </c>
+      <c r="B435" t="s">
         <v>1144</v>
-      </c>
-      <c r="B435" t="s">
-        <v>1145</v>
       </c>
     </row>
     <row r="436">
       <c r="A436" t="s">
+        <v>1145</v>
+      </c>
+      <c r="B436" t="s">
         <v>1146</v>
-      </c>
-      <c r="B436" t="s">
-        <v>1147</v>
       </c>
     </row>
     <row r="437">
       <c r="A437" t="s">
+        <v>1147</v>
+      </c>
+      <c r="B437" t="s">
         <v>1148</v>
-      </c>
-      <c r="B437" t="s">
-        <v>1149</v>
       </c>
     </row>
     <row r="438">
       <c r="A438" t="s">
+        <v>1149</v>
+      </c>
+      <c r="B438" t="s">
         <v>1150</v>
-      </c>
-      <c r="B438" t="s">
-        <v>1151</v>
       </c>
     </row>
     <row r="439">
       <c r="A439" t="s">
+        <v>1151</v>
+      </c>
+      <c r="B439" t="s">
         <v>1152</v>
-      </c>
-      <c r="B439" t="s">
-        <v>1153</v>
       </c>
     </row>
     <row r="440">
       <c r="A440" t="s">
+        <v>1153</v>
+      </c>
+      <c r="B440" t="s">
         <v>1154</v>
-      </c>
-      <c r="B440" t="s">
-        <v>1155</v>
       </c>
     </row>
     <row r="441">
       <c r="A441" t="s">
+        <v>1155</v>
+      </c>
+      <c r="B441" t="s">
         <v>1156</v>
-      </c>
-      <c r="B441" t="s">
-        <v>1157</v>
       </c>
     </row>
     <row r="442">
       <c r="A442" t="s">
+        <v>1157</v>
+      </c>
+      <c r="B442" t="s">
         <v>1158</v>
-      </c>
-      <c r="B442" t="s">
-        <v>1159</v>
       </c>
     </row>
     <row r="443">
       <c r="A443" t="s">
+        <v>1159</v>
+      </c>
+      <c r="B443" t="s">
         <v>1160</v>
-      </c>
-      <c r="B443" t="s">
-        <v>1161</v>
       </c>
     </row>
     <row r="444">
       <c r="A444" t="s">
+        <v>1161</v>
+      </c>
+      <c r="B444" t="s">
         <v>1162</v>
-      </c>
-      <c r="B444" t="s">
-        <v>1163</v>
       </c>
     </row>
     <row r="445">
       <c r="A445" t="s">
+        <v>1163</v>
+      </c>
+      <c r="B445" t="s">
         <v>1164</v>
-      </c>
-      <c r="B445" t="s">
-        <v>1165</v>
       </c>
     </row>
     <row r="446">
       <c r="A446" t="s">
+        <v>1165</v>
+      </c>
+      <c r="B446" t="s">
         <v>1166</v>
-      </c>
-      <c r="B446" t="s">
-        <v>1167</v>
       </c>
     </row>
     <row r="447">
       <c r="A447" t="s">
+        <v>1167</v>
+      </c>
+      <c r="B447" t="s">
         <v>1168</v>
-      </c>
-      <c r="B447" t="s">
-        <v>1169</v>
       </c>
     </row>
     <row r="448">
       <c r="A448" t="s">
+        <v>1169</v>
+      </c>
+      <c r="B448" t="s">
         <v>1170</v>
-      </c>
-      <c r="B448" t="s">
-        <v>1171</v>
       </c>
     </row>
     <row r="449">
       <c r="A449" t="s">
+        <v>1171</v>
+      </c>
+      <c r="B449" t="s">
         <v>1172</v>
-      </c>
-      <c r="B449" t="s">
-        <v>1173</v>
       </c>
     </row>
     <row r="450">
       <c r="A450" t="s">
+        <v>1173</v>
+      </c>
+      <c r="B450" t="s">
         <v>1174</v>
-      </c>
-      <c r="B450" t="s">
-        <v>1175</v>
       </c>
     </row>
     <row r="451">
       <c r="A451" t="s">
+        <v>1175</v>
+      </c>
+      <c r="B451" t="s">
         <v>1176</v>
-      </c>
-      <c r="B451" t="s">
-        <v>1177</v>
       </c>
     </row>
     <row r="452">
       <c r="A452" t="s">
+        <v>1177</v>
+      </c>
+      <c r="B452" t="s">
         <v>1178</v>
-      </c>
-      <c r="B452" t="s">
-        <v>1179</v>
       </c>
     </row>
     <row r="453">
       <c r="A453" t="s">
+        <v>1179</v>
+      </c>
+      <c r="B453" t="s">
         <v>1180</v>
-      </c>
-      <c r="B453" t="s">
-        <v>1181</v>
       </c>
     </row>
     <row r="454">
       <c r="A454" t="s">
+        <v>1181</v>
+      </c>
+      <c r="B454" t="s">
         <v>1182</v>
-      </c>
-      <c r="B454" t="s">
-        <v>1183</v>
       </c>
     </row>
     <row r="455">
       <c r="A455" t="s">
+        <v>1183</v>
+      </c>
+      <c r="B455" t="s">
         <v>1184</v>
-      </c>
-      <c r="B455" t="s">
-        <v>1185</v>
       </c>
     </row>
     <row r="456">
       <c r="A456" t="s">
+        <v>1185</v>
+      </c>
+      <c r="B456" t="s">
         <v>1186</v>
-      </c>
-      <c r="B456" t="s">
-        <v>1187</v>
       </c>
     </row>
     <row r="457">
       <c r="A457" t="s">
+        <v>1187</v>
+      </c>
+      <c r="B457" t="s">
         <v>1188</v>
-      </c>
-      <c r="B457" t="s">
-        <v>1189</v>
       </c>
     </row>
     <row r="458">
       <c r="A458" t="s">
+        <v>1189</v>
+      </c>
+      <c r="B458" t="s">
         <v>1190</v>
-      </c>
-      <c r="B458" t="s">
-        <v>1191</v>
       </c>
     </row>
     <row r="459">
       <c r="A459" t="s">
+        <v>1191</v>
+      </c>
+      <c r="B459" t="s">
         <v>1192</v>
-      </c>
-      <c r="B459" t="s">
-        <v>1193</v>
       </c>
     </row>
     <row r="460">
       <c r="A460" t="s">
+        <v>1193</v>
+      </c>
+      <c r="B460" t="s">
         <v>1194</v>
-      </c>
-      <c r="B460" t="s">
-        <v>1195</v>
       </c>
     </row>
     <row r="461">
       <c r="A461" t="s">
+        <v>1195</v>
+      </c>
+      <c r="B461" t="s">
         <v>1196</v>
-      </c>
-      <c r="B461" t="s">
-        <v>1197</v>
       </c>
     </row>
     <row r="462">
       <c r="A462" t="s">
+        <v>1197</v>
+      </c>
+      <c r="B462" t="s">
         <v>1198</v>
-      </c>
-      <c r="B462" t="s">
-        <v>1199</v>
       </c>
     </row>
     <row r="463">
       <c r="A463" t="s">
+        <v>1199</v>
+      </c>
+      <c r="B463" t="s">
         <v>1200</v>
-      </c>
-      <c r="B463" t="s">
-        <v>1201</v>
       </c>
     </row>
     <row r="464">
       <c r="A464" t="s">
+        <v>1201</v>
+      </c>
+      <c r="B464" t="s">
         <v>1202</v>
-      </c>
-      <c r="B464" t="s">
-        <v>1203</v>
       </c>
     </row>
     <row r="465">
       <c r="A465" t="s">
+        <v>1203</v>
+      </c>
+      <c r="B465" t="s">
         <v>1204</v>
-      </c>
-      <c r="B465" t="s">
-        <v>1205</v>
       </c>
     </row>
     <row r="466">
       <c r="A466" t="s">
+        <v>1205</v>
+      </c>
+      <c r="B466" t="s">
         <v>1206</v>
-      </c>
-      <c r="B466" t="s">
-        <v>1207</v>
       </c>
     </row>
     <row r="467">
       <c r="A467" t="s">
+        <v>1207</v>
+      </c>
+      <c r="B467" t="s">
         <v>1208</v>
-      </c>
-      <c r="B467" t="s">
-        <v>1209</v>
       </c>
     </row>
     <row r="468">
       <c r="A468" t="s">
+        <v>1209</v>
+      </c>
+      <c r="B468" t="s">
         <v>1210</v>
-      </c>
-      <c r="B468" t="s">
-        <v>1211</v>
       </c>
     </row>
     <row r="469">
       <c r="A469" t="s">
+        <v>1211</v>
+      </c>
+      <c r="B469" t="s">
         <v>1212</v>
-      </c>
-      <c r="B469" t="s">
-        <v>1213</v>
       </c>
     </row>
     <row r="470">
       <c r="A470" t="s">
+        <v>1213</v>
+      </c>
+      <c r="B470" t="s">
         <v>1214</v>
-      </c>
-      <c r="B470" t="s">
-        <v>1215</v>
       </c>
     </row>
   </sheetData>
@@ -26845,13 +26842,13 @@
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="B5" t="n">
         <v>0</v>
       </c>
       <c r="C5" t="n">
-        <v>63</v>
+        <v>74</v>
       </c>
       <c r="D5" t="n">
         <v>0</v>
@@ -26890,13 +26887,13 @@
         <v>91</v>
       </c>
       <c r="B8" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C8" t="n">
         <v>86</v>
       </c>
       <c r="D8" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="9">

</xml_diff>

<commit_message>
EJAM v2.32.4 all commits
</commit_message>
<xml_diff>
--- a/inst/testdata/examples_of_output/testoutput_ejam2excel_10pts_1miles.xlsx
+++ b/inst/testdata/examples_of_output/testoutput_ejam2excel_10pts_1miles.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1216" uniqueCount="1216">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1215" uniqueCount="1215">
   <si>
     <t xml:space="preserve">Analysis Title</t>
   </si>
@@ -38,7 +38,7 @@
     <t xml:space="preserve">Locations analyzed</t>
   </si>
   <si>
-    <t xml:space="preserve">Within 1 miles</t>
+    <t xml:space="preserve">Locations defined by latitude, longitude and radius</t>
   </si>
   <si>
     <t xml:space="preserve">Distance in miles</t>
@@ -3164,9 +3164,6 @@
     <t xml:space="preserve">US percentile for Supplemental Summary Index for Particulate Matter</t>
   </si>
   <si>
-    <t xml:space="preserve">46</t>
-  </si>
-  <si>
     <t xml:space="preserve">US percentile for Supplemental Summary Index for Ozone</t>
   </si>
   <si>
@@ -3362,7 +3359,7 @@
     <t xml:space="preserve">US type of raw score for Particulate Matter Summary Index</t>
   </si>
   <si>
-    <t xml:space="preserve">66.855</t>
+    <t xml:space="preserve">83.142</t>
   </si>
   <si>
     <t xml:space="preserve">US type of raw score for Ozone Summary Index</t>
@@ -3392,7 +3389,7 @@
     <t xml:space="preserve">US type of raw score for Traffic Proximity and Volume Summary Index</t>
   </si>
   <si>
-    <t xml:space="preserve">94.667</t>
+    <t xml:space="preserve">94.692</t>
   </si>
   <si>
     <t xml:space="preserve">US type of raw score for Lead Paint Summary Index</t>
@@ -3410,7 +3407,7 @@
     <t xml:space="preserve">US type of raw score for RMP Proximity Summary Index</t>
   </si>
   <si>
-    <t xml:space="preserve">122.999</t>
+    <t xml:space="preserve">123.057</t>
   </si>
   <si>
     <t xml:space="preserve">US type of raw score for Hazardous Waste Proximity Summary Index</t>
@@ -3428,7 +3425,7 @@
     <t xml:space="preserve">US type of raw score for Wastewater Discharge Summary Index</t>
   </si>
   <si>
-    <t xml:space="preserve">80.283</t>
+    <t xml:space="preserve">80.294</t>
   </si>
   <si>
     <t xml:space="preserve">US type of raw score for Drinking Water Non-Compliance Summary Index</t>
@@ -3440,7 +3437,7 @@
     <t xml:space="preserve">State type of raw score for Particulate Matter Summary Index</t>
   </si>
   <si>
-    <t xml:space="preserve">48.636</t>
+    <t xml:space="preserve">58.857</t>
   </si>
   <si>
     <t xml:space="preserve">State type of raw score for Ozone Summary Index</t>
@@ -3488,7 +3485,7 @@
     <t xml:space="preserve">State type of raw score for RMP Proximity Summary Index</t>
   </si>
   <si>
-    <t xml:space="preserve">106.014</t>
+    <t xml:space="preserve">106.043</t>
   </si>
   <si>
     <t xml:space="preserve">State type of raw score for Hazardous Waste Proximity Summary Index</t>
@@ -3506,7 +3503,7 @@
     <t xml:space="preserve">State type of raw score for Wastewater Discharge Summary Index</t>
   </si>
   <si>
-    <t xml:space="preserve">46.43</t>
+    <t xml:space="preserve">46.56</t>
   </si>
   <si>
     <t xml:space="preserve">State type of raw score for Drinking Water Non-Compliance Summary Index</t>
@@ -3518,7 +3515,7 @@
     <t xml:space="preserve">US type of raw score for Particulate Matter Supplemental Summary Index</t>
   </si>
   <si>
-    <t xml:space="preserve">62.937</t>
+    <t xml:space="preserve">78.034</t>
   </si>
   <si>
     <t xml:space="preserve">US type of raw score for Ozone Supplemental Summary Index</t>
@@ -3548,7 +3545,7 @@
     <t xml:space="preserve">US type of raw score for Traffic Proximity and Volume Supplemental Summary Index</t>
   </si>
   <si>
-    <t xml:space="preserve">91.252</t>
+    <t xml:space="preserve">91.293</t>
   </si>
   <si>
     <t xml:space="preserve">US type of raw score for Lead Paint Supplemental Summary Index</t>
@@ -3566,7 +3563,7 @@
     <t xml:space="preserve">US type of raw score for RMP Proximity Supplemental Summary Index</t>
   </si>
   <si>
-    <t xml:space="preserve">114.012</t>
+    <t xml:space="preserve">114.085</t>
   </si>
   <si>
     <t xml:space="preserve">US type of raw score for Hazardous Waste Proximity Supplemental Summary Index</t>
@@ -3584,7 +3581,7 @@
     <t xml:space="preserve">US type of raw score for Wastewater Discharge Supplemental Summary Index</t>
   </si>
   <si>
-    <t xml:space="preserve">78.077</t>
+    <t xml:space="preserve">78.09</t>
   </si>
   <si>
     <t xml:space="preserve">US type of raw score for Drinking Water Non-Compliance Supplemental Summary Index</t>
@@ -3596,7 +3593,7 @@
     <t xml:space="preserve">State type of raw score for Particulate Matter Supplemental Summary Index</t>
   </si>
   <si>
-    <t xml:space="preserve">45.359</t>
+    <t xml:space="preserve">55.113</t>
   </si>
   <si>
     <t xml:space="preserve">State type of raw score for Ozone Supplemental Summary Index</t>
@@ -3644,7 +3641,7 @@
     <t xml:space="preserve">State type of raw score for RMP Proximity Supplemental Summary Index</t>
   </si>
   <si>
-    <t xml:space="preserve">97.655</t>
+    <t xml:space="preserve">97.693</t>
   </si>
   <si>
     <t xml:space="preserve">State type of raw score for Hazardous Waste Proximity Supplemental Summary Index</t>
@@ -3662,7 +3659,7 @@
     <t xml:space="preserve">State type of raw score for Wastewater Discharge Supplemental Summary Index</t>
   </si>
   <si>
-    <t xml:space="preserve">47.177</t>
+    <t xml:space="preserve">47.318</t>
   </si>
   <si>
     <t xml:space="preserve">State type of raw score for Drinking Water Non-Compliance Supplemental Summary Index</t>
@@ -3954,6 +3951,41 @@
     </dxf>
   </dxfs>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <xdr:oneCellAnchor xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+    <xdr:from xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+      <xdr:col xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">0</xdr:col>
+      <xdr:colOff xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">0</xdr:colOff>
+      <xdr:row xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">0</xdr:row>
+      <xdr:rowOff xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" cx="9144000" cy="29260800"/>
+    <xdr:pic xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+      <xdr:nvPicPr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+        <xdr:cNvPr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" id="1" name="Picture 1"/>
+        <xdr:cNvPicPr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+          <a:picLocks xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+        </a:blip>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
@@ -5587,322 +5619,322 @@
         <v>1045</v>
       </c>
       <c r="MZ1" s="19" t="s">
+        <v>1046</v>
+      </c>
+      <c r="NA1" s="19" t="s">
         <v>1047</v>
       </c>
-      <c r="NA1" s="19" t="s">
+      <c r="NB1" s="19" t="s">
         <v>1048</v>
       </c>
-      <c r="NB1" s="19" t="s">
+      <c r="NC1" s="19" t="s">
         <v>1049</v>
       </c>
-      <c r="NC1" s="19" t="s">
+      <c r="ND1" s="19" t="s">
         <v>1050</v>
       </c>
-      <c r="ND1" s="19" t="s">
+      <c r="NE1" s="19" t="s">
         <v>1051</v>
       </c>
-      <c r="NE1" s="19" t="s">
+      <c r="NF1" s="19" t="s">
         <v>1052</v>
       </c>
-      <c r="NF1" s="19" t="s">
-        <v>1053</v>
-      </c>
       <c r="NG1" s="19" t="s">
-        <v>1055</v>
+        <v>1054</v>
       </c>
       <c r="NH1" s="19" t="s">
-        <v>1057</v>
+        <v>1056</v>
       </c>
       <c r="NI1" s="19" t="s">
+        <v>1058</v>
+      </c>
+      <c r="NJ1" s="19" t="s">
         <v>1059</v>
       </c>
-      <c r="NJ1" s="19" t="s">
+      <c r="NK1" s="19" t="s">
         <v>1060</v>
       </c>
-      <c r="NK1" s="19" t="s">
+      <c r="NL1" s="20" t="s">
         <v>1061</v>
       </c>
-      <c r="NL1" s="20" t="s">
+      <c r="NM1" s="20" t="s">
         <v>1062</v>
       </c>
-      <c r="NM1" s="20" t="s">
+      <c r="NN1" s="20" t="s">
         <v>1063</v>
       </c>
-      <c r="NN1" s="20" t="s">
+      <c r="NO1" s="20" t="s">
         <v>1064</v>
       </c>
-      <c r="NO1" s="20" t="s">
+      <c r="NP1" s="20" t="s">
         <v>1065</v>
       </c>
-      <c r="NP1" s="20" t="s">
+      <c r="NQ1" s="20" t="s">
         <v>1066</v>
       </c>
-      <c r="NQ1" s="20" t="s">
+      <c r="NR1" s="20" t="s">
         <v>1067</v>
       </c>
-      <c r="NR1" s="20" t="s">
+      <c r="NS1" s="20" t="s">
         <v>1068</v>
       </c>
-      <c r="NS1" s="20" t="s">
+      <c r="NT1" s="20" t="s">
         <v>1069</v>
       </c>
-      <c r="NT1" s="20" t="s">
+      <c r="NU1" s="20" t="s">
         <v>1070</v>
       </c>
-      <c r="NU1" s="20" t="s">
+      <c r="NV1" s="20" t="s">
         <v>1071</v>
       </c>
-      <c r="NV1" s="20" t="s">
+      <c r="NW1" s="20" t="s">
         <v>1072</v>
       </c>
-      <c r="NW1" s="20" t="s">
+      <c r="NX1" s="20" t="s">
         <v>1073</v>
       </c>
-      <c r="NX1" s="20" t="s">
+      <c r="NY1" s="20" t="s">
         <v>1074</v>
       </c>
-      <c r="NY1" s="20" t="s">
+      <c r="NZ1" s="20" t="s">
         <v>1075</v>
       </c>
-      <c r="NZ1" s="20" t="s">
+      <c r="OA1" s="20" t="s">
         <v>1076</v>
       </c>
-      <c r="OA1" s="20" t="s">
+      <c r="OB1" s="20" t="s">
         <v>1077</v>
       </c>
-      <c r="OB1" s="20" t="s">
+      <c r="OC1" s="20" t="s">
         <v>1078</v>
       </c>
-      <c r="OC1" s="20" t="s">
+      <c r="OD1" s="20" t="s">
         <v>1079</v>
       </c>
-      <c r="OD1" s="20" t="s">
+      <c r="OE1" s="20" t="s">
         <v>1080</v>
       </c>
-      <c r="OE1" s="20" t="s">
+      <c r="OF1" s="20" t="s">
         <v>1081</v>
       </c>
-      <c r="OF1" s="20" t="s">
-        <v>1082</v>
-      </c>
       <c r="OG1" s="20" t="s">
+        <v>1083</v>
+      </c>
+      <c r="OH1" s="20" t="s">
         <v>1084</v>
       </c>
-      <c r="OH1" s="20" t="s">
-        <v>1085</v>
-      </c>
       <c r="OI1" s="20" t="s">
+        <v>1086</v>
+      </c>
+      <c r="OJ1" s="20" t="s">
         <v>1087</v>
       </c>
-      <c r="OJ1" s="20" t="s">
+      <c r="OK1" s="20" t="s">
         <v>1088</v>
       </c>
-      <c r="OK1" s="20" t="s">
-        <v>1089</v>
-      </c>
       <c r="OL1" s="10" t="s">
-        <v>1091</v>
+        <v>1090</v>
       </c>
       <c r="OM1" s="10" t="s">
+        <v>1092</v>
+      </c>
+      <c r="ON1" s="10" t="s">
         <v>1093</v>
       </c>
-      <c r="ON1" s="10" t="s">
+      <c r="OO1" s="9" t="s">
         <v>1094</v>
       </c>
-      <c r="OO1" s="9" t="s">
-        <v>1095</v>
-      </c>
       <c r="OP1" s="9" t="s">
-        <v>1097</v>
+        <v>1096</v>
       </c>
       <c r="OQ1" s="3" t="s">
-        <v>1099</v>
+        <v>1098</v>
       </c>
       <c r="OR1" s="3" t="s">
+        <v>1100</v>
+      </c>
+      <c r="OS1" s="3" t="s">
         <v>1101</v>
       </c>
-      <c r="OS1" s="3" t="s">
+      <c r="OT1" s="9" t="s">
         <v>1102</v>
       </c>
-      <c r="OT1" s="9" t="s">
+      <c r="OU1" s="9" t="s">
         <v>1103</v>
       </c>
-      <c r="OU1" s="9" t="s">
+      <c r="OV1" s="9" t="s">
         <v>1104</v>
       </c>
-      <c r="OV1" s="9" t="s">
+      <c r="OW1" s="9" t="s">
         <v>1105</v>
       </c>
-      <c r="OW1" s="9" t="s">
+      <c r="OX1" s="9" t="s">
         <v>1106</v>
       </c>
-      <c r="OX1" s="9" t="s">
+      <c r="OY1" s="9" t="s">
         <v>1107</v>
       </c>
-      <c r="OY1" s="9" t="s">
+      <c r="OZ1" s="9" t="s">
         <v>1108</v>
       </c>
-      <c r="OZ1" s="9" t="s">
-        <v>1109</v>
-      </c>
       <c r="PA1" s="21" t="s">
-        <v>1111</v>
+        <v>1110</v>
       </c>
       <c r="PB1" s="21" t="s">
-        <v>1113</v>
+        <v>1112</v>
       </c>
       <c r="PC1" s="21" t="s">
-        <v>1115</v>
+        <v>1114</v>
       </c>
       <c r="PD1" s="21" t="s">
-        <v>1117</v>
+        <v>1116</v>
       </c>
       <c r="PE1" s="21" t="s">
-        <v>1119</v>
+        <v>1118</v>
       </c>
       <c r="PF1" s="21" t="s">
-        <v>1121</v>
+        <v>1120</v>
       </c>
       <c r="PG1" s="21" t="s">
-        <v>1123</v>
+        <v>1122</v>
       </c>
       <c r="PH1" s="21" t="s">
-        <v>1125</v>
+        <v>1124</v>
       </c>
       <c r="PI1" s="21" t="s">
-        <v>1127</v>
+        <v>1126</v>
       </c>
       <c r="PJ1" s="21" t="s">
-        <v>1129</v>
+        <v>1128</v>
       </c>
       <c r="PK1" s="21" t="s">
-        <v>1131</v>
+        <v>1130</v>
       </c>
       <c r="PL1" s="21" t="s">
-        <v>1133</v>
+        <v>1132</v>
       </c>
       <c r="PM1" s="21" t="s">
-        <v>1135</v>
+        <v>1134</v>
       </c>
       <c r="PN1" s="19" t="s">
-        <v>1137</v>
+        <v>1136</v>
       </c>
       <c r="PO1" s="19" t="s">
-        <v>1139</v>
+        <v>1138</v>
       </c>
       <c r="PP1" s="19" t="s">
-        <v>1141</v>
+        <v>1140</v>
       </c>
       <c r="PQ1" s="19" t="s">
-        <v>1143</v>
+        <v>1142</v>
       </c>
       <c r="PR1" s="19" t="s">
-        <v>1145</v>
+        <v>1144</v>
       </c>
       <c r="PS1" s="19" t="s">
-        <v>1147</v>
+        <v>1146</v>
       </c>
       <c r="PT1" s="19" t="s">
-        <v>1149</v>
+        <v>1148</v>
       </c>
       <c r="PU1" s="19" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="PV1" s="19" t="s">
-        <v>1153</v>
+        <v>1152</v>
       </c>
       <c r="PW1" s="19" t="s">
-        <v>1155</v>
+        <v>1154</v>
       </c>
       <c r="PX1" s="19" t="s">
-        <v>1157</v>
+        <v>1156</v>
       </c>
       <c r="PY1" s="19" t="s">
-        <v>1159</v>
+        <v>1158</v>
       </c>
       <c r="PZ1" s="19" t="s">
-        <v>1161</v>
+        <v>1160</v>
       </c>
       <c r="QA1" s="21" t="s">
-        <v>1163</v>
+        <v>1162</v>
       </c>
       <c r="QB1" s="21" t="s">
-        <v>1165</v>
+        <v>1164</v>
       </c>
       <c r="QC1" s="21" t="s">
-        <v>1167</v>
+        <v>1166</v>
       </c>
       <c r="QD1" s="21" t="s">
-        <v>1169</v>
+        <v>1168</v>
       </c>
       <c r="QE1" s="21" t="s">
-        <v>1171</v>
+        <v>1170</v>
       </c>
       <c r="QF1" s="21" t="s">
-        <v>1173</v>
+        <v>1172</v>
       </c>
       <c r="QG1" s="21" t="s">
-        <v>1175</v>
+        <v>1174</v>
       </c>
       <c r="QH1" s="21" t="s">
-        <v>1177</v>
+        <v>1176</v>
       </c>
       <c r="QI1" s="21" t="s">
-        <v>1179</v>
+        <v>1178</v>
       </c>
       <c r="QJ1" s="21" t="s">
-        <v>1181</v>
+        <v>1180</v>
       </c>
       <c r="QK1" s="21" t="s">
-        <v>1183</v>
+        <v>1182</v>
       </c>
       <c r="QL1" s="21" t="s">
-        <v>1185</v>
+        <v>1184</v>
       </c>
       <c r="QM1" s="21" t="s">
-        <v>1187</v>
+        <v>1186</v>
       </c>
       <c r="QN1" s="19" t="s">
-        <v>1189</v>
+        <v>1188</v>
       </c>
       <c r="QO1" s="19" t="s">
-        <v>1191</v>
+        <v>1190</v>
       </c>
       <c r="QP1" s="19" t="s">
-        <v>1193</v>
+        <v>1192</v>
       </c>
       <c r="QQ1" s="19" t="s">
-        <v>1195</v>
+        <v>1194</v>
       </c>
       <c r="QR1" s="19" t="s">
-        <v>1197</v>
+        <v>1196</v>
       </c>
       <c r="QS1" s="19" t="s">
-        <v>1199</v>
+        <v>1198</v>
       </c>
       <c r="QT1" s="19" t="s">
-        <v>1201</v>
+        <v>1200</v>
       </c>
       <c r="QU1" s="19" t="s">
-        <v>1203</v>
+        <v>1202</v>
       </c>
       <c r="QV1" s="19" t="s">
-        <v>1205</v>
+        <v>1204</v>
       </c>
       <c r="QW1" s="19" t="s">
-        <v>1207</v>
+        <v>1206</v>
       </c>
       <c r="QX1" s="19" t="s">
-        <v>1209</v>
+        <v>1208</v>
       </c>
       <c r="QY1" s="19" t="s">
-        <v>1211</v>
+        <v>1210</v>
       </c>
       <c r="QZ1" s="19" t="s">
-        <v>1213</v>
+        <v>1212</v>
       </c>
       <c r="RA1" s="3" t="s">
-        <v>1215</v>
+        <v>1214</v>
       </c>
     </row>
     <row r="2">
@@ -5944,7 +5976,7 @@
         <v>1.2971052975883</v>
       </c>
       <c r="P2" s="28" t="n">
-        <v>0.88843281886032</v>
+        <v>0.888432818860319</v>
       </c>
       <c r="Q2" s="28" t="n">
         <v>0.504501586747553</v>
@@ -6151,7 +6183,7 @@
         <v>0.165534349534978</v>
       </c>
       <c r="CG2" s="30" t="n">
-        <v>0.0363344063498082</v>
+        <v>0.0363344063498081</v>
       </c>
       <c r="CH2" s="30" t="n">
         <v>0.114685712835881</v>
@@ -6274,7 +6306,7 @@
         <v>4.09841464967071</v>
       </c>
       <c r="DV2" s="24" t="n">
-        <v>8.64702294436021</v>
+        <v>8.64702294436022</v>
       </c>
       <c r="DW2" s="24" t="n">
         <v>4.84812175044326</v>
@@ -6301,7 +6333,7 @@
         <v>0.18685476581036</v>
       </c>
       <c r="EE2" s="24" t="n">
-        <v>9.70949446123183</v>
+        <v>9.70949446123182</v>
       </c>
       <c r="EF2" s="23" t="n">
         <v>45.4388149700272</v>
@@ -6319,7 +6351,7 @@
         <v>5904786.24802174</v>
       </c>
       <c r="EK2" s="30" t="n">
-        <v>0.562024279351765</v>
+        <v>0.562024279351764</v>
       </c>
       <c r="EL2" s="24" t="n">
         <v>0.109480426162384</v>
@@ -6929,7 +6961,7 @@
         <v>85</v>
       </c>
       <c r="MM2" s="29" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="MN2" s="29" t="n">
         <v>76</v>
@@ -6968,7 +7000,7 @@
         <v>78</v>
       </c>
       <c r="MZ2" s="29" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="NA2" s="29" t="n">
         <v>67</v>
@@ -7130,13 +7162,13 @@
         <v>147.526020073567</v>
       </c>
       <c r="PB2" s="25" t="n">
-        <v>1.73908625064187</v>
+        <v>0</v>
       </c>
       <c r="PC2" s="25" t="n">
         <v>117.411682117158</v>
       </c>
       <c r="PD2" s="25" t="n">
-        <v>71.1082403321686</v>
+        <v>71.1082403321685</v>
       </c>
       <c r="PE2" s="25" t="n">
         <v>49.3337969312927</v>
@@ -7169,7 +7201,7 @@
         <v>30.261877629349</v>
       </c>
       <c r="PO2" s="25" t="n">
-        <v>7.62900682444058</v>
+        <v>7.81492351857363</v>
       </c>
       <c r="PP2" s="25" t="n">
         <v>102.341562793256</v>
@@ -7208,7 +7240,7 @@
         <v>123.623333748108</v>
       </c>
       <c r="QB2" s="25" t="n">
-        <v>1.45910485025071</v>
+        <v>0</v>
       </c>
       <c r="QC2" s="25" t="n">
         <v>97.5633727537407</v>
@@ -7247,7 +7279,7 @@
         <v>20.1659993085997</v>
       </c>
       <c r="QO2" s="25" t="n">
-        <v>5.13716694653457</v>
+        <v>5.25275661180307</v>
       </c>
       <c r="QP2" s="25" t="n">
         <v>67.4866656619721</v>
@@ -8302,7 +8334,7 @@
         <v>2</v>
       </c>
       <c r="MM3" s="29" t="n">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="MN3" s="29" t="n">
         <v>20</v>
@@ -8341,7 +8373,7 @@
         <v>2</v>
       </c>
       <c r="MZ3" s="29" t="n">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="NA3" s="29" t="n">
         <v>25</v>
@@ -8380,7 +8412,7 @@
         <v>31</v>
       </c>
       <c r="NM3" s="29" t="n">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="NN3" s="29" t="n">
         <v>52</v>
@@ -8419,7 +8451,7 @@
         <v>34</v>
       </c>
       <c r="NZ3" s="29" t="n">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="OA3" s="29" t="n">
         <v>58</v>
@@ -8503,10 +8535,10 @@
         <v>1.02026861584964</v>
       </c>
       <c r="PB3" s="25" t="n">
-        <v>8.67228323472191</v>
+        <v>1.53040292377445</v>
       </c>
       <c r="PC3" s="25" t="n">
-        <v>13.1908713550648</v>
+        <v>13.1908713550649</v>
       </c>
       <c r="PD3" s="25" t="n">
         <v>1.53040292377445</v>
@@ -8527,7 +8559,7 @@
         <v>0</v>
       </c>
       <c r="PJ3" s="25" t="n">
-        <v>0.387310138562227</v>
+        <v>0.387310138562228</v>
       </c>
       <c r="PK3" s="25" t="n">
         <v>33.69486095776</v>
@@ -8536,13 +8568,13 @@
         <v>4.66382942230378</v>
       </c>
       <c r="PM3" s="25" t="n">
-        <v>39.7904760181358</v>
+        <v>39.9115104364365</v>
       </c>
       <c r="PN3" s="25" t="n">
         <v>29.3478476488843</v>
       </c>
       <c r="PO3" s="25" t="n">
-        <v>20.8275047830792</v>
+        <v>9.46704762867236</v>
       </c>
       <c r="PP3" s="25" t="n">
         <v>55.7276054566087</v>
@@ -8581,7 +8613,7 @@
         <v>2.56516565088795</v>
       </c>
       <c r="QB3" s="25" t="n">
-        <v>21.8039080325476</v>
+        <v>3.84774847633193</v>
       </c>
       <c r="QC3" s="25" t="n">
         <v>33.1607334747035</v>
@@ -8614,13 +8646,13 @@
         <v>11.7296654158357</v>
       </c>
       <c r="QM3" s="25" t="n">
-        <v>100.04146038463</v>
+        <v>100.352160362697</v>
       </c>
       <c r="QN3" s="25" t="n">
         <v>40.9150689864568</v>
       </c>
       <c r="QO3" s="25" t="n">
-        <v>29.0365005710339</v>
+        <v>13.1984093504699</v>
       </c>
       <c r="QP3" s="25" t="n">
         <v>77.6720353423386</v>
@@ -8800,7 +8832,7 @@
         <v>0.808440505802706</v>
       </c>
       <c r="AX4" s="28" t="n">
-        <v>0.696691533769616</v>
+        <v>0.696691533769615</v>
       </c>
       <c r="AY4" s="28" t="n">
         <v>1.13451089342981</v>
@@ -8968,7 +9000,7 @@
         <v>0.178593561152135</v>
       </c>
       <c r="DB4" s="30" t="n">
-        <v>0.821406438847864</v>
+        <v>0.821406438847865</v>
       </c>
       <c r="DC4" s="30" t="n">
         <v>0.0756098645666114</v>
@@ -9043,7 +9075,7 @@
         <v>0</v>
       </c>
       <c r="EA4" s="30" t="n">
-        <v>0.0774551392158331</v>
+        <v>0.077455139215833</v>
       </c>
       <c r="EB4" s="30" t="n">
         <v>0.000286464856163381</v>
@@ -9683,7 +9715,7 @@
         <v>58</v>
       </c>
       <c r="MM4" s="29" t="n">
-        <v>66</v>
+        <v>73</v>
       </c>
       <c r="MN4" s="29" t="n">
         <v>79</v>
@@ -9722,7 +9754,7 @@
         <v>43</v>
       </c>
       <c r="MZ4" s="29" t="n">
-        <v>52</v>
+        <v>64</v>
       </c>
       <c r="NA4" s="29" t="n">
         <v>78</v>
@@ -9761,7 +9793,7 @@
         <v>72</v>
       </c>
       <c r="NM4" s="29" t="n">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="NN4" s="29" t="n">
         <v>74</v>
@@ -9800,7 +9832,7 @@
         <v>72</v>
       </c>
       <c r="NZ4" s="29" t="n">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="OA4" s="29" t="n">
         <v>76</v>
@@ -9833,7 +9865,7 @@
         <v>71</v>
       </c>
       <c r="OK4" s="29" t="n">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="OL4" s="22" t="n">
         <v>121</v>
@@ -9884,7 +9916,7 @@
         <v>61.9334383542575</v>
       </c>
       <c r="PB4" s="25" t="n">
-        <v>73.583148629747</v>
+        <v>92.0170480357706</v>
       </c>
       <c r="PC4" s="25" t="n">
         <v>130.362913541297</v>
@@ -9917,13 +9949,13 @@
         <v>116.507485254061</v>
       </c>
       <c r="PM4" s="25" t="n">
-        <v>122.665964781077</v>
+        <v>122.681265493211</v>
       </c>
       <c r="PN4" s="25" t="n">
         <v>99.5955004053087</v>
       </c>
       <c r="PO4" s="25" t="n">
-        <v>52.2258272098887</v>
+        <v>64.9079205832168</v>
       </c>
       <c r="PP4" s="25" t="n">
         <v>116.992026021754</v>
@@ -9956,13 +9988,13 @@
         <v>99.498695445133</v>
       </c>
       <c r="PZ4" s="25" t="n">
-        <v>70.1255436840799</v>
+        <v>70.3255780609697</v>
       </c>
       <c r="QA4" s="25" t="n">
         <v>59.8066990248148</v>
       </c>
       <c r="QB4" s="25" t="n">
-        <v>70.9223064278375</v>
+        <v>88.7164059904571</v>
       </c>
       <c r="QC4" s="25" t="n">
         <v>125.729072309413</v>
@@ -9977,7 +10009,7 @@
         <v>120.668901902014</v>
       </c>
       <c r="QG4" s="25" t="n">
-        <v>99.6111751270708</v>
+        <v>99.6111751270709</v>
       </c>
       <c r="QH4" s="25" t="n">
         <v>121.583029317863</v>
@@ -9995,13 +10027,13 @@
         <v>112.464386000112</v>
       </c>
       <c r="QM4" s="25" t="n">
-        <v>118.326861908482</v>
+        <v>118.342435978211</v>
       </c>
       <c r="QN4" s="25" t="n">
         <v>100.535119459682</v>
       </c>
       <c r="QO4" s="25" t="n">
-        <v>52.5458095107339</v>
+        <v>65.3126791318764</v>
       </c>
       <c r="QP4" s="25" t="n">
         <v>118.02557250542</v>
@@ -10034,7 +10066,7 @@
         <v>100.504794101966</v>
       </c>
       <c r="QZ4" s="25" t="n">
-        <v>70.7484835206945</v>
+        <v>70.9656682960832</v>
       </c>
       <c r="RA4" s="23" t="n">
         <v>3.14159265358979</v>
@@ -10082,7 +10114,7 @@
         <v>0.74041760014635</v>
       </c>
       <c r="Q5" s="28" t="n">
-        <v>0.47406498186589</v>
+        <v>0.474064981865891</v>
       </c>
       <c r="R5" s="28" t="n">
         <v>0.138140865358155</v>
@@ -10160,7 +10192,7 @@
         <v>0.161042981935975</v>
       </c>
       <c r="AQ5" s="28" t="n">
-        <v>0.00000000700600282267474</v>
+        <v>0.00000000700600282267473</v>
       </c>
       <c r="AR5" s="28" t="n">
         <v>0</v>
@@ -10187,7 +10219,7 @@
         <v>1.55763880639431</v>
       </c>
       <c r="AZ5" s="28" t="n">
-        <v>0.828307293378407</v>
+        <v>0.828307293378408</v>
       </c>
       <c r="BA5" s="28" t="n">
         <v>1.03749085655535</v>
@@ -10262,7 +10294,7 @@
         <v>0</v>
       </c>
       <c r="BY5" s="28" t="n">
-        <v>1.10861249778536</v>
+        <v>1.10861249778537</v>
       </c>
       <c r="BZ5" s="28" t="n">
         <v>1.05420820922925</v>
@@ -11064,7 +11096,7 @@
         <v>10</v>
       </c>
       <c r="MM5" s="29" t="n">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="MN5" s="29" t="n">
         <v>29</v>
@@ -11103,7 +11135,7 @@
         <v>12</v>
       </c>
       <c r="MZ5" s="29" t="n">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="NA5" s="29" t="n">
         <v>41</v>
@@ -11142,7 +11174,7 @@
         <v>40</v>
       </c>
       <c r="NM5" s="29" t="n">
-        <v>43</v>
+        <v>52</v>
       </c>
       <c r="NN5" s="29" t="n">
         <v>34</v>
@@ -11181,7 +11213,7 @@
         <v>55</v>
       </c>
       <c r="NZ5" s="29" t="n">
-        <v>63</v>
+        <v>74</v>
       </c>
       <c r="OA5" s="29" t="n">
         <v>42</v>
@@ -11265,7 +11297,7 @@
         <v>6.18106233110586</v>
       </c>
       <c r="PB5" s="25" t="n">
-        <v>13.670686056997</v>
+        <v>15.2311958777375</v>
       </c>
       <c r="PC5" s="25" t="n">
         <v>20.7134557649812</v>
@@ -11280,7 +11312,7 @@
         <v>17.5273118887225</v>
       </c>
       <c r="PG5" s="25" t="n">
-        <v>23.4354008386388</v>
+        <v>23.4354008386389</v>
       </c>
       <c r="PH5" s="25" t="n">
         <v>0</v>
@@ -11304,7 +11336,7 @@
         <v>26.4793069071469</v>
       </c>
       <c r="PO5" s="25" t="n">
-        <v>34.7549654650404</v>
+        <v>43.2873588710858</v>
       </c>
       <c r="PP5" s="25" t="n">
         <v>20.9065803078131</v>
@@ -11343,7 +11375,7 @@
         <v>15.5800649015706</v>
       </c>
       <c r="QB5" s="25" t="n">
-        <v>34.7504070270963</v>
+        <v>38.7170574772691</v>
       </c>
       <c r="QC5" s="25" t="n">
         <v>53.4826080364208</v>
@@ -11382,7 +11414,7 @@
         <v>53.6364288591919</v>
       </c>
       <c r="QO5" s="25" t="n">
-        <v>71.2110570067934</v>
+        <v>88.2582589647063</v>
       </c>
       <c r="QP5" s="25" t="n">
         <v>43.7864105760659</v>
@@ -11607,7 +11639,7 @@
         <v>0.92214072895529</v>
       </c>
       <c r="BM6" s="28" t="n">
-        <v>0.928737528344376</v>
+        <v>0.928737528344377</v>
       </c>
       <c r="BN6" s="28" t="n">
         <v>0.349566853352133</v>
@@ -12437,7 +12469,7 @@
         <v>30</v>
       </c>
       <c r="MM6" s="29" t="n">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="MN6" s="29" t="n">
         <v>14</v>
@@ -12461,7 +12493,7 @@
         <v>0</v>
       </c>
       <c r="MU6" s="29" t="n">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="MV6" s="29" t="n">
         <v>59</v>
@@ -12476,7 +12508,7 @@
         <v>24</v>
       </c>
       <c r="MZ6" s="29" t="n">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="NA6" s="29" t="n">
         <v>8</v>
@@ -12500,7 +12532,7 @@
         <v>0</v>
       </c>
       <c r="NH6" s="29" t="n">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="NI6" s="29" t="n">
         <v>57</v>
@@ -12515,7 +12547,7 @@
         <v>30</v>
       </c>
       <c r="NM6" s="29" t="n">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="NN6" s="29" t="n">
         <v>5</v>
@@ -12539,7 +12571,7 @@
         <v>0</v>
       </c>
       <c r="NU6" s="29" t="n">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="NV6" s="29" t="n">
         <v>42</v>
@@ -12554,7 +12586,7 @@
         <v>28</v>
       </c>
       <c r="NZ6" s="29" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="OA6" s="29" t="n">
         <v>2</v>
@@ -12578,7 +12610,7 @@
         <v>0</v>
       </c>
       <c r="OH6" s="29" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="OI6" s="29" t="n">
         <v>40</v>
@@ -12638,7 +12670,7 @@
         <v>23.0409848173639</v>
       </c>
       <c r="PB6" s="25" t="n">
-        <v>39.6968154045372</v>
+        <v>38.3412972176782</v>
       </c>
       <c r="PC6" s="25" t="n">
         <v>8.60817609314943</v>
@@ -12656,13 +12688,13 @@
         <v>63.4037977829396</v>
       </c>
       <c r="PH6" s="25" t="n">
-        <v>89.9767834707365</v>
+        <v>89.9767834707364</v>
       </c>
       <c r="PI6" s="25" t="n">
         <v>0</v>
       </c>
       <c r="PJ6" s="25" t="n">
-        <v>6.19607543280081</v>
+        <v>14.4085372098873</v>
       </c>
       <c r="PK6" s="25" t="n">
         <v>58.2397351865338</v>
@@ -12677,7 +12709,7 @@
         <v>19.9775292553547</v>
       </c>
       <c r="PO6" s="25" t="n">
-        <v>0.592906303592776</v>
+        <v>3.51759786028714</v>
       </c>
       <c r="PP6" s="25" t="n">
         <v>1.78813830308018</v>
@@ -12701,7 +12733,7 @@
         <v>0</v>
       </c>
       <c r="PW6" s="25" t="n">
-        <v>0</v>
+        <v>3.9915237843948</v>
       </c>
       <c r="PX6" s="25" t="n">
         <v>30.4151655251991</v>
@@ -12710,13 +12742,13 @@
         <v>14.2500183574574</v>
       </c>
       <c r="PZ6" s="25" t="n">
-        <v>38.4699021294061</v>
+        <v>38.4739015817123</v>
       </c>
       <c r="QA6" s="25" t="n">
         <v>31.3458835047324</v>
       </c>
       <c r="QB6" s="25" t="n">
-        <v>54.0675406722285</v>
+        <v>52.279349558934</v>
       </c>
       <c r="QC6" s="25" t="n">
         <v>11.9004922248481</v>
@@ -12740,7 +12772,7 @@
         <v>0</v>
       </c>
       <c r="QJ6" s="25" t="n">
-        <v>10.3630513735587</v>
+        <v>20.6658053899061</v>
       </c>
       <c r="QK6" s="25" t="n">
         <v>79.2183890714953</v>
@@ -12755,7 +12787,7 @@
         <v>24.9374188259632</v>
       </c>
       <c r="QO6" s="25" t="n">
-        <v>0.692512809959195</v>
+        <v>4.37388171593421</v>
       </c>
       <c r="QP6" s="25" t="n">
         <v>2.28970040109511</v>
@@ -12779,7 +12811,7 @@
         <v>0</v>
       </c>
       <c r="QW6" s="25" t="n">
-        <v>0</v>
+        <v>5.26382328212159</v>
       </c>
       <c r="QX6" s="25" t="n">
         <v>37.4967271481087</v>
@@ -12788,7 +12820,7 @@
         <v>17.6579693326827</v>
       </c>
       <c r="QZ6" s="25" t="n">
-        <v>51.6031654117135</v>
+        <v>51.6122746427208</v>
       </c>
       <c r="RA6" s="23" t="n">
         <v>3.14159265358979</v>
@@ -12995,7 +13027,7 @@
         <v>0.0506566683158606</v>
       </c>
       <c r="BR7" s="28" t="n">
-        <v>1.23409828060073</v>
+        <v>1.23409828060074</v>
       </c>
       <c r="BS7" s="28" t="n">
         <v>0</v>
@@ -13896,7 +13928,7 @@
         <v>30</v>
       </c>
       <c r="NM7" s="29" t="n">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="NN7" s="29" t="n">
         <v>52</v>
@@ -13935,7 +13967,7 @@
         <v>17</v>
       </c>
       <c r="NZ7" s="29" t="n">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="OA7" s="29" t="n">
         <v>40</v>
@@ -14019,7 +14051,7 @@
         <v>2.57799526706975</v>
       </c>
       <c r="PB7" s="25" t="n">
-        <v>21.5561089571271</v>
+        <v>21.4832938922479</v>
       </c>
       <c r="PC7" s="25" t="n">
         <v>37.6638998618618</v>
@@ -14058,7 +14090,7 @@
         <v>18.5456956459861</v>
       </c>
       <c r="PO7" s="25" t="n">
-        <v>45.0342108257509</v>
+        <v>51.7381606363633</v>
       </c>
       <c r="PP7" s="25" t="n">
         <v>42.0493123414748</v>
@@ -14097,7 +14129,7 @@
         <v>3.44053764346531</v>
       </c>
       <c r="QB7" s="25" t="n">
-        <v>28.7381910170622</v>
+        <v>28.6711470288776</v>
       </c>
       <c r="QC7" s="25" t="n">
         <v>45.0936442405563</v>
@@ -14136,7 +14168,7 @@
         <v>20.2600396385842</v>
       </c>
       <c r="QO7" s="25" t="n">
-        <v>49.2575284291922</v>
+        <v>56.6697766152045</v>
       </c>
       <c r="QP7" s="25" t="n">
         <v>41.0611492852566</v>
@@ -15199,7 +15231,7 @@
         <v>91</v>
       </c>
       <c r="MM8" s="29" t="n">
-        <v>78</v>
+        <v>88</v>
       </c>
       <c r="MN8" s="29" t="n">
         <v>70</v>
@@ -15238,7 +15270,7 @@
         <v>86</v>
       </c>
       <c r="MZ8" s="29" t="n">
-        <v>63</v>
+        <v>82</v>
       </c>
       <c r="NA8" s="29" t="n">
         <v>57</v>
@@ -15277,7 +15309,7 @@
         <v>67</v>
       </c>
       <c r="NM8" s="29" t="n">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="NN8" s="29" t="n">
         <v>39</v>
@@ -15316,7 +15348,7 @@
         <v>60</v>
       </c>
       <c r="NZ8" s="29" t="n">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="OA8" s="29" t="n">
         <v>33</v>
@@ -15400,7 +15432,7 @@
         <v>183.713982493363</v>
       </c>
       <c r="PB8" s="25" t="n">
-        <v>107.969029034477</v>
+        <v>160.11928862861</v>
       </c>
       <c r="PC8" s="25" t="n">
         <v>96.1876930283443</v>
@@ -15439,7 +15471,7 @@
         <v>121.916671389955</v>
       </c>
       <c r="PO8" s="25" t="n">
-        <v>69.164659040453</v>
+        <v>71.6344433323325</v>
       </c>
       <c r="PP8" s="25" t="n">
         <v>58.4536247063949</v>
@@ -15478,7 +15510,7 @@
         <v>149.792008783348</v>
       </c>
       <c r="QB8" s="25" t="n">
-        <v>88.0883946524944</v>
+        <v>130.53747044082</v>
       </c>
       <c r="QC8" s="25" t="n">
         <v>78.042392169296</v>
@@ -15517,7 +15549,7 @@
         <v>80.0075160437923</v>
       </c>
       <c r="QO8" s="25" t="n">
-        <v>45.3850939945673</v>
+        <v>47.0387666280044</v>
       </c>
       <c r="QP8" s="25" t="n">
         <v>37.9858914292202</v>
@@ -15610,7 +15642,7 @@
         <v>0.0778111794196792</v>
       </c>
       <c r="U9" s="28" t="n">
-        <v>0.626972300779197</v>
+        <v>0.626972300779196</v>
       </c>
       <c r="V9" s="28" t="n">
         <v>0.782126127209215</v>
@@ -15619,10 +15651,10 @@
         <v>0.680295662341148</v>
       </c>
       <c r="X9" s="28" t="n">
-        <v>0.482767619786045</v>
+        <v>0.482767619786044</v>
       </c>
       <c r="Y9" s="28" t="n">
-        <v>0.798109029343264</v>
+        <v>0.798109029343263</v>
       </c>
       <c r="Z9" s="28" t="n">
         <v>0.689443247912263</v>
@@ -15658,7 +15690,7 @@
         <v>0.315597493372166</v>
       </c>
       <c r="AK9" s="28" t="n">
-        <v>0.718916814525676</v>
+        <v>0.718916814525675</v>
       </c>
       <c r="AL9" s="28" t="n">
         <v>0.865774955289836</v>
@@ -15673,7 +15705,7 @@
         <v>0.323275781370935</v>
       </c>
       <c r="AP9" s="28" t="n">
-        <v>1.14239273939864</v>
+        <v>1.14239273939863</v>
       </c>
       <c r="AQ9" s="28" t="n">
         <v>0.00127945668741552</v>
@@ -15682,7 +15714,7 @@
         <v>0</v>
       </c>
       <c r="AS9" s="28" t="n">
-        <v>0.641215092504475</v>
+        <v>0.641215092504474</v>
       </c>
       <c r="AT9" s="28" t="n">
         <v>0.850273582914954</v>
@@ -15706,7 +15738,7 @@
         <v>0.0734344856287364</v>
       </c>
       <c r="BA9" s="28" t="n">
-        <v>0.643516130269683</v>
+        <v>0.643516130269682</v>
       </c>
       <c r="BB9" s="28" t="n">
         <v>0.711586175835813</v>
@@ -15838,7 +15870,7 @@
         <v>0.62495592971167</v>
       </c>
       <c r="CS9" s="30" t="n">
-        <v>0.406186862457548</v>
+        <v>0.406186862457547</v>
       </c>
       <c r="CT9" s="30" t="n">
         <v>0.0277818589783509</v>
@@ -15940,7 +15972,7 @@
         <v>0</v>
       </c>
       <c r="EA9" s="30" t="n">
-        <v>0.0362382863913995</v>
+        <v>0.0362382863913994</v>
       </c>
       <c r="EB9" s="30" t="n">
         <v>0.000213959160340706</v>
@@ -16580,7 +16612,7 @@
         <v>28</v>
       </c>
       <c r="MM9" s="29" t="n">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="MN9" s="29" t="n">
         <v>34</v>
@@ -16619,7 +16651,7 @@
         <v>21</v>
       </c>
       <c r="MZ9" s="29" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="NA9" s="29" t="n">
         <v>28</v>
@@ -16658,7 +16690,7 @@
         <v>33</v>
       </c>
       <c r="NM9" s="29" t="n">
-        <v>35</v>
+        <v>16</v>
       </c>
       <c r="NN9" s="29" t="n">
         <v>50</v>
@@ -16697,7 +16729,7 @@
         <v>18</v>
       </c>
       <c r="NZ9" s="29" t="n">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="OA9" s="29" t="n">
         <v>29</v>
@@ -16781,7 +16813,7 @@
         <v>21.0934471762864</v>
       </c>
       <c r="PB9" s="25" t="n">
-        <v>8.27365312211825</v>
+        <v>3.87543581374187</v>
       </c>
       <c r="PC9" s="25" t="n">
         <v>25.9808235385794</v>
@@ -16790,7 +16822,7 @@
         <v>27.577735351445</v>
       </c>
       <c r="PE9" s="25" t="n">
-        <v>36.0995966939888</v>
+        <v>36.0995966939889</v>
       </c>
       <c r="PF9" s="25" t="n">
         <v>31.6729652349235</v>
@@ -16820,7 +16852,7 @@
         <v>37.5073196608144</v>
       </c>
       <c r="PO9" s="25" t="n">
-        <v>38.6350906668497</v>
+        <v>17.5255175520074</v>
       </c>
       <c r="PP9" s="25" t="n">
         <v>56.4852300203805</v>
@@ -16859,7 +16891,7 @@
         <v>27.8119851657603</v>
       </c>
       <c r="QB9" s="25" t="n">
-        <v>10.8947662597267</v>
+        <v>5.13898531536718</v>
       </c>
       <c r="QC9" s="25" t="n">
         <v>36.2860097736636</v>
@@ -16874,7 +16906,7 @@
         <v>43.0561631764392</v>
       </c>
       <c r="QG9" s="25" t="n">
-        <v>27.9374867988811</v>
+        <v>27.937486798881</v>
       </c>
       <c r="QH9" s="25" t="n">
         <v>0</v>
@@ -16898,7 +16930,7 @@
         <v>24.7792011444907</v>
       </c>
       <c r="QO9" s="25" t="n">
-        <v>25.1104498138086</v>
+        <v>11.4833476487372</v>
       </c>
       <c r="QP9" s="25" t="n">
         <v>37.7679634019357</v>
@@ -17961,7 +17993,7 @@
         <v>49</v>
       </c>
       <c r="MM10" s="29" t="n">
-        <v>45</v>
+        <v>55</v>
       </c>
       <c r="MN10" s="29" t="n">
         <v>53</v>
@@ -17976,7 +18008,7 @@
         <v>58</v>
       </c>
       <c r="MR10" s="29" t="n">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="MS10" s="29" t="n">
         <v>66</v>
@@ -18000,7 +18032,7 @@
         <v>46</v>
       </c>
       <c r="MZ10" s="29" t="n">
-        <v>40</v>
+        <v>54</v>
       </c>
       <c r="NA10" s="29" t="n">
         <v>51</v>
@@ -18039,7 +18071,7 @@
         <v>71</v>
       </c>
       <c r="NM10" s="29" t="n">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="NN10" s="29" t="n">
         <v>67</v>
@@ -18078,7 +18110,7 @@
         <v>61</v>
       </c>
       <c r="NZ10" s="29" t="n">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="OA10" s="29" t="n">
         <v>54</v>
@@ -18159,10 +18191,10 @@
         <v>0.843764143081404</v>
       </c>
       <c r="PA10" s="25" t="n">
-        <v>47.1479182343852</v>
+        <v>47.1479182343853</v>
       </c>
       <c r="PB10" s="25" t="n">
-        <v>39.4522146565577</v>
+        <v>53.6611490887787</v>
       </c>
       <c r="PC10" s="25" t="n">
         <v>55.0335196211626</v>
@@ -18174,13 +18206,13 @@
         <v>25.2133589307869</v>
       </c>
       <c r="PF10" s="25" t="n">
-        <v>64.7822363720812</v>
+        <v>64.7822363720813</v>
       </c>
       <c r="PG10" s="25" t="n">
-        <v>16.4827165782504</v>
+        <v>17.7422557329089</v>
       </c>
       <c r="PH10" s="25" t="n">
-        <v>50.6139912575259</v>
+        <v>50.613991257526</v>
       </c>
       <c r="PI10" s="25" t="n">
         <v>21.2077916366126</v>
@@ -18201,7 +18233,7 @@
         <v>69.0723068317792</v>
       </c>
       <c r="PO10" s="25" t="n">
-        <v>48.6275430037101</v>
+        <v>44.8413229406556</v>
       </c>
       <c r="PP10" s="25" t="n">
         <v>66.9741704985442</v>
@@ -18240,7 +18272,7 @@
         <v>64.926617169684</v>
       </c>
       <c r="QB10" s="25" t="n">
-        <v>54.7405821338403</v>
+        <v>73.9210013386079</v>
       </c>
       <c r="QC10" s="25" t="n">
         <v>68.8855863379048</v>
@@ -18255,7 +18287,7 @@
         <v>86.7990563292608</v>
       </c>
       <c r="QG10" s="25" t="n">
-        <v>10.8284537243925</v>
+        <v>12.9397720475342</v>
       </c>
       <c r="QH10" s="25" t="n">
         <v>70.9644761564981</v>
@@ -18279,7 +18311,7 @@
         <v>67.6349438776366</v>
       </c>
       <c r="QO10" s="25" t="n">
-        <v>47.097680605551</v>
+        <v>42.889994072906</v>
       </c>
       <c r="QP10" s="25" t="n">
         <v>59.0302599490193</v>
@@ -18471,7 +18503,7 @@
         <v>1.09871073312351</v>
       </c>
       <c r="BB11" s="28" t="n">
-        <v>0.658595626196821</v>
+        <v>0.658595626196822</v>
       </c>
       <c r="BC11" s="28" t="n">
         <v>1.18633324483875</v>
@@ -18522,7 +18554,7 @@
         <v>1.51687716869712</v>
       </c>
       <c r="BS11" s="28" t="n">
-        <v>0.84999137485337</v>
+        <v>0.849991374853371</v>
       </c>
       <c r="BT11" s="28" t="n">
         <v>0.023933646156425</v>
@@ -18579,7 +18611,7 @@
         <v>0.267898109029031</v>
       </c>
       <c r="CL11" s="30" t="n">
-        <v>0.0949390994966346</v>
+        <v>0.0949390994966347</v>
       </c>
       <c r="CM11" s="30" t="n">
         <v>0.0030914807013023</v>
@@ -18627,7 +18659,7 @@
         <v>0.223840629509771</v>
       </c>
       <c r="DB11" s="30" t="n">
-        <v>0.776159370490229</v>
+        <v>0.77615937049023</v>
       </c>
       <c r="DC11" s="30" t="n">
         <v>0.108503870057065</v>
@@ -19342,7 +19374,7 @@
         <v>57</v>
       </c>
       <c r="MM11" s="29" t="n">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="MN11" s="29" t="n">
         <v>76</v>
@@ -19381,7 +19413,7 @@
         <v>37</v>
       </c>
       <c r="MZ11" s="29" t="n">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="NA11" s="29" t="n">
         <v>67</v>
@@ -19420,7 +19452,7 @@
         <v>71</v>
       </c>
       <c r="NM11" s="29" t="n">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="NN11" s="29" t="n">
         <v>71</v>
@@ -19459,7 +19491,7 @@
         <v>64</v>
       </c>
       <c r="NZ11" s="29" t="n">
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="OA11" s="29" t="n">
         <v>65</v>
@@ -19543,7 +19575,7 @@
         <v>61.0020809233515</v>
       </c>
       <c r="PB11" s="25" t="n">
-        <v>71.0396690997364</v>
+        <v>75.8067266377541</v>
       </c>
       <c r="PC11" s="25" t="n">
         <v>117.483965121849</v>
@@ -19582,7 +19614,7 @@
         <v>101.543406542951</v>
       </c>
       <c r="PO11" s="25" t="n">
-        <v>47.6740729628828</v>
+        <v>63.417268256965</v>
       </c>
       <c r="PP11" s="25" t="n">
         <v>104.662130239603</v>
@@ -19609,7 +19641,7 @@
         <v>83.1993729865977</v>
       </c>
       <c r="PX11" s="25" t="n">
-        <v>90.7557800578932</v>
+        <v>90.7557800578933</v>
       </c>
       <c r="PY11" s="25" t="n">
         <v>59.5523789188553</v>
@@ -19621,10 +19653,10 @@
         <v>50.5022609094815</v>
       </c>
       <c r="QB11" s="25" t="n">
-        <v>58.9329405461773</v>
+        <v>62.7649371293407</v>
       </c>
       <c r="QC11" s="25" t="n">
-        <v>97.2135957776165</v>
+        <v>97.2135957776166</v>
       </c>
       <c r="QD11" s="25" t="n">
         <v>103.999306846195</v>
@@ -19660,13 +19692,13 @@
         <v>72.4675006882293</v>
       </c>
       <c r="QO11" s="25" t="n">
-        <v>34.145699505396</v>
+        <v>45.0975937644931</v>
       </c>
       <c r="QP11" s="25" t="n">
         <v>74.9016792834264</v>
       </c>
       <c r="QQ11" s="25" t="n">
-        <v>75.8156145969067</v>
+        <v>75.8156145969068</v>
       </c>
       <c r="QR11" s="25" t="n">
         <v>51.3527503052087</v>
@@ -21071,322 +21103,322 @@
         <v>1045</v>
       </c>
       <c r="MZ1" s="19" t="s">
+        <v>1046</v>
+      </c>
+      <c r="NA1" s="19" t="s">
         <v>1047</v>
       </c>
-      <c r="NA1" s="19" t="s">
+      <c r="NB1" s="19" t="s">
         <v>1048</v>
       </c>
-      <c r="NB1" s="19" t="s">
+      <c r="NC1" s="19" t="s">
         <v>1049</v>
       </c>
-      <c r="NC1" s="19" t="s">
+      <c r="ND1" s="19" t="s">
         <v>1050</v>
       </c>
-      <c r="ND1" s="19" t="s">
+      <c r="NE1" s="19" t="s">
         <v>1051</v>
       </c>
-      <c r="NE1" s="19" t="s">
+      <c r="NF1" s="19" t="s">
         <v>1052</v>
       </c>
-      <c r="NF1" s="19" t="s">
-        <v>1053</v>
-      </c>
       <c r="NG1" s="19" t="s">
-        <v>1055</v>
+        <v>1054</v>
       </c>
       <c r="NH1" s="19" t="s">
-        <v>1057</v>
+        <v>1056</v>
       </c>
       <c r="NI1" s="19" t="s">
+        <v>1058</v>
+      </c>
+      <c r="NJ1" s="19" t="s">
         <v>1059</v>
       </c>
-      <c r="NJ1" s="19" t="s">
+      <c r="NK1" s="19" t="s">
         <v>1060</v>
       </c>
-      <c r="NK1" s="19" t="s">
+      <c r="NL1" s="20" t="s">
         <v>1061</v>
       </c>
-      <c r="NL1" s="20" t="s">
+      <c r="NM1" s="20" t="s">
         <v>1062</v>
       </c>
-      <c r="NM1" s="20" t="s">
+      <c r="NN1" s="20" t="s">
         <v>1063</v>
       </c>
-      <c r="NN1" s="20" t="s">
+      <c r="NO1" s="20" t="s">
         <v>1064</v>
       </c>
-      <c r="NO1" s="20" t="s">
+      <c r="NP1" s="20" t="s">
         <v>1065</v>
       </c>
-      <c r="NP1" s="20" t="s">
+      <c r="NQ1" s="20" t="s">
         <v>1066</v>
       </c>
-      <c r="NQ1" s="20" t="s">
+      <c r="NR1" s="20" t="s">
         <v>1067</v>
       </c>
-      <c r="NR1" s="20" t="s">
+      <c r="NS1" s="20" t="s">
         <v>1068</v>
       </c>
-      <c r="NS1" s="20" t="s">
+      <c r="NT1" s="20" t="s">
         <v>1069</v>
       </c>
-      <c r="NT1" s="20" t="s">
+      <c r="NU1" s="20" t="s">
         <v>1070</v>
       </c>
-      <c r="NU1" s="20" t="s">
+      <c r="NV1" s="20" t="s">
         <v>1071</v>
       </c>
-      <c r="NV1" s="20" t="s">
+      <c r="NW1" s="20" t="s">
         <v>1072</v>
       </c>
-      <c r="NW1" s="20" t="s">
+      <c r="NX1" s="20" t="s">
         <v>1073</v>
       </c>
-      <c r="NX1" s="20" t="s">
+      <c r="NY1" s="20" t="s">
         <v>1074</v>
       </c>
-      <c r="NY1" s="20" t="s">
+      <c r="NZ1" s="20" t="s">
         <v>1075</v>
       </c>
-      <c r="NZ1" s="20" t="s">
+      <c r="OA1" s="20" t="s">
         <v>1076</v>
       </c>
-      <c r="OA1" s="20" t="s">
+      <c r="OB1" s="20" t="s">
         <v>1077</v>
       </c>
-      <c r="OB1" s="20" t="s">
+      <c r="OC1" s="20" t="s">
         <v>1078</v>
       </c>
-      <c r="OC1" s="20" t="s">
+      <c r="OD1" s="20" t="s">
         <v>1079</v>
       </c>
-      <c r="OD1" s="20" t="s">
+      <c r="OE1" s="20" t="s">
         <v>1080</v>
       </c>
-      <c r="OE1" s="20" t="s">
+      <c r="OF1" s="20" t="s">
         <v>1081</v>
       </c>
-      <c r="OF1" s="20" t="s">
-        <v>1082</v>
-      </c>
       <c r="OG1" s="20" t="s">
+        <v>1083</v>
+      </c>
+      <c r="OH1" s="20" t="s">
         <v>1084</v>
       </c>
-      <c r="OH1" s="20" t="s">
-        <v>1085</v>
-      </c>
       <c r="OI1" s="20" t="s">
+        <v>1086</v>
+      </c>
+      <c r="OJ1" s="20" t="s">
         <v>1087</v>
       </c>
-      <c r="OJ1" s="20" t="s">
+      <c r="OK1" s="20" t="s">
         <v>1088</v>
       </c>
-      <c r="OK1" s="20" t="s">
-        <v>1089</v>
-      </c>
       <c r="OL1" s="10" t="s">
-        <v>1091</v>
+        <v>1090</v>
       </c>
       <c r="OM1" s="10" t="s">
+        <v>1092</v>
+      </c>
+      <c r="ON1" s="10" t="s">
         <v>1093</v>
       </c>
-      <c r="ON1" s="10" t="s">
+      <c r="OO1" s="9" t="s">
         <v>1094</v>
       </c>
-      <c r="OO1" s="9" t="s">
-        <v>1095</v>
-      </c>
       <c r="OP1" s="9" t="s">
-        <v>1097</v>
+        <v>1096</v>
       </c>
       <c r="OQ1" s="3" t="s">
-        <v>1099</v>
+        <v>1098</v>
       </c>
       <c r="OR1" s="3" t="s">
+        <v>1100</v>
+      </c>
+      <c r="OS1" s="3" t="s">
         <v>1101</v>
       </c>
-      <c r="OS1" s="3" t="s">
+      <c r="OT1" s="9" t="s">
         <v>1102</v>
       </c>
-      <c r="OT1" s="9" t="s">
+      <c r="OU1" s="9" t="s">
         <v>1103</v>
       </c>
-      <c r="OU1" s="9" t="s">
+      <c r="OV1" s="9" t="s">
         <v>1104</v>
       </c>
-      <c r="OV1" s="9" t="s">
+      <c r="OW1" s="9" t="s">
         <v>1105</v>
       </c>
-      <c r="OW1" s="9" t="s">
+      <c r="OX1" s="9" t="s">
         <v>1106</v>
       </c>
-      <c r="OX1" s="9" t="s">
+      <c r="OY1" s="9" t="s">
         <v>1107</v>
       </c>
-      <c r="OY1" s="9" t="s">
+      <c r="OZ1" s="9" t="s">
         <v>1108</v>
       </c>
-      <c r="OZ1" s="9" t="s">
-        <v>1109</v>
-      </c>
       <c r="PA1" s="21" t="s">
-        <v>1111</v>
+        <v>1110</v>
       </c>
       <c r="PB1" s="21" t="s">
-        <v>1113</v>
+        <v>1112</v>
       </c>
       <c r="PC1" s="21" t="s">
-        <v>1115</v>
+        <v>1114</v>
       </c>
       <c r="PD1" s="21" t="s">
-        <v>1117</v>
+        <v>1116</v>
       </c>
       <c r="PE1" s="21" t="s">
-        <v>1119</v>
+        <v>1118</v>
       </c>
       <c r="PF1" s="21" t="s">
-        <v>1121</v>
+        <v>1120</v>
       </c>
       <c r="PG1" s="21" t="s">
-        <v>1123</v>
+        <v>1122</v>
       </c>
       <c r="PH1" s="21" t="s">
-        <v>1125</v>
+        <v>1124</v>
       </c>
       <c r="PI1" s="21" t="s">
-        <v>1127</v>
+        <v>1126</v>
       </c>
       <c r="PJ1" s="21" t="s">
-        <v>1129</v>
+        <v>1128</v>
       </c>
       <c r="PK1" s="21" t="s">
-        <v>1131</v>
+        <v>1130</v>
       </c>
       <c r="PL1" s="21" t="s">
-        <v>1133</v>
+        <v>1132</v>
       </c>
       <c r="PM1" s="21" t="s">
-        <v>1135</v>
+        <v>1134</v>
       </c>
       <c r="PN1" s="19" t="s">
-        <v>1137</v>
+        <v>1136</v>
       </c>
       <c r="PO1" s="19" t="s">
-        <v>1139</v>
+        <v>1138</v>
       </c>
       <c r="PP1" s="19" t="s">
-        <v>1141</v>
+        <v>1140</v>
       </c>
       <c r="PQ1" s="19" t="s">
-        <v>1143</v>
+        <v>1142</v>
       </c>
       <c r="PR1" s="19" t="s">
-        <v>1145</v>
+        <v>1144</v>
       </c>
       <c r="PS1" s="19" t="s">
-        <v>1147</v>
+        <v>1146</v>
       </c>
       <c r="PT1" s="19" t="s">
-        <v>1149</v>
+        <v>1148</v>
       </c>
       <c r="PU1" s="19" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="PV1" s="19" t="s">
-        <v>1153</v>
+        <v>1152</v>
       </c>
       <c r="PW1" s="19" t="s">
-        <v>1155</v>
+        <v>1154</v>
       </c>
       <c r="PX1" s="19" t="s">
-        <v>1157</v>
+        <v>1156</v>
       </c>
       <c r="PY1" s="19" t="s">
-        <v>1159</v>
+        <v>1158</v>
       </c>
       <c r="PZ1" s="19" t="s">
-        <v>1161</v>
+        <v>1160</v>
       </c>
       <c r="QA1" s="21" t="s">
-        <v>1163</v>
+        <v>1162</v>
       </c>
       <c r="QB1" s="21" t="s">
-        <v>1165</v>
+        <v>1164</v>
       </c>
       <c r="QC1" s="21" t="s">
-        <v>1167</v>
+        <v>1166</v>
       </c>
       <c r="QD1" s="21" t="s">
-        <v>1169</v>
+        <v>1168</v>
       </c>
       <c r="QE1" s="21" t="s">
-        <v>1171</v>
+        <v>1170</v>
       </c>
       <c r="QF1" s="21" t="s">
-        <v>1173</v>
+        <v>1172</v>
       </c>
       <c r="QG1" s="21" t="s">
-        <v>1175</v>
+        <v>1174</v>
       </c>
       <c r="QH1" s="21" t="s">
-        <v>1177</v>
+        <v>1176</v>
       </c>
       <c r="QI1" s="21" t="s">
-        <v>1179</v>
+        <v>1178</v>
       </c>
       <c r="QJ1" s="21" t="s">
-        <v>1181</v>
+        <v>1180</v>
       </c>
       <c r="QK1" s="21" t="s">
-        <v>1183</v>
+        <v>1182</v>
       </c>
       <c r="QL1" s="21" t="s">
-        <v>1185</v>
+        <v>1184</v>
       </c>
       <c r="QM1" s="21" t="s">
-        <v>1187</v>
+        <v>1186</v>
       </c>
       <c r="QN1" s="19" t="s">
-        <v>1189</v>
+        <v>1188</v>
       </c>
       <c r="QO1" s="19" t="s">
-        <v>1191</v>
+        <v>1190</v>
       </c>
       <c r="QP1" s="19" t="s">
-        <v>1193</v>
+        <v>1192</v>
       </c>
       <c r="QQ1" s="19" t="s">
-        <v>1195</v>
+        <v>1194</v>
       </c>
       <c r="QR1" s="19" t="s">
-        <v>1197</v>
+        <v>1196</v>
       </c>
       <c r="QS1" s="19" t="s">
-        <v>1199</v>
+        <v>1198</v>
       </c>
       <c r="QT1" s="19" t="s">
-        <v>1201</v>
+        <v>1200</v>
       </c>
       <c r="QU1" s="19" t="s">
-        <v>1203</v>
+        <v>1202</v>
       </c>
       <c r="QV1" s="19" t="s">
-        <v>1205</v>
+        <v>1204</v>
       </c>
       <c r="QW1" s="19" t="s">
-        <v>1207</v>
+        <v>1206</v>
       </c>
       <c r="QX1" s="19" t="s">
-        <v>1209</v>
+        <v>1208</v>
       </c>
       <c r="QY1" s="19" t="s">
-        <v>1211</v>
+        <v>1210</v>
       </c>
       <c r="QZ1" s="19" t="s">
-        <v>1213</v>
+        <v>1212</v>
       </c>
       <c r="RA1" s="3" t="s">
-        <v>1215</v>
+        <v>1214</v>
       </c>
     </row>
     <row r="2">
@@ -21548,7 +21580,7 @@
         <v>0.758430432514813</v>
       </c>
       <c r="BH2" s="28" t="n">
-        <v>4.92688757722838</v>
+        <v>4.92688757722837</v>
       </c>
       <c r="BI2" s="28" t="n">
         <v>0.963434380345267</v>
@@ -21575,7 +21607,7 @@
         <v>0.664954765658187</v>
       </c>
       <c r="BQ2" s="28" t="n">
-        <v>1.84259473798669</v>
+        <v>1.8425947379867</v>
       </c>
       <c r="BR2" s="28" t="n">
         <v>1.15717129040457</v>
@@ -22401,7 +22433,7 @@
         <v>63</v>
       </c>
       <c r="MM2" s="29" t="n">
-        <v>62</v>
+        <v>69</v>
       </c>
       <c r="MN2" s="29" t="n">
         <v>76</v>
@@ -22440,7 +22472,7 @@
         <v>47</v>
       </c>
       <c r="MZ2" s="29" t="n">
-        <v>46</v>
+        <v>57</v>
       </c>
       <c r="NA2" s="29" t="n">
         <v>72</v>
@@ -22479,7 +22511,7 @@
         <v>65.9916718868485</v>
       </c>
       <c r="NM2" s="29" t="n">
-        <v>48.1651798960988</v>
+        <v>52.9351361407706</v>
       </c>
       <c r="NN2" s="29" t="n">
         <v>68.1843319187818</v>
@@ -22503,7 +22535,7 @@
         <v>58.4935831798678</v>
       </c>
       <c r="NU2" s="29" t="n">
-        <v>68.0993250658214</v>
+        <v>68.1637358289727</v>
       </c>
       <c r="NV2" s="29" t="n">
         <v>58.9182420625763</v>
@@ -22518,7 +22550,7 @@
         <v>63.6663550257398</v>
       </c>
       <c r="NZ2" s="29" t="n">
-        <v>38.4349863647282</v>
+        <v>44.9597728867684</v>
       </c>
       <c r="OA2" s="29" t="n">
         <v>67.030258528521</v>
@@ -22542,7 +22574,7 @@
         <v>50.8433719391288</v>
       </c>
       <c r="OH2" s="29" t="n">
-        <v>67.0110170170076</v>
+        <v>67.0468007743139</v>
       </c>
       <c r="OI2" s="29" t="n">
         <v>56.1140017049977</v>
@@ -22551,7 +22583,7 @@
         <v>63.0163547902429</v>
       </c>
       <c r="OK2" s="29" t="n">
-        <v>42.6417173377544</v>
+        <v>43.2909107607964</v>
       </c>
       <c r="OL2" s="22" t="n">
         <v>211</v>
@@ -22602,7 +22634,7 @@
         <v>72.6619597700568</v>
       </c>
       <c r="PB2" s="25" t="n">
-        <v>66.8545766278586</v>
+        <v>83.1416945170066</v>
       </c>
       <c r="PC2" s="25" t="n">
         <v>117.640621006597</v>
@@ -22617,7 +22649,7 @@
         <v>118.693098519419</v>
       </c>
       <c r="PG2" s="25" t="n">
-        <v>94.6674584422416</v>
+        <v>94.6922782888973</v>
       </c>
       <c r="PH2" s="25" t="n">
         <v>108.064546401517</v>
@@ -22626,7 +22658,7 @@
         <v>36.5023495513042</v>
       </c>
       <c r="PJ2" s="25" t="n">
-        <v>122.998695800964</v>
+        <v>123.057468677466</v>
       </c>
       <c r="PK2" s="25" t="n">
         <v>99.9937829973154</v>
@@ -22635,13 +22667,13 @@
         <v>105.869093064804</v>
       </c>
       <c r="PM2" s="25" t="n">
-        <v>80.2827525589517</v>
+        <v>80.2935890241642</v>
       </c>
       <c r="PN2" s="25" t="n">
         <v>91.9527509182466</v>
       </c>
       <c r="PO2" s="25" t="n">
-        <v>48.6357262376477</v>
+        <v>58.8572690001761</v>
       </c>
       <c r="PP2" s="25" t="n">
         <v>104.733423555764</v>
@@ -22665,7 +22697,7 @@
         <v>54.6269558563915</v>
       </c>
       <c r="PW2" s="25" t="n">
-        <v>106.014229317612</v>
+        <v>106.042794848972</v>
       </c>
       <c r="PX2" s="25" t="n">
         <v>83.8538521918065</v>
@@ -22674,13 +22706,13 @@
         <v>91.4786217624796</v>
       </c>
       <c r="PZ2" s="25" t="n">
-        <v>46.4304775726821</v>
+        <v>46.5603671912465</v>
       </c>
       <c r="QA2" s="25" t="n">
         <v>66.5518972827937</v>
       </c>
       <c r="QB2" s="25" t="n">
-        <v>62.9365352710808</v>
+        <v>78.033507483792</v>
       </c>
       <c r="QC2" s="25" t="n">
         <v>110.354042859017</v>
@@ -22695,7 +22727,7 @@
         <v>110.814812977949</v>
       </c>
       <c r="QG2" s="25" t="n">
-        <v>91.2517621384903</v>
+        <v>91.2933667180923</v>
       </c>
       <c r="QH2" s="25" t="n">
         <v>101.69882674781</v>
@@ -22704,7 +22736,7 @@
         <v>35.5090691453336</v>
       </c>
       <c r="QJ2" s="25" t="n">
-        <v>114.011764982258</v>
+        <v>114.085497135402</v>
       </c>
       <c r="QK2" s="25" t="n">
         <v>94.9010404844178</v>
@@ -22713,13 +22745,13 @@
         <v>99.4132247539213</v>
       </c>
       <c r="QM2" s="25" t="n">
-        <v>78.0770874130736</v>
+        <v>78.0895169147354</v>
       </c>
       <c r="QN2" s="25" t="n">
         <v>85.1457224445399</v>
       </c>
       <c r="QO2" s="25" t="n">
-        <v>45.3592755597441</v>
+        <v>55.1130700140601</v>
       </c>
       <c r="QP2" s="25" t="n">
         <v>97.4761401450092</v>
@@ -22743,7 +22775,7 @@
         <v>53.506016172586</v>
       </c>
       <c r="QW2" s="25" t="n">
-        <v>97.6551846876399</v>
+        <v>97.6928554913635</v>
       </c>
       <c r="QX2" s="25" t="n">
         <v>80.1989678532379</v>
@@ -22752,7 +22784,7 @@
         <v>84.6056979431081</v>
       </c>
       <c r="QZ2" s="25" t="n">
-        <v>47.1774346803506</v>
+        <v>47.3184947927219</v>
       </c>
       <c r="RA2" s="23" t="n">
         <v>31.4159265358979</v>
@@ -25654,7 +25686,7 @@
     </row>
     <row r="352">
       <c r="A352" t="s">
-        <v>812</v>
+        <v>714</v>
       </c>
       <c r="B352" t="s">
         <v>1030</v>
@@ -25758,10 +25790,10 @@
     </row>
     <row r="365">
       <c r="A365" t="s">
+        <v>797</v>
+      </c>
+      <c r="B365" t="s">
         <v>1046</v>
-      </c>
-      <c r="B365" t="s">
-        <v>1047</v>
       </c>
     </row>
     <row r="366">
@@ -25769,7 +25801,7 @@
         <v>717</v>
       </c>
       <c r="B366" t="s">
-        <v>1048</v>
+        <v>1047</v>
       </c>
     </row>
     <row r="367">
@@ -25777,7 +25809,7 @@
         <v>1035</v>
       </c>
       <c r="B367" t="s">
-        <v>1049</v>
+        <v>1048</v>
       </c>
     </row>
     <row r="368">
@@ -25785,7 +25817,7 @@
         <v>799</v>
       </c>
       <c r="B368" t="s">
-        <v>1050</v>
+        <v>1049</v>
       </c>
     </row>
     <row r="369">
@@ -25793,7 +25825,7 @@
         <v>816</v>
       </c>
       <c r="B369" t="s">
-        <v>1051</v>
+        <v>1050</v>
       </c>
     </row>
     <row r="370">
@@ -25801,7 +25833,7 @@
         <v>871</v>
       </c>
       <c r="B370" t="s">
-        <v>1052</v>
+        <v>1051</v>
       </c>
     </row>
     <row r="371">
@@ -25809,31 +25841,31 @@
         <v>816</v>
       </c>
       <c r="B371" t="s">
-        <v>1053</v>
+        <v>1052</v>
       </c>
     </row>
     <row r="372">
       <c r="A372" t="s">
+        <v>1053</v>
+      </c>
+      <c r="B372" t="s">
         <v>1054</v>
-      </c>
-      <c r="B372" t="s">
-        <v>1055</v>
       </c>
     </row>
     <row r="373">
       <c r="A373" t="s">
+        <v>1055</v>
+      </c>
+      <c r="B373" t="s">
         <v>1056</v>
-      </c>
-      <c r="B373" t="s">
-        <v>1057</v>
       </c>
     </row>
     <row r="374">
       <c r="A374" t="s">
+        <v>1057</v>
+      </c>
+      <c r="B374" t="s">
         <v>1058</v>
-      </c>
-      <c r="B374" t="s">
-        <v>1059</v>
       </c>
     </row>
     <row r="375">
@@ -25841,7 +25873,7 @@
         <v>754</v>
       </c>
       <c r="B375" t="s">
-        <v>1060</v>
+        <v>1059</v>
       </c>
     </row>
     <row r="376">
@@ -25849,7 +25881,7 @@
         <v>835</v>
       </c>
       <c r="B376" t="s">
-        <v>1061</v>
+        <v>1060</v>
       </c>
     </row>
     <row r="377">
@@ -25857,15 +25889,15 @@
         <v>808</v>
       </c>
       <c r="B377" t="s">
-        <v>1062</v>
+        <v>1061</v>
       </c>
     </row>
     <row r="378">
       <c r="A378" t="s">
-        <v>641</v>
+        <v>621</v>
       </c>
       <c r="B378" t="s">
-        <v>1063</v>
+        <v>1062</v>
       </c>
     </row>
     <row r="379">
@@ -25873,7 +25905,7 @@
         <v>746</v>
       </c>
       <c r="B379" t="s">
-        <v>1064</v>
+        <v>1063</v>
       </c>
     </row>
     <row r="380">
@@ -25881,7 +25913,7 @@
         <v>750</v>
       </c>
       <c r="B380" t="s">
-        <v>1065</v>
+        <v>1064</v>
       </c>
     </row>
     <row r="381">
@@ -25889,7 +25921,7 @@
         <v>808</v>
       </c>
       <c r="B381" t="s">
-        <v>1066</v>
+        <v>1065</v>
       </c>
     </row>
     <row r="382">
@@ -25897,7 +25929,7 @@
         <v>746</v>
       </c>
       <c r="B382" t="s">
-        <v>1067</v>
+        <v>1066</v>
       </c>
     </row>
     <row r="383">
@@ -25905,15 +25937,15 @@
         <v>871</v>
       </c>
       <c r="B383" t="s">
-        <v>1068</v>
+        <v>1067</v>
       </c>
     </row>
     <row r="384">
       <c r="A384" t="s">
-        <v>1058</v>
+        <v>1057</v>
       </c>
       <c r="B384" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="385">
@@ -25921,7 +25953,7 @@
         <v>738</v>
       </c>
       <c r="B385" t="s">
-        <v>1070</v>
+        <v>1069</v>
       </c>
     </row>
     <row r="386">
@@ -25929,7 +25961,7 @@
         <v>746</v>
       </c>
       <c r="B386" t="s">
-        <v>1071</v>
+        <v>1070</v>
       </c>
     </row>
     <row r="387">
@@ -25937,7 +25969,7 @@
         <v>777</v>
       </c>
       <c r="B387" t="s">
-        <v>1072</v>
+        <v>1071</v>
       </c>
     </row>
     <row r="388">
@@ -25945,7 +25977,7 @@
         <v>808</v>
       </c>
       <c r="B388" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="389">
@@ -25953,23 +25985,23 @@
         <v>1038</v>
       </c>
       <c r="B389" t="s">
-        <v>1074</v>
+        <v>1073</v>
       </c>
     </row>
     <row r="390">
       <c r="A390" t="s">
-        <v>1058</v>
+        <v>1057</v>
       </c>
       <c r="B390" t="s">
-        <v>1075</v>
+        <v>1074</v>
       </c>
     </row>
     <row r="391">
       <c r="A391" t="s">
-        <v>649</v>
+        <v>1038</v>
       </c>
       <c r="B391" t="s">
-        <v>1076</v>
+        <v>1075</v>
       </c>
     </row>
     <row r="392">
@@ -25977,7 +26009,7 @@
         <v>754</v>
       </c>
       <c r="B392" t="s">
-        <v>1077</v>
+        <v>1076</v>
       </c>
     </row>
     <row r="393">
@@ -25985,7 +26017,7 @@
         <v>750</v>
       </c>
       <c r="B393" t="s">
-        <v>1078</v>
+        <v>1077</v>
       </c>
     </row>
     <row r="394">
@@ -25993,7 +26025,7 @@
         <v>779</v>
       </c>
       <c r="B394" t="s">
-        <v>1079</v>
+        <v>1078</v>
       </c>
     </row>
     <row r="395">
@@ -26001,7 +26033,7 @@
         <v>754</v>
       </c>
       <c r="B395" t="s">
-        <v>1080</v>
+        <v>1079</v>
       </c>
     </row>
     <row r="396">
@@ -26009,23 +26041,23 @@
         <v>748</v>
       </c>
       <c r="B396" t="s">
-        <v>1081</v>
+        <v>1080</v>
       </c>
     </row>
     <row r="397">
       <c r="A397" t="s">
-        <v>1058</v>
+        <v>1057</v>
       </c>
       <c r="B397" t="s">
-        <v>1082</v>
+        <v>1081</v>
       </c>
     </row>
     <row r="398">
       <c r="A398" t="s">
+        <v>1082</v>
+      </c>
+      <c r="B398" t="s">
         <v>1083</v>
-      </c>
-      <c r="B398" t="s">
-        <v>1084</v>
       </c>
     </row>
     <row r="399">
@@ -26033,15 +26065,15 @@
         <v>754</v>
       </c>
       <c r="B399" t="s">
-        <v>1085</v>
+        <v>1084</v>
       </c>
     </row>
     <row r="400">
       <c r="A400" t="s">
+        <v>1085</v>
+      </c>
+      <c r="B400" t="s">
         <v>1086</v>
-      </c>
-      <c r="B400" t="s">
-        <v>1087</v>
       </c>
     </row>
     <row r="401">
@@ -26049,7 +26081,7 @@
         <v>804</v>
       </c>
       <c r="B401" t="s">
-        <v>1088</v>
+        <v>1087</v>
       </c>
     </row>
     <row r="402">
@@ -26057,23 +26089,23 @@
         <v>742</v>
       </c>
       <c r="B402" t="s">
-        <v>1089</v>
+        <v>1088</v>
       </c>
     </row>
     <row r="403">
       <c r="A403" t="s">
+        <v>1089</v>
+      </c>
+      <c r="B403" t="s">
         <v>1090</v>
-      </c>
-      <c r="B403" t="s">
-        <v>1091</v>
       </c>
     </row>
     <row r="404">
       <c r="A404" t="s">
+        <v>1091</v>
+      </c>
+      <c r="B404" t="s">
         <v>1092</v>
-      </c>
-      <c r="B404" t="s">
-        <v>1093</v>
       </c>
     </row>
     <row r="405">
@@ -26081,7 +26113,7 @@
         <v>7</v>
       </c>
       <c r="B405" t="s">
-        <v>1094</v>
+        <v>1093</v>
       </c>
     </row>
     <row r="406">
@@ -26089,31 +26121,31 @@
         <v>982</v>
       </c>
       <c r="B406" t="s">
-        <v>1095</v>
+        <v>1094</v>
       </c>
     </row>
     <row r="407">
       <c r="A407" t="s">
+        <v>1095</v>
+      </c>
+      <c r="B407" t="s">
         <v>1096</v>
-      </c>
-      <c r="B407" t="s">
-        <v>1097</v>
       </c>
     </row>
     <row r="408">
       <c r="A408" t="s">
+        <v>1097</v>
+      </c>
+      <c r="B408" t="s">
         <v>1098</v>
-      </c>
-      <c r="B408" t="s">
-        <v>1099</v>
       </c>
     </row>
     <row r="409">
       <c r="A409" t="s">
+        <v>1099</v>
+      </c>
+      <c r="B409" t="s">
         <v>1100</v>
-      </c>
-      <c r="B409" t="s">
-        <v>1101</v>
       </c>
     </row>
     <row r="410">
@@ -26121,7 +26153,7 @@
         <v>562</v>
       </c>
       <c r="B410" t="s">
-        <v>1102</v>
+        <v>1101</v>
       </c>
     </row>
     <row r="411">
@@ -26129,7 +26161,7 @@
         <v>674</v>
       </c>
       <c r="B411" t="s">
-        <v>1103</v>
+        <v>1102</v>
       </c>
     </row>
     <row r="412">
@@ -26137,7 +26169,7 @@
         <v>627</v>
       </c>
       <c r="B412" t="s">
-        <v>1104</v>
+        <v>1103</v>
       </c>
     </row>
     <row r="413">
@@ -26145,7 +26177,7 @@
         <v>562</v>
       </c>
       <c r="B413" t="s">
-        <v>1105</v>
+        <v>1104</v>
       </c>
     </row>
     <row r="414">
@@ -26153,7 +26185,7 @@
         <v>562</v>
       </c>
       <c r="B414" t="s">
-        <v>1106</v>
+        <v>1105</v>
       </c>
     </row>
     <row r="415">
@@ -26161,7 +26193,7 @@
         <v>514</v>
       </c>
       <c r="B415" t="s">
-        <v>1107</v>
+        <v>1106</v>
       </c>
     </row>
     <row r="416">
@@ -26169,7 +26201,7 @@
         <v>857</v>
       </c>
       <c r="B416" t="s">
-        <v>1108</v>
+        <v>1107</v>
       </c>
     </row>
     <row r="417">
@@ -26177,431 +26209,431 @@
         <v>621</v>
       </c>
       <c r="B417" t="s">
-        <v>1109</v>
+        <v>1108</v>
       </c>
     </row>
     <row r="418">
       <c r="A418" t="s">
+        <v>1109</v>
+      </c>
+      <c r="B418" t="s">
         <v>1110</v>
-      </c>
-      <c r="B418" t="s">
-        <v>1111</v>
       </c>
     </row>
     <row r="419">
       <c r="A419" t="s">
+        <v>1111</v>
+      </c>
+      <c r="B419" t="s">
         <v>1112</v>
-      </c>
-      <c r="B419" t="s">
-        <v>1113</v>
       </c>
     </row>
     <row r="420">
       <c r="A420" t="s">
+        <v>1113</v>
+      </c>
+      <c r="B420" t="s">
         <v>1114</v>
-      </c>
-      <c r="B420" t="s">
-        <v>1115</v>
       </c>
     </row>
     <row r="421">
       <c r="A421" t="s">
+        <v>1115</v>
+      </c>
+      <c r="B421" t="s">
         <v>1116</v>
-      </c>
-      <c r="B421" t="s">
-        <v>1117</v>
       </c>
     </row>
     <row r="422">
       <c r="A422" t="s">
+        <v>1117</v>
+      </c>
+      <c r="B422" t="s">
         <v>1118</v>
-      </c>
-      <c r="B422" t="s">
-        <v>1119</v>
       </c>
     </row>
     <row r="423">
       <c r="A423" t="s">
+        <v>1119</v>
+      </c>
+      <c r="B423" t="s">
         <v>1120</v>
-      </c>
-      <c r="B423" t="s">
-        <v>1121</v>
       </c>
     </row>
     <row r="424">
       <c r="A424" t="s">
+        <v>1121</v>
+      </c>
+      <c r="B424" t="s">
         <v>1122</v>
-      </c>
-      <c r="B424" t="s">
-        <v>1123</v>
       </c>
     </row>
     <row r="425">
       <c r="A425" t="s">
+        <v>1123</v>
+      </c>
+      <c r="B425" t="s">
         <v>1124</v>
-      </c>
-      <c r="B425" t="s">
-        <v>1125</v>
       </c>
     </row>
     <row r="426">
       <c r="A426" t="s">
+        <v>1125</v>
+      </c>
+      <c r="B426" t="s">
         <v>1126</v>
-      </c>
-      <c r="B426" t="s">
-        <v>1127</v>
       </c>
     </row>
     <row r="427">
       <c r="A427" t="s">
+        <v>1127</v>
+      </c>
+      <c r="B427" t="s">
         <v>1128</v>
-      </c>
-      <c r="B427" t="s">
-        <v>1129</v>
       </c>
     </row>
     <row r="428">
       <c r="A428" t="s">
+        <v>1129</v>
+      </c>
+      <c r="B428" t="s">
         <v>1130</v>
-      </c>
-      <c r="B428" t="s">
-        <v>1131</v>
       </c>
     </row>
     <row r="429">
       <c r="A429" t="s">
+        <v>1131</v>
+      </c>
+      <c r="B429" t="s">
         <v>1132</v>
-      </c>
-      <c r="B429" t="s">
-        <v>1133</v>
       </c>
     </row>
     <row r="430">
       <c r="A430" t="s">
+        <v>1133</v>
+      </c>
+      <c r="B430" t="s">
         <v>1134</v>
-      </c>
-      <c r="B430" t="s">
-        <v>1135</v>
       </c>
     </row>
     <row r="431">
       <c r="A431" t="s">
+        <v>1135</v>
+      </c>
+      <c r="B431" t="s">
         <v>1136</v>
-      </c>
-      <c r="B431" t="s">
-        <v>1137</v>
       </c>
     </row>
     <row r="432">
       <c r="A432" t="s">
+        <v>1137</v>
+      </c>
+      <c r="B432" t="s">
         <v>1138</v>
-      </c>
-      <c r="B432" t="s">
-        <v>1139</v>
       </c>
     </row>
     <row r="433">
       <c r="A433" t="s">
+        <v>1139</v>
+      </c>
+      <c r="B433" t="s">
         <v>1140</v>
-      </c>
-      <c r="B433" t="s">
-        <v>1141</v>
       </c>
     </row>
     <row r="434">
       <c r="A434" t="s">
+        <v>1141</v>
+      </c>
+      <c r="B434" t="s">
         <v>1142</v>
-      </c>
-      <c r="B434" t="s">
-        <v>1143</v>
       </c>
     </row>
     <row r="435">
       <c r="A435" t="s">
+        <v>1143</v>
+      </c>
+      <c r="B435" t="s">
         <v>1144</v>
-      </c>
-      <c r="B435" t="s">
-        <v>1145</v>
       </c>
     </row>
     <row r="436">
       <c r="A436" t="s">
+        <v>1145</v>
+      </c>
+      <c r="B436" t="s">
         <v>1146</v>
-      </c>
-      <c r="B436" t="s">
-        <v>1147</v>
       </c>
     </row>
     <row r="437">
       <c r="A437" t="s">
+        <v>1147</v>
+      </c>
+      <c r="B437" t="s">
         <v>1148</v>
-      </c>
-      <c r="B437" t="s">
-        <v>1149</v>
       </c>
     </row>
     <row r="438">
       <c r="A438" t="s">
+        <v>1149</v>
+      </c>
+      <c r="B438" t="s">
         <v>1150</v>
-      </c>
-      <c r="B438" t="s">
-        <v>1151</v>
       </c>
     </row>
     <row r="439">
       <c r="A439" t="s">
+        <v>1151</v>
+      </c>
+      <c r="B439" t="s">
         <v>1152</v>
-      </c>
-      <c r="B439" t="s">
-        <v>1153</v>
       </c>
     </row>
     <row r="440">
       <c r="A440" t="s">
+        <v>1153</v>
+      </c>
+      <c r="B440" t="s">
         <v>1154</v>
-      </c>
-      <c r="B440" t="s">
-        <v>1155</v>
       </c>
     </row>
     <row r="441">
       <c r="A441" t="s">
+        <v>1155</v>
+      </c>
+      <c r="B441" t="s">
         <v>1156</v>
-      </c>
-      <c r="B441" t="s">
-        <v>1157</v>
       </c>
     </row>
     <row r="442">
       <c r="A442" t="s">
+        <v>1157</v>
+      </c>
+      <c r="B442" t="s">
         <v>1158</v>
-      </c>
-      <c r="B442" t="s">
-        <v>1159</v>
       </c>
     </row>
     <row r="443">
       <c r="A443" t="s">
+        <v>1159</v>
+      </c>
+      <c r="B443" t="s">
         <v>1160</v>
-      </c>
-      <c r="B443" t="s">
-        <v>1161</v>
       </c>
     </row>
     <row r="444">
       <c r="A444" t="s">
+        <v>1161</v>
+      </c>
+      <c r="B444" t="s">
         <v>1162</v>
-      </c>
-      <c r="B444" t="s">
-        <v>1163</v>
       </c>
     </row>
     <row r="445">
       <c r="A445" t="s">
+        <v>1163</v>
+      </c>
+      <c r="B445" t="s">
         <v>1164</v>
-      </c>
-      <c r="B445" t="s">
-        <v>1165</v>
       </c>
     </row>
     <row r="446">
       <c r="A446" t="s">
+        <v>1165</v>
+      </c>
+      <c r="B446" t="s">
         <v>1166</v>
-      </c>
-      <c r="B446" t="s">
-        <v>1167</v>
       </c>
     </row>
     <row r="447">
       <c r="A447" t="s">
+        <v>1167</v>
+      </c>
+      <c r="B447" t="s">
         <v>1168</v>
-      </c>
-      <c r="B447" t="s">
-        <v>1169</v>
       </c>
     </row>
     <row r="448">
       <c r="A448" t="s">
+        <v>1169</v>
+      </c>
+      <c r="B448" t="s">
         <v>1170</v>
-      </c>
-      <c r="B448" t="s">
-        <v>1171</v>
       </c>
     </row>
     <row r="449">
       <c r="A449" t="s">
+        <v>1171</v>
+      </c>
+      <c r="B449" t="s">
         <v>1172</v>
-      </c>
-      <c r="B449" t="s">
-        <v>1173</v>
       </c>
     </row>
     <row r="450">
       <c r="A450" t="s">
+        <v>1173</v>
+      </c>
+      <c r="B450" t="s">
         <v>1174</v>
-      </c>
-      <c r="B450" t="s">
-        <v>1175</v>
       </c>
     </row>
     <row r="451">
       <c r="A451" t="s">
+        <v>1175</v>
+      </c>
+      <c r="B451" t="s">
         <v>1176</v>
-      </c>
-      <c r="B451" t="s">
-        <v>1177</v>
       </c>
     </row>
     <row r="452">
       <c r="A452" t="s">
+        <v>1177</v>
+      </c>
+      <c r="B452" t="s">
         <v>1178</v>
-      </c>
-      <c r="B452" t="s">
-        <v>1179</v>
       </c>
     </row>
     <row r="453">
       <c r="A453" t="s">
+        <v>1179</v>
+      </c>
+      <c r="B453" t="s">
         <v>1180</v>
-      </c>
-      <c r="B453" t="s">
-        <v>1181</v>
       </c>
     </row>
     <row r="454">
       <c r="A454" t="s">
+        <v>1181</v>
+      </c>
+      <c r="B454" t="s">
         <v>1182</v>
-      </c>
-      <c r="B454" t="s">
-        <v>1183</v>
       </c>
     </row>
     <row r="455">
       <c r="A455" t="s">
+        <v>1183</v>
+      </c>
+      <c r="B455" t="s">
         <v>1184</v>
-      </c>
-      <c r="B455" t="s">
-        <v>1185</v>
       </c>
     </row>
     <row r="456">
       <c r="A456" t="s">
+        <v>1185</v>
+      </c>
+      <c r="B456" t="s">
         <v>1186</v>
-      </c>
-      <c r="B456" t="s">
-        <v>1187</v>
       </c>
     </row>
     <row r="457">
       <c r="A457" t="s">
+        <v>1187</v>
+      </c>
+      <c r="B457" t="s">
         <v>1188</v>
-      </c>
-      <c r="B457" t="s">
-        <v>1189</v>
       </c>
     </row>
     <row r="458">
       <c r="A458" t="s">
+        <v>1189</v>
+      </c>
+      <c r="B458" t="s">
         <v>1190</v>
-      </c>
-      <c r="B458" t="s">
-        <v>1191</v>
       </c>
     </row>
     <row r="459">
       <c r="A459" t="s">
+        <v>1191</v>
+      </c>
+      <c r="B459" t="s">
         <v>1192</v>
-      </c>
-      <c r="B459" t="s">
-        <v>1193</v>
       </c>
     </row>
     <row r="460">
       <c r="A460" t="s">
+        <v>1193</v>
+      </c>
+      <c r="B460" t="s">
         <v>1194</v>
-      </c>
-      <c r="B460" t="s">
-        <v>1195</v>
       </c>
     </row>
     <row r="461">
       <c r="A461" t="s">
+        <v>1195</v>
+      </c>
+      <c r="B461" t="s">
         <v>1196</v>
-      </c>
-      <c r="B461" t="s">
-        <v>1197</v>
       </c>
     </row>
     <row r="462">
       <c r="A462" t="s">
+        <v>1197</v>
+      </c>
+      <c r="B462" t="s">
         <v>1198</v>
-      </c>
-      <c r="B462" t="s">
-        <v>1199</v>
       </c>
     </row>
     <row r="463">
       <c r="A463" t="s">
+        <v>1199</v>
+      </c>
+      <c r="B463" t="s">
         <v>1200</v>
-      </c>
-      <c r="B463" t="s">
-        <v>1201</v>
       </c>
     </row>
     <row r="464">
       <c r="A464" t="s">
+        <v>1201</v>
+      </c>
+      <c r="B464" t="s">
         <v>1202</v>
-      </c>
-      <c r="B464" t="s">
-        <v>1203</v>
       </c>
     </row>
     <row r="465">
       <c r="A465" t="s">
+        <v>1203</v>
+      </c>
+      <c r="B465" t="s">
         <v>1204</v>
-      </c>
-      <c r="B465" t="s">
-        <v>1205</v>
       </c>
     </row>
     <row r="466">
       <c r="A466" t="s">
+        <v>1205</v>
+      </c>
+      <c r="B466" t="s">
         <v>1206</v>
-      </c>
-      <c r="B466" t="s">
-        <v>1207</v>
       </c>
     </row>
     <row r="467">
       <c r="A467" t="s">
+        <v>1207</v>
+      </c>
+      <c r="B467" t="s">
         <v>1208</v>
-      </c>
-      <c r="B467" t="s">
-        <v>1209</v>
       </c>
     </row>
     <row r="468">
       <c r="A468" t="s">
+        <v>1209</v>
+      </c>
+      <c r="B468" t="s">
         <v>1210</v>
-      </c>
-      <c r="B468" t="s">
-        <v>1211</v>
       </c>
     </row>
     <row r="469">
       <c r="A469" t="s">
+        <v>1211</v>
+      </c>
+      <c r="B469" t="s">
         <v>1212</v>
-      </c>
-      <c r="B469" t="s">
-        <v>1213</v>
       </c>
     </row>
     <row r="470">
       <c r="A470" t="s">
+        <v>1213</v>
+      </c>
+      <c r="B470" t="s">
         <v>1214</v>
-      </c>
-      <c r="B470" t="s">
-        <v>1215</v>
       </c>
     </row>
   </sheetData>
@@ -26620,6 +26652,7 @@
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -26809,13 +26842,13 @@
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="B5" t="n">
         <v>0</v>
       </c>
       <c r="C5" t="n">
-        <v>63</v>
+        <v>74</v>
       </c>
       <c r="D5" t="n">
         <v>0</v>
@@ -26854,13 +26887,13 @@
         <v>91</v>
       </c>
       <c r="B8" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C8" t="n">
         <v>86</v>
       </c>
       <c r="D8" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="9">

</xml_diff>